<commit_message>
Set ACT_BND for medium and high potential to zero
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
+++ b/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006CB853-38E9-4667-B314-8B4E9D9F0CA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DCEAC2-FCE2-42D8-9216-F5355325BE80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BioenergySupply-Baseline" sheetId="17" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="111">
   <si>
     <t>ktoe to PJ</t>
   </si>
@@ -468,9 +468,6 @@
   </si>
   <si>
     <t>TFM_INS-TS</t>
-  </si>
-  <si>
-    <t>DISABLED</t>
   </si>
 </sst>
 </file>
@@ -22999,8 +22996,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:DO69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BR13" sqref="BR13"/>
+    <sheetView tabSelected="1" topLeftCell="AW13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BL50" sqref="BL50:CJ65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30753,7 +30750,7 @@
       <c r="BC26" s="46"/>
       <c r="BD26" s="32"/>
       <c r="BG26" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BL26" s="2"/>
       <c r="BM26" s="2"/>
@@ -31230,103 +31227,78 @@
         <v>1</v>
       </c>
       <c r="BL28" s="66">
-        <f>E28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM28" s="66">
-        <f>F28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN28" s="66">
-        <f>G28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO28" s="66">
-        <f>H28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP28" s="66">
-        <f>I28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ28" s="66">
-        <f>J28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR28" s="66">
-        <f>K28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS28" s="66">
-        <f>L28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT28" s="66">
-        <f>M28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU28" s="66">
-        <f>N28/1000*Conversions!$B$2</f>
-        <v>1.1178E-2</v>
+        <v>0</v>
       </c>
       <c r="BV28" s="66">
-        <f>O28/1000*Conversions!$B$2</f>
-        <v>2.4839999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="BW28" s="66">
-        <f>P28/1000*Conversions!$B$2</f>
-        <v>4.0365000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="BX28" s="66">
-        <f>Q28/1000*Conversions!$B$2</f>
-        <v>5.1060000000000008E-2</v>
+        <v>0</v>
       </c>
       <c r="BY28" s="66">
-        <f>R28/1000*Conversions!$B$2</f>
-        <v>6.3825000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="BZ28" s="66">
-        <f>S28/1000*Conversions!$B$2</f>
-        <v>7.4520000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="CA28" s="66">
-        <f>T28/1000*Conversions!$B$2</f>
-        <v>8.6940000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="CB28" s="66">
-        <f>U28/1000*Conversions!$B$2</f>
-        <v>9.3840000000000021E-2</v>
+        <v>0</v>
       </c>
       <c r="CC28" s="66">
-        <f>V28/1000*Conversions!$B$2</f>
-        <v>0.102465</v>
+        <v>0</v>
       </c>
       <c r="CD28" s="66">
-        <f>W28/1000*Conversions!$B$2</f>
-        <v>0.11385000000000001</v>
+        <v>0</v>
       </c>
       <c r="CE28" s="66">
-        <f>X28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF28" s="66">
-        <f>Y28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG28" s="66">
-        <f>Z28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH28" s="66">
-        <f>AA28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI28" s="66">
-        <f>AB28/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ28" s="73">
-        <f>CI28</f>
+        <v>0</v>
+      </c>
+      <c r="CJ28" s="66">
         <v>0</v>
       </c>
       <c r="CL28" s="52" t="str">
@@ -31632,103 +31604,78 @@
         <v>1</v>
       </c>
       <c r="BL29" s="66">
-        <f>E29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM29" s="66">
-        <f>F29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN29" s="66">
-        <f>G29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO29" s="66">
-        <f>H29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP29" s="66">
-        <f>I29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ29" s="66">
-        <f>J29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR29" s="66">
-        <f>K29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS29" s="66">
-        <f>L29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT29" s="66">
-        <f>M29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU29" s="66">
-        <f>N29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV29" s="66">
-        <f>O29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW29" s="66">
-        <f>P29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX29" s="66">
-        <f>Q29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY29" s="66">
-        <f>R29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ29" s="66">
-        <f>S29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA29" s="66">
-        <f>T29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB29" s="66">
-        <f>U29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC29" s="66">
-        <f>V29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD29" s="66">
-        <f>W29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE29" s="66">
-        <f>X29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF29" s="66">
-        <f>Y29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG29" s="66">
-        <f>Z29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH29" s="66">
-        <f>AA29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI29" s="66">
-        <f>AB29/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ29" s="73">
-        <f>CI29</f>
+        <v>0</v>
+      </c>
+      <c r="CJ29" s="66">
         <v>0</v>
       </c>
       <c r="CL29" s="52" t="str">
@@ -32034,104 +31981,79 @@
         <v>1</v>
       </c>
       <c r="BL30" s="66">
-        <f>E30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM30" s="66">
-        <f>F30/1000*Conversions!$B$2</f>
-        <v>5.1812930016045949E-17</v>
+        <v>0</v>
       </c>
       <c r="BN30" s="66">
-        <f>G30/1000*Conversions!$B$2</f>
-        <v>5.219026286149803E-17</v>
+        <v>0</v>
       </c>
       <c r="BO30" s="66">
-        <f>H30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP30" s="66">
-        <f>I30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ30" s="66">
-        <f>J30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR30" s="66">
-        <f>K30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS30" s="66">
-        <f>L30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT30" s="66">
-        <f>M30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU30" s="66">
-        <f>N30/1000*Conversions!$B$2</f>
-        <v>2.807786322151316E-2</v>
+        <v>0</v>
       </c>
       <c r="BV30" s="66">
-        <f>O30/1000*Conversions!$B$2</f>
-        <v>5.6980968889485645E-2</v>
+        <v>0</v>
       </c>
       <c r="BW30" s="66">
-        <f>P30/1000*Conversions!$B$2</f>
-        <v>8.6734066550921973E-2</v>
+        <v>0</v>
       </c>
       <c r="BX30" s="66">
-        <f>Q30/1000*Conversions!$B$2</f>
-        <v>0.11716682271649489</v>
+        <v>0</v>
       </c>
       <c r="BY30" s="66">
-        <f>R30/1000*Conversions!$B$2</f>
-        <v>0.14869140948565346</v>
+        <v>0</v>
       </c>
       <c r="BZ30" s="66">
-        <f>S30/1000*Conversions!$B$2</f>
-        <v>0.18120432867915748</v>
+        <v>0</v>
       </c>
       <c r="CA30" s="66">
-        <f>T30/1000*Conversions!$B$2</f>
-        <v>0.21469246452501728</v>
+        <v>0</v>
       </c>
       <c r="CB30" s="66">
-        <f>U30/1000*Conversions!$B$2</f>
-        <v>0.24917828484863763</v>
+        <v>0</v>
       </c>
       <c r="CC30" s="66">
-        <f>V30/1000*Conversions!$B$2</f>
-        <v>0.28468472041951881</v>
+        <v>0</v>
       </c>
       <c r="CD30" s="66">
-        <f>W30/1000*Conversions!$B$2</f>
-        <v>0.48185276087417128</v>
+        <v>0</v>
       </c>
       <c r="CE30" s="66">
-        <f>X30/1000*Conversions!$B$2</f>
-        <v>0.48934572144211735</v>
+        <v>0</v>
       </c>
       <c r="CF30" s="66">
-        <f>Y30/1000*Conversions!$B$2</f>
-        <v>0.49695519988156245</v>
+        <v>0</v>
       </c>
       <c r="CG30" s="66">
-        <f>Z30/1000*Conversions!$B$2</f>
-        <v>0.50468300808171207</v>
+        <v>0</v>
       </c>
       <c r="CH30" s="66">
-        <f>AA30/1000*Conversions!$B$2</f>
-        <v>0.51253098610721592</v>
+        <v>0</v>
       </c>
       <c r="CI30" s="66">
-        <f>AB30/1000*Conversions!$B$2</f>
-        <v>0.52050100263629984</v>
-      </c>
-      <c r="CJ30" s="73">
-        <f>TREND(CD30:CI30,$CD$5:$CI$5,$CJ$5)</f>
-        <v>0.63624051867355824</v>
+        <v>0</v>
+      </c>
+      <c r="CJ30" s="66">
+        <v>0</v>
       </c>
       <c r="CL30" s="52" t="str">
         <f t="shared" si="5"/>
@@ -32434,103 +32356,78 @@
         <v>1</v>
       </c>
       <c r="BL31" s="66">
-        <f>E31/1000*Conversions!$B$2</f>
-        <v>2.0096724582357348</v>
+        <v>0</v>
       </c>
       <c r="BM31" s="66">
-        <f>F31/1000*Conversions!$B$2</f>
-        <v>3.6110097381970108</v>
+        <v>0</v>
       </c>
       <c r="BN31" s="66">
-        <f>G31/1000*Conversions!$B$2</f>
-        <v>3.3041335877500391</v>
+        <v>0</v>
       </c>
       <c r="BO31" s="66">
-        <f>H31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP31" s="66">
-        <f>I31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ31" s="66">
-        <f>J31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR31" s="66">
-        <f>K31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS31" s="66">
-        <f>L31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT31" s="66">
-        <f>M31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU31" s="66">
-        <f>N31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV31" s="66">
-        <f>O31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW31" s="66">
-        <f>P31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX31" s="66">
-        <f>Q31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY31" s="66">
-        <f>R31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ31" s="66">
-        <f>S31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA31" s="66">
-        <f>T31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB31" s="66">
-        <f>U31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC31" s="66">
-        <f>V31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD31" s="66">
-        <f>W31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE31" s="66">
-        <f>X31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF31" s="66">
-        <f>Y31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG31" s="66">
-        <f>Z31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH31" s="66">
-        <f>AA31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI31" s="66">
-        <f>AB31/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ31" s="73">
-        <f>CI31</f>
+        <v>0</v>
+      </c>
+      <c r="CJ31" s="66">
         <v>0</v>
       </c>
       <c r="CL31" s="52" t="str">
@@ -32836,104 +32733,79 @@
         <v>1</v>
       </c>
       <c r="BL32" s="66">
-        <f>E32/1000*Conversions!$B$2</f>
-        <v>0.60833943916817546</v>
+        <v>0</v>
       </c>
       <c r="BM32" s="66">
-        <f>F32/1000*Conversions!$B$2</f>
-        <v>0.60494794278408781</v>
+        <v>0</v>
       </c>
       <c r="BN32" s="66">
-        <f>G32/1000*Conversions!$B$2</f>
-        <v>0.60155644640000006</v>
+        <v>0</v>
       </c>
       <c r="BO32" s="66">
-        <f>H32/1000*Conversions!$B$2</f>
-        <v>0.59816495001591241</v>
+        <v>0</v>
       </c>
       <c r="BP32" s="66">
-        <f>I32/1000*Conversions!$B$2</f>
-        <v>0.59783828825204466</v>
+        <v>0</v>
       </c>
       <c r="BQ32" s="66">
-        <f>J32/1000*Conversions!$B$2</f>
-        <v>0.59362587749525431</v>
+        <v>0</v>
       </c>
       <c r="BR32" s="66">
-        <f>K32/1000*Conversions!$B$2</f>
-        <v>0.59699193210217305</v>
+        <v>0</v>
       </c>
       <c r="BS32" s="66">
-        <f>L32/1000*Conversions!$B$2</f>
-        <v>0.59969899041571162</v>
+        <v>0</v>
       </c>
       <c r="BT32" s="66">
-        <f>M32/1000*Conversions!$B$2</f>
-        <v>0.60194164187080423</v>
+        <v>0</v>
       </c>
       <c r="BU32" s="66">
-        <f>N32/1000*Conversions!$B$2</f>
-        <v>0.6037828686867307</v>
+        <v>0</v>
       </c>
       <c r="BV32" s="66">
-        <f>O32/1000*Conversions!$B$2</f>
-        <v>0.6057480542288245</v>
+        <v>0</v>
       </c>
       <c r="BW32" s="66">
-        <f>P32/1000*Conversions!$B$2</f>
-        <v>0.60723383584960289</v>
+        <v>0</v>
       </c>
       <c r="BX32" s="66">
-        <f>Q32/1000*Conversions!$B$2</f>
-        <v>0.60777540616237802</v>
+        <v>0</v>
       </c>
       <c r="BY32" s="66">
-        <f>R32/1000*Conversions!$B$2</f>
-        <v>0.60755335770849983</v>
+        <v>0</v>
       </c>
       <c r="BZ32" s="66">
-        <f>S32/1000*Conversions!$B$2</f>
-        <v>0.60612399939333761</v>
+        <v>0</v>
       </c>
       <c r="CA32" s="66">
-        <f>T32/1000*Conversions!$B$2</f>
-        <v>0.60382014388181271</v>
+        <v>0</v>
       </c>
       <c r="CB32" s="66">
-        <f>U32/1000*Conversions!$B$2</f>
-        <v>0.60085551274157856</v>
+        <v>0</v>
       </c>
       <c r="CC32" s="66">
-        <f>V32/1000*Conversions!$B$2</f>
-        <v>0.59739021176375418</v>
+        <v>0</v>
       </c>
       <c r="CD32" s="66">
-        <f>W32/1000*Conversions!$B$2</f>
-        <v>0.59356519121776741</v>
+        <v>0</v>
       </c>
       <c r="CE32" s="66">
-        <f>X32/1000*Conversions!$B$2</f>
-        <v>0.58953154480323344</v>
+        <v>0</v>
       </c>
       <c r="CF32" s="66">
-        <f>Y32/1000*Conversions!$B$2</f>
-        <v>0.58536081147713315</v>
+        <v>0</v>
       </c>
       <c r="CG32" s="66">
-        <f>Z32/1000*Conversions!$B$2</f>
-        <v>0.58110715645002375</v>
+        <v>0</v>
       </c>
       <c r="CH32" s="66">
-        <f>AA32/1000*Conversions!$B$2</f>
-        <v>0.576846835596591</v>
+        <v>0</v>
       </c>
       <c r="CI32" s="66">
-        <f>AB32/1000*Conversions!$B$2</f>
-        <v>0.57245925757788385</v>
-      </c>
-      <c r="CJ32" s="73">
-        <f>TREND(BT32:CI32,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.54711214261263752</v>
+        <v>0</v>
+      </c>
+      <c r="CJ32" s="66">
+        <v>0</v>
       </c>
       <c r="CL32" s="52" t="str">
         <f t="shared" si="5"/>
@@ -33238,104 +33110,79 @@
         <v>1</v>
       </c>
       <c r="BL33" s="66">
-        <f>E33/1000*Conversions!$B$2</f>
-        <v>0.16513689600000003</v>
+        <v>0</v>
       </c>
       <c r="BM33" s="66">
-        <f>F33/1000*Conversions!$B$2</f>
-        <v>0.165740796</v>
+        <v>0</v>
       </c>
       <c r="BN33" s="66">
-        <f>G33/1000*Conversions!$B$2</f>
-        <v>0.16655122800000002</v>
+        <v>0</v>
       </c>
       <c r="BO33" s="66">
-        <f>H33/1000*Conversions!$B$2</f>
-        <v>0.16754954400000002</v>
+        <v>0</v>
       </c>
       <c r="BP33" s="66">
-        <f>I33/1000*Conversions!$B$2</f>
-        <v>0.16871342400000003</v>
+        <v>0</v>
       </c>
       <c r="BQ33" s="66">
-        <f>J33/1000*Conversions!$B$2</f>
-        <v>0.16996435199999999</v>
+        <v>0</v>
       </c>
       <c r="BR33" s="66">
-        <f>K33/1000*Conversions!$B$2</f>
-        <v>0.17134549199999999</v>
+        <v>0</v>
       </c>
       <c r="BS33" s="66">
-        <f>L33/1000*Conversions!$B$2</f>
-        <v>0.17272681199999998</v>
+        <v>0</v>
       </c>
       <c r="BT33" s="66">
-        <f>M33/1000*Conversions!$B$2</f>
-        <v>0.17411101199999998</v>
+        <v>0</v>
       </c>
       <c r="BU33" s="66">
-        <f>N33/1000*Conversions!$B$2</f>
-        <v>0.17550439200000001</v>
+        <v>0</v>
       </c>
       <c r="BV33" s="66">
-        <f>O33/1000*Conversions!$B$2</f>
-        <v>0.17682555599999999</v>
+        <v>0</v>
       </c>
       <c r="BW33" s="66">
-        <f>P33/1000*Conversions!$B$2</f>
-        <v>0.17808159600000001</v>
+        <v>0</v>
       </c>
       <c r="BX33" s="66">
-        <f>Q33/1000*Conversions!$B$2</f>
-        <v>0.17927715600000002</v>
+        <v>0</v>
       </c>
       <c r="BY33" s="66">
-        <f>R33/1000*Conversions!$B$2</f>
-        <v>0.18041958</v>
+        <v>0</v>
       </c>
       <c r="BZ33" s="66">
-        <f>S33/1000*Conversions!$B$2</f>
-        <v>0.18151545600000005</v>
+        <v>0</v>
       </c>
       <c r="CA33" s="66">
-        <f>T33/1000*Conversions!$B$2</f>
-        <v>0.18256878000000001</v>
+        <v>0</v>
       </c>
       <c r="CB33" s="66">
-        <f>U33/1000*Conversions!$B$2</f>
-        <v>0.18360957600000002</v>
+        <v>0</v>
       </c>
       <c r="CC33" s="66">
-        <f>V33/1000*Conversions!$B$2</f>
-        <v>0.18464907600000005</v>
+        <v>0</v>
       </c>
       <c r="CD33" s="66">
-        <f>W33/1000*Conversions!$B$2</f>
-        <v>0.18569534400000004</v>
+        <v>0</v>
       </c>
       <c r="CE33" s="66">
-        <f>X33/1000*Conversions!$B$2</f>
-        <v>0.18674776800000001</v>
+        <v>0</v>
       </c>
       <c r="CF33" s="66">
-        <f>Y33/1000*Conversions!$B$2</f>
-        <v>0.187804692</v>
+        <v>0</v>
       </c>
       <c r="CG33" s="66">
-        <f>Z33/1000*Conversions!$B$2</f>
-        <v>0.188869752</v>
+        <v>0</v>
       </c>
       <c r="CH33" s="66">
-        <f>AA33/1000*Conversions!$B$2</f>
-        <v>0.18994924800000001</v>
+        <v>0</v>
       </c>
       <c r="CI33" s="66">
-        <f>AB33/1000*Conversions!$B$2</f>
-        <v>0.19104368400000005</v>
-      </c>
-      <c r="CJ33" s="73">
-        <f>TREND(BL33:CI33,$BL$5:$CI$5,$CJ$5)</f>
-        <v>0.20912996939478257</v>
+        <v>0</v>
+      </c>
+      <c r="CJ33" s="66">
+        <v>0</v>
       </c>
       <c r="CL33" s="52" t="str">
         <f t="shared" si="5"/>
@@ -33640,104 +33487,79 @@
         <v>1</v>
       </c>
       <c r="BL34" s="66">
-        <f>E34/1000*Conversions!$B$2</f>
-        <v>1.770767689226878</v>
+        <v>0</v>
       </c>
       <c r="BM34" s="66">
-        <f>F34/1000*Conversions!$B$2</f>
-        <v>1.1177084415156699</v>
+        <v>0</v>
       </c>
       <c r="BN34" s="66">
-        <f>G34/1000*Conversions!$B$2</f>
-        <v>1.3270406387788061</v>
+        <v>0</v>
       </c>
       <c r="BO34" s="66">
-        <f>H34/1000*Conversions!$B$2</f>
-        <v>1.2740152033445633</v>
+        <v>0</v>
       </c>
       <c r="BP34" s="66">
-        <f>I34/1000*Conversions!$B$2</f>
-        <v>1.3741252346560144</v>
+        <v>0</v>
       </c>
       <c r="BQ34" s="66">
-        <f>J34/1000*Conversions!$B$2</f>
-        <v>1.6879089999428629</v>
+        <v>0</v>
       </c>
       <c r="BR34" s="66">
-        <f>K34/1000*Conversions!$B$2</f>
-        <v>1.8348537362957613</v>
+        <v>0</v>
       </c>
       <c r="BS34" s="66">
-        <f>L34/1000*Conversions!$B$2</f>
-        <v>1.9836970880945337</v>
+        <v>0</v>
       </c>
       <c r="BT34" s="66">
-        <f>M34/1000*Conversions!$B$2</f>
-        <v>2.1256553048646114</v>
+        <v>0</v>
       </c>
       <c r="BU34" s="66">
-        <f>N34/1000*Conversions!$B$2</f>
-        <v>2.2488138115815683</v>
+        <v>0</v>
       </c>
       <c r="BV34" s="66">
-        <f>O34/1000*Conversions!$B$2</f>
-        <v>2.3513089975614161</v>
+        <v>0</v>
       </c>
       <c r="BW34" s="66">
-        <f>P34/1000*Conversions!$B$2</f>
-        <v>2.4435836021963722</v>
+        <v>0</v>
       </c>
       <c r="BX34" s="66">
-        <f>Q34/1000*Conversions!$B$2</f>
-        <v>2.5410850488083638</v>
+        <v>0</v>
       </c>
       <c r="BY34" s="66">
-        <f>R34/1000*Conversions!$B$2</f>
-        <v>2.5886509196059588</v>
+        <v>0</v>
       </c>
       <c r="BZ34" s="66">
-        <f>S34/1000*Conversions!$B$2</f>
-        <v>2.5393083958545417</v>
+        <v>0</v>
       </c>
       <c r="CA34" s="66">
-        <f>T34/1000*Conversions!$B$2</f>
-        <v>2.6034237203715316</v>
+        <v>0</v>
       </c>
       <c r="CB34" s="66">
-        <f>U34/1000*Conversions!$B$2</f>
-        <v>2.6753365644213138</v>
+        <v>0</v>
       </c>
       <c r="CC34" s="66">
-        <f>V34/1000*Conversions!$B$2</f>
-        <v>2.7532941486375093</v>
+        <v>0</v>
       </c>
       <c r="CD34" s="66">
-        <f>W34/1000*Conversions!$B$2</f>
-        <v>2.8357648780751545</v>
+        <v>0</v>
       </c>
       <c r="CE34" s="66">
-        <f>X34/1000*Conversions!$B$2</f>
-        <v>2.9211455718959964</v>
+        <v>0</v>
       </c>
       <c r="CF34" s="66">
-        <f>Y34/1000*Conversions!$B$2</f>
-        <v>3.0082873136909374</v>
+        <v>0</v>
       </c>
       <c r="CG34" s="66">
-        <f>Z34/1000*Conversions!$B$2</f>
-        <v>3.095652912218525</v>
+        <v>0</v>
       </c>
       <c r="CH34" s="66">
-        <f>AA34/1000*Conversions!$B$2</f>
-        <v>3.1823681388545353</v>
+        <v>0</v>
       </c>
       <c r="CI34" s="66">
-        <f>AB34/1000*Conversions!$B$2</f>
-        <v>3.2709431661860919</v>
-      </c>
-      <c r="CJ34" s="73">
-        <f>TREND(BT34:CI34,$BT$5:$CI$5,$CJ$5)</f>
-        <v>4.2606548535687239</v>
+        <v>0</v>
+      </c>
+      <c r="CJ34" s="66">
+        <v>0</v>
       </c>
       <c r="CL34" s="52" t="str">
         <f t="shared" si="5"/>
@@ -34042,104 +33864,79 @@
         <v>1</v>
       </c>
       <c r="BL35" s="66">
-        <f>E35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM35" s="66">
-        <f>F35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN35" s="66">
-        <f>G35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO35" s="66">
-        <f>H35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP35" s="66">
-        <f>I35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ35" s="66">
-        <f>J35/1000*Conversions!$B$2</f>
-        <v>6.7641966399291265E-2</v>
+        <v>0</v>
       </c>
       <c r="BR35" s="66">
-        <f>K35/1000*Conversions!$B$2</f>
-        <v>0.13779234946867608</v>
+        <v>0</v>
       </c>
       <c r="BS35" s="66">
-        <f>L35/1000*Conversions!$B$2</f>
-        <v>0.2117851444394139</v>
+        <v>0</v>
       </c>
       <c r="BT35" s="66">
-        <f>M35/1000*Conversions!$B$2</f>
-        <v>0.28989921295845283</v>
+        <v>0</v>
       </c>
       <c r="BU35" s="66">
-        <f>N35/1000*Conversions!$B$2</f>
-        <v>0.3709288734391214</v>
+        <v>0</v>
       </c>
       <c r="BV35" s="66">
-        <f>O35/1000*Conversions!$B$2</f>
-        <v>0.80656895221945313</v>
+        <v>0</v>
       </c>
       <c r="BW35" s="66">
-        <f>P35/1000*Conversions!$B$2</f>
-        <v>0.7458325491628599</v>
+        <v>0</v>
       </c>
       <c r="BX35" s="66">
-        <f>Q35/1000*Conversions!$B$2</f>
-        <v>0.83306465217502856</v>
+        <v>0</v>
       </c>
       <c r="BY35" s="66">
-        <f>R35/1000*Conversions!$B$2</f>
-        <v>0.84388125435670847</v>
+        <v>0</v>
       </c>
       <c r="BZ35" s="66">
-        <f>S35/1000*Conversions!$B$2</f>
-        <v>0.85315317512712041</v>
+        <v>0</v>
       </c>
       <c r="CA35" s="66">
-        <f>T35/1000*Conversions!$B$2</f>
-        <v>0.86081447974301006</v>
+        <v>0</v>
       </c>
       <c r="CB35" s="66">
-        <f>U35/1000*Conversions!$B$2</f>
-        <v>0.867048170203914</v>
+        <v>0</v>
       </c>
       <c r="CC35" s="66">
-        <f>V35/1000*Conversions!$B$2</f>
-        <v>0.87210039212741552</v>
+        <v>0</v>
       </c>
       <c r="CD35" s="66">
-        <f>W35/1000*Conversions!$B$2</f>
-        <v>0.87614443316643242</v>
+        <v>0</v>
       </c>
       <c r="CE35" s="66">
-        <f>X35/1000*Conversions!$B$2</f>
-        <v>0.8792880405744673</v>
+        <v>0</v>
       </c>
       <c r="CF35" s="66">
-        <f>Y35/1000*Conversions!$B$2</f>
-        <v>0.88144307444776182</v>
+        <v>0</v>
       </c>
       <c r="CG35" s="66">
-        <f>Z35/1000*Conversions!$B$2</f>
-        <v>0.88279254179335465</v>
+        <v>0</v>
       </c>
       <c r="CH35" s="66">
-        <f>AA35/1000*Conversions!$B$2</f>
-        <v>0.88364521747595381</v>
+        <v>0</v>
       </c>
       <c r="CI35" s="66">
-        <f>AB35/1000*Conversions!$B$2</f>
-        <v>0.8839723886486005</v>
-      </c>
-      <c r="CJ35" s="73">
-        <f>TREND(CD35:CI35,$CD$5:$CI$5,$CJ$5)</f>
-        <v>0.90799467041487469</v>
+        <v>0</v>
+      </c>
+      <c r="CJ35" s="66">
+        <v>0</v>
       </c>
       <c r="CL35" s="52" t="str">
         <f t="shared" si="5"/>
@@ -34444,104 +34241,79 @@
         <v>1</v>
       </c>
       <c r="BL36" s="66">
-        <f>E36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM36" s="66">
-        <f>F36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN36" s="66">
-        <f>G36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO36" s="66">
-        <f>H36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP36" s="66">
-        <f>I36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ36" s="66">
-        <f>J36/1000*Conversions!$B$2</f>
-        <v>0.1084334897841296</v>
+        <v>0</v>
       </c>
       <c r="BR36" s="66">
-        <f>K36/1000*Conversions!$B$2</f>
-        <v>0.21812713872853223</v>
+        <v>0</v>
       </c>
       <c r="BS36" s="66">
-        <f>L36/1000*Conversions!$B$2</f>
-        <v>0.32847071459076899</v>
+        <v>0</v>
       </c>
       <c r="BT36" s="66">
-        <f>M36/1000*Conversions!$B$2</f>
-        <v>0.439103529833199</v>
+        <v>0</v>
       </c>
       <c r="BU36" s="66">
-        <f>N36/1000*Conversions!$B$2</f>
-        <v>0.54975242796096446</v>
+        <v>0</v>
       </c>
       <c r="BV36" s="66">
-        <f>O36/1000*Conversions!$B$2</f>
-        <v>0.55016849812349256</v>
+        <v>0</v>
       </c>
       <c r="BW36" s="66">
-        <f>P36/1000*Conversions!$B$2</f>
-        <v>0.55025735270974896</v>
+        <v>0</v>
       </c>
       <c r="BX36" s="66">
-        <f>Q36/1000*Conversions!$B$2</f>
-        <v>0.55017588333945222</v>
+        <v>0</v>
       </c>
       <c r="BY36" s="66">
-        <f>R36/1000*Conversions!$B$2</f>
-        <v>0.55002453557010877</v>
+        <v>0</v>
       </c>
       <c r="BZ36" s="66">
-        <f>S36/1000*Conversions!$B$2</f>
-        <v>0.54983403846371204</v>
+        <v>0</v>
       </c>
       <c r="CA36" s="66">
-        <f>T36/1000*Conversions!$B$2</f>
-        <v>0.54961850644870391</v>
+        <v>0</v>
       </c>
       <c r="CB36" s="66">
-        <f>U36/1000*Conversions!$B$2</f>
-        <v>0.54937634756216625</v>
+        <v>0</v>
       </c>
       <c r="CC36" s="66">
-        <f>V36/1000*Conversions!$B$2</f>
-        <v>0.54910574957447889</v>
+        <v>0</v>
       </c>
       <c r="CD36" s="66">
-        <f>W36/1000*Conversions!$B$2</f>
-        <v>0.54883925546334955</v>
+        <v>0</v>
       </c>
       <c r="CE36" s="66">
-        <f>X36/1000*Conversions!$B$2</f>
-        <v>0.54886646384295834</v>
+        <v>0</v>
       </c>
       <c r="CF36" s="66">
-        <f>Y36/1000*Conversions!$B$2</f>
-        <v>0.54909431570408362</v>
+        <v>0</v>
       </c>
       <c r="CG36" s="66">
-        <f>Z36/1000*Conversions!$B$2</f>
-        <v>0.54922130535333369</v>
+        <v>0</v>
       </c>
       <c r="CH36" s="66">
-        <f>AA36/1000*Conversions!$B$2</f>
-        <v>0.54920487326040868</v>
+        <v>0</v>
       </c>
       <c r="CI36" s="66">
-        <f>AB36/1000*Conversions!$B$2</f>
-        <v>0.54906884563548053</v>
-      </c>
-      <c r="CJ36" s="73">
-        <f>CI36</f>
-        <v>0.54906884563548053</v>
+        <v>0</v>
+      </c>
+      <c r="CJ36" s="66">
+        <v>0</v>
       </c>
       <c r="CL36" s="52" t="str">
         <f t="shared" si="5"/>
@@ -34846,104 +34618,79 @@
         <v>1</v>
       </c>
       <c r="BL37" s="66">
-        <f>E37/1000*Conversions!$B$2</f>
-        <v>0.10206997179437498</v>
+        <v>0</v>
       </c>
       <c r="BM37" s="66">
-        <f>F37/1000*Conversions!$B$2</f>
-        <v>0.12762687536742101</v>
+        <v>0</v>
       </c>
       <c r="BN37" s="66">
-        <f>G37/1000*Conversions!$B$2</f>
-        <v>0.13111111859407756</v>
+        <v>0</v>
       </c>
       <c r="BO37" s="66">
-        <f>H37/1000*Conversions!$B$2</f>
-        <v>0.13706461804322786</v>
+        <v>0</v>
       </c>
       <c r="BP37" s="66">
-        <f>I37/1000*Conversions!$B$2</f>
-        <v>0.14772651632149808</v>
+        <v>0</v>
       </c>
       <c r="BQ37" s="66">
-        <f>J37/1000*Conversions!$B$2</f>
-        <v>0.15305968942151191</v>
+        <v>0</v>
       </c>
       <c r="BR37" s="66">
-        <f>K37/1000*Conversions!$B$2</f>
-        <v>0.16342250661010063</v>
+        <v>0</v>
       </c>
       <c r="BS37" s="66">
-        <f>L37/1000*Conversions!$B$2</f>
-        <v>0.17411982451599994</v>
+        <v>0</v>
       </c>
       <c r="BT37" s="66">
-        <f>M37/1000*Conversions!$B$2</f>
-        <v>0.18514262911615337</v>
+        <v>0</v>
       </c>
       <c r="BU37" s="66">
-        <f>N37/1000*Conversions!$B$2</f>
-        <v>0.19540645193976094</v>
+        <v>0</v>
       </c>
       <c r="BV37" s="66">
-        <f>O37/1000*Conversions!$B$2</f>
-        <v>0.2049849195679046</v>
+        <v>0</v>
       </c>
       <c r="BW37" s="66">
-        <f>P37/1000*Conversions!$B$2</f>
-        <v>0.21484890129349377</v>
+        <v>0</v>
       </c>
       <c r="BX37" s="66">
-        <f>Q37/1000*Conversions!$B$2</f>
-        <v>0.22463133791701467</v>
+        <v>0</v>
       </c>
       <c r="BY37" s="66">
-        <f>R37/1000*Conversions!$B$2</f>
-        <v>0.23514839929326761</v>
+        <v>0</v>
       </c>
       <c r="BZ37" s="66">
-        <f>S37/1000*Conversions!$B$2</f>
-        <v>0.24603832348428883</v>
+        <v>0</v>
       </c>
       <c r="CA37" s="66">
-        <f>T37/1000*Conversions!$B$2</f>
-        <v>0.25724095232418215</v>
+        <v>0</v>
       </c>
       <c r="CB37" s="66">
-        <f>U37/1000*Conversions!$B$2</f>
-        <v>0.26156619669433079</v>
+        <v>0</v>
       </c>
       <c r="CC37" s="66">
-        <f>V37/1000*Conversions!$B$2</f>
-        <v>0.26596226492448166</v>
+        <v>0</v>
       </c>
       <c r="CD37" s="66">
-        <f>W37/1000*Conversions!$B$2</f>
-        <v>0.27043027294917671</v>
+        <v>0</v>
       </c>
       <c r="CE37" s="66">
-        <f>X37/1000*Conversions!$B$2</f>
-        <v>0.27497292588992328</v>
+        <v>0</v>
       </c>
       <c r="CF37" s="66">
-        <f>Y37/1000*Conversions!$B$2</f>
-        <v>0.27959146483132008</v>
+        <v>0</v>
       </c>
       <c r="CG37" s="66">
-        <f>Z37/1000*Conversions!$B$2</f>
-        <v>0.28428715140641891</v>
+        <v>0</v>
       </c>
       <c r="CH37" s="66">
-        <f>AA37/1000*Conversions!$B$2</f>
-        <v>0.28906126813568656</v>
+        <v>0</v>
       </c>
       <c r="CI37" s="66">
-        <f>AB37/1000*Conversions!$B$2</f>
-        <v>0.29391511877153675</v>
-      </c>
-      <c r="CJ37" s="73">
-        <f>TREND(BT37:CI37,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.4109850441439864</v>
+        <v>0</v>
+      </c>
+      <c r="CJ37" s="66">
+        <v>0</v>
       </c>
       <c r="CL37" s="52" t="str">
         <f t="shared" si="5"/>
@@ -35248,104 +34995,79 @@
         <v>1</v>
       </c>
       <c r="BL38" s="66">
-        <f>E38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM38" s="66">
-        <f>F38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN38" s="66">
-        <f>G38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO38" s="66">
-        <f>H38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP38" s="66">
-        <f>I38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ38" s="66">
-        <f>J38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR38" s="66">
-        <f>K38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS38" s="66">
-        <f>L38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT38" s="66">
-        <f>M38/1000*Conversions!$B$2</f>
-        <v>8.1066666666666648E-2</v>
+        <v>0</v>
       </c>
       <c r="BU38" s="66">
-        <f>N38/1000*Conversions!$B$2</f>
-        <v>0.28727999999999992</v>
+        <v>0</v>
       </c>
       <c r="BV38" s="66">
-        <f>O38/1000*Conversions!$B$2</f>
-        <v>0.60242666666666655</v>
+        <v>0</v>
       </c>
       <c r="BW38" s="66">
-        <f>P38/1000*Conversions!$B$2</f>
-        <v>1.063949333333333</v>
+        <v>0</v>
       </c>
       <c r="BX38" s="66">
-        <f>Q38/1000*Conversions!$B$2</f>
-        <v>1.6283455999999996</v>
+        <v>0</v>
       </c>
       <c r="BY38" s="66">
-        <f>R38/1000*Conversions!$B$2</f>
-        <v>2.3175034666666656</v>
+        <v>0</v>
       </c>
       <c r="BZ38" s="66">
-        <f>S38/1000*Conversions!$B$2</f>
-        <v>3.1579511893333323</v>
+        <v>0</v>
       </c>
       <c r="CA38" s="66">
-        <f>T38/1000*Conversions!$B$2</f>
-        <v>4.1818378623999974</v>
+        <v>0</v>
       </c>
       <c r="CB38" s="66">
-        <f>U38/1000*Conversions!$B$2</f>
-        <v>5.4281206237866622</v>
+        <v>0</v>
       </c>
       <c r="CC38" s="66">
-        <f>V38/1000*Conversions!$B$2</f>
-        <v>6.9440019085653288</v>
+        <v>0</v>
       </c>
       <c r="CD38" s="66">
-        <f>W38/1000*Conversions!$B$2</f>
-        <v>8.7866692823039987</v>
+        <v>0</v>
       </c>
       <c r="CE38" s="66">
-        <f>X38/1000*Conversions!$B$2</f>
-        <v>11.02540139586219</v>
+        <v>0</v>
       </c>
       <c r="CF38" s="66">
-        <f>Y38/1000*Conversions!$B$2</f>
-        <v>13.744116916884833</v>
+        <v>0</v>
       </c>
       <c r="CG38" s="66">
-        <f>Z38/1000*Conversions!$B$2</f>
-        <v>17.044459390482043</v>
+        <v>0</v>
       </c>
       <c r="CH38" s="66">
-        <f>AA38/1000*Conversions!$B$2</f>
-        <v>17.227733147368951</v>
+        <v>0</v>
       </c>
       <c r="CI38" s="66">
-        <f>AB38/1000*Conversions!$B$2</f>
-        <v>17.411006904255867</v>
-      </c>
-      <c r="CJ38" s="73">
-        <f>TREND(BL38:CI38,$BL$5:$CI$5,$CJ$5)</f>
-        <v>25.054162231125929</v>
+        <v>0</v>
+      </c>
+      <c r="CJ38" s="66">
+        <v>0</v>
       </c>
       <c r="CL38" s="52" t="str">
         <f t="shared" si="5"/>
@@ -35650,104 +35372,79 @@
         <v>1</v>
       </c>
       <c r="BL39" s="66">
-        <f>E39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM39" s="66">
-        <f>F39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN39" s="66">
-        <f>G39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO39" s="66">
-        <f>H39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP39" s="66">
-        <f>I39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ39" s="66">
-        <f>J39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR39" s="66">
-        <f>K39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS39" s="66">
-        <f>L39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT39" s="66">
-        <f>M39/1000*Conversions!$B$2</f>
-        <v>0.12666666666666665</v>
+        <v>0</v>
       </c>
       <c r="BU39" s="66">
-        <f>N39/1000*Conversions!$B$2</f>
-        <v>0.38474999999999993</v>
+        <v>0</v>
       </c>
       <c r="BV39" s="66">
-        <f>O39/1000*Conversions!$B$2</f>
-        <v>0.70109999999999983</v>
+        <v>0</v>
       </c>
       <c r="BW39" s="66">
-        <f>P39/1000*Conversions!$B$2</f>
-        <v>1.0881299999999994</v>
+        <v>0</v>
       </c>
       <c r="BX39" s="66">
-        <f>Q39/1000*Conversions!$B$2</f>
-        <v>1.5608879999999994</v>
+        <v>0</v>
       </c>
       <c r="BY39" s="66">
-        <f>R39/1000*Conversions!$B$2</f>
-        <v>2.1376139999999992</v>
+        <v>0</v>
       </c>
       <c r="BZ39" s="66">
-        <f>S39/1000*Conversions!$B$2</f>
-        <v>2.8404148799999991</v>
+        <v>0</v>
       </c>
       <c r="CA39" s="66">
-        <f>T39/1000*Conversions!$B$2</f>
-        <v>3.6960815519999972</v>
+        <v>0</v>
       </c>
       <c r="CB39" s="66">
-        <f>U39/1000*Conversions!$B$2</f>
-        <v>4.7370782975999965</v>
+        <v>0</v>
       </c>
       <c r="CC39" s="66">
-        <f>V39/1000*Conversions!$B$2</f>
-        <v>6.0027404793599954</v>
+        <v>0</v>
       </c>
       <c r="CD39" s="66">
-        <f>W39/1000*Conversions!$B$2</f>
-        <v>7.5407244019199968</v>
+        <v>0</v>
       </c>
       <c r="CE39" s="66">
-        <f>X39/1000*Conversions!$B$2</f>
-        <v>9.408762274329602</v>
+        <v>0</v>
       </c>
       <c r="CF39" s="66">
-        <f>Y39/1000*Conversions!$B$2</f>
-        <v>11.676786319626247</v>
+        <v>0</v>
       </c>
       <c r="CG39" s="66">
-        <f>Z39/1000*Conversions!$B$2</f>
-        <v>14.429499492068368</v>
+        <v>0</v>
       </c>
       <c r="CH39" s="66">
-        <f>AA39/1000*Conversions!$B$2</f>
-        <v>14.584655400585239</v>
+        <v>0</v>
       </c>
       <c r="CI39" s="66">
-        <f>AB39/1000*Conversions!$B$2</f>
-        <v>14.739811309102111</v>
-      </c>
-      <c r="CJ39" s="73">
-        <f>TREND(BL39:CI39,$BL$5:$CI$5,$CJ$5)</f>
-        <v>21.358484097597056</v>
+        <v>0</v>
+      </c>
+      <c r="CJ39" s="66">
+        <v>0</v>
       </c>
       <c r="CL39" s="52" t="str">
         <f t="shared" si="5"/>
@@ -36052,104 +35749,79 @@
         <v>1</v>
       </c>
       <c r="BL40" s="66">
-        <f>E40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM40" s="66">
-        <f>F40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN40" s="66">
-        <f>G40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO40" s="66">
-        <f>H40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP40" s="66">
-        <f>I40/1000*Conversions!$B$2</f>
-        <v>0.10941619502112578</v>
+        <v>0</v>
       </c>
       <c r="BQ40" s="66">
-        <f>J40/1000*Conversions!$B$2</f>
-        <v>0.22039468698481438</v>
+        <v>0</v>
       </c>
       <c r="BR40" s="66">
-        <f>K40/1000*Conversions!$B$2</f>
-        <v>0.33317520873033607</v>
+        <v>0</v>
       </c>
       <c r="BS40" s="66">
-        <f>L40/1000*Conversions!$B$2</f>
-        <v>0.447472717807405</v>
+        <v>0</v>
       </c>
       <c r="BT40" s="66">
-        <f>M40/1000*Conversions!$B$2</f>
-        <v>0.5630035683450757</v>
+        <v>0</v>
       </c>
       <c r="BU40" s="66">
-        <f>N40/1000*Conversions!$B$2</f>
-        <v>0.56698421665493748</v>
+        <v>0</v>
       </c>
       <c r="BV40" s="66">
-        <f>O40/1000*Conversions!$B$2</f>
-        <v>0.57096486496479937</v>
+        <v>0</v>
       </c>
       <c r="BW40" s="66">
-        <f>P40/1000*Conversions!$B$2</f>
-        <v>0.57494551327466115</v>
+        <v>0</v>
       </c>
       <c r="BX40" s="66">
-        <f>Q40/1000*Conversions!$B$2</f>
-        <v>0.57892616158452292</v>
+        <v>0</v>
       </c>
       <c r="BY40" s="66">
-        <f>R40/1000*Conversions!$B$2</f>
-        <v>0.58290680989438481</v>
+        <v>0</v>
       </c>
       <c r="BZ40" s="66">
-        <f>S40/1000*Conversions!$B$2</f>
-        <v>0.58688745820424659</v>
+        <v>0</v>
       </c>
       <c r="CA40" s="66">
-        <f>T40/1000*Conversions!$B$2</f>
-        <v>0.59086810651410837</v>
+        <v>0</v>
       </c>
       <c r="CB40" s="66">
-        <f>U40/1000*Conversions!$B$2</f>
-        <v>0.59484875482397015</v>
+        <v>0</v>
       </c>
       <c r="CC40" s="66">
-        <f>V40/1000*Conversions!$B$2</f>
-        <v>0.59882940313383193</v>
+        <v>0</v>
       </c>
       <c r="CD40" s="66">
-        <f>W40/1000*Conversions!$B$2</f>
-        <v>0.60281005144369371</v>
+        <v>0</v>
       </c>
       <c r="CE40" s="66">
-        <f>X40/1000*Conversions!$B$2</f>
-        <v>0.60679069975355548</v>
+        <v>0</v>
       </c>
       <c r="CF40" s="66">
-        <f>Y40/1000*Conversions!$B$2</f>
-        <v>0.61077134806341726</v>
+        <v>0</v>
       </c>
       <c r="CG40" s="66">
-        <f>Z40/1000*Conversions!$B$2</f>
-        <v>0.61475199637327915</v>
+        <v>0</v>
       </c>
       <c r="CH40" s="66">
-        <f>AA40/1000*Conversions!$B$2</f>
-        <v>0.61873264468314093</v>
+        <v>0</v>
       </c>
       <c r="CI40" s="66">
-        <f>AB40/1000*Conversions!$B$2</f>
-        <v>0.62271329299300271</v>
-      </c>
-      <c r="CJ40" s="73">
-        <f>TREND(BT40:CI40,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.6824230176409305</v>
+        <v>0</v>
+      </c>
+      <c r="CJ40" s="66">
+        <v>0</v>
       </c>
       <c r="CL40" s="52" t="str">
         <f t="shared" si="5"/>
@@ -36454,104 +36126,79 @@
         <v>1</v>
       </c>
       <c r="BL41" s="66">
-        <f>E41/1000*Conversions!$B$2</f>
-        <v>0.25039919937369937</v>
+        <v>0</v>
       </c>
       <c r="BM41" s="66">
-        <f>F41/1000*Conversions!$B$2</f>
-        <v>0.3283283160568311</v>
+        <v>0</v>
       </c>
       <c r="BN41" s="66">
-        <f>G41/1000*Conversions!$B$2</f>
-        <v>0.16547747129264292</v>
+        <v>0</v>
       </c>
       <c r="BO41" s="66">
-        <f>H41/1000*Conversions!$B$2</f>
-        <v>0.12510096829723802</v>
+        <v>0</v>
       </c>
       <c r="BP41" s="66">
-        <f>I41/1000*Conversions!$B$2</f>
-        <v>0.33627140278297579</v>
+        <v>0</v>
       </c>
       <c r="BQ41" s="66">
-        <f>J41/1000*Conversions!$B$2</f>
-        <v>0.5719976561338419</v>
+        <v>0</v>
       </c>
       <c r="BR41" s="66">
-        <f>K41/1000*Conversions!$B$2</f>
-        <v>0.81147400816854365</v>
+        <v>0</v>
       </c>
       <c r="BS41" s="66">
-        <f>L41/1000*Conversions!$B$2</f>
-        <v>1.0547453739858081</v>
+        <v>0</v>
       </c>
       <c r="BT41" s="66">
-        <f>M41/1000*Conversions!$B$2</f>
-        <v>1.2996873854074265</v>
+        <v>0</v>
       </c>
       <c r="BU41" s="66">
-        <f>N41/1000*Conversions!$B$2</f>
-        <v>1.3100848844906861</v>
+        <v>0</v>
       </c>
       <c r="BV41" s="66">
-        <f>O41/1000*Conversions!$B$2</f>
-        <v>1.3205655635666114</v>
+        <v>0</v>
       </c>
       <c r="BW41" s="66">
-        <f>P41/1000*Conversions!$B$2</f>
-        <v>1.3311300880751442</v>
+        <v>0</v>
       </c>
       <c r="BX41" s="66">
-        <f>Q41/1000*Conversions!$B$2</f>
-        <v>1.3417791287797456</v>
+        <v>0</v>
       </c>
       <c r="BY41" s="66">
-        <f>R41/1000*Conversions!$B$2</f>
-        <v>1.3525133618099832</v>
+        <v>0</v>
       </c>
       <c r="BZ41" s="66">
-        <f>S41/1000*Conversions!$B$2</f>
-        <v>1.3633334687044634</v>
+        <v>0</v>
       </c>
       <c r="CA41" s="66">
-        <f>T41/1000*Conversions!$B$2</f>
-        <v>1.3742401364540988</v>
+        <v>0</v>
       </c>
       <c r="CB41" s="66">
-        <f>U41/1000*Conversions!$B$2</f>
-        <v>1.385234057545732</v>
+        <v>0</v>
       </c>
       <c r="CC41" s="66">
-        <f>V41/1000*Conversions!$B$2</f>
-        <v>1.3963159300060974</v>
+        <v>0</v>
       </c>
       <c r="CD41" s="66">
-        <f>W41/1000*Conversions!$B$2</f>
-        <v>1.4074864574461463</v>
+        <v>0</v>
       </c>
       <c r="CE41" s="66">
-        <f>X41/1000*Conversions!$B$2</f>
-        <v>1.4186569848861941</v>
+        <v>0</v>
       </c>
       <c r="CF41" s="66">
-        <f>Y41/1000*Conversions!$B$2</f>
-        <v>1.4298275123262427</v>
+        <v>0</v>
       </c>
       <c r="CG41" s="66">
-        <f>Z41/1000*Conversions!$B$2</f>
-        <v>1.4409980397662905</v>
+        <v>0</v>
       </c>
       <c r="CH41" s="66">
-        <f>AA41/1000*Conversions!$B$2</f>
-        <v>1.4521685672063418</v>
+        <v>0</v>
       </c>
       <c r="CI41" s="66">
-        <f>AB41/1000*Conversions!$B$2</f>
-        <v>1.46333909464639</v>
-      </c>
-      <c r="CJ41" s="73">
-        <f>TREND(BT41:CI41,$BT$5:$CI$5,$CJ$5)</f>
-        <v>1.626565350571326</v>
+        <v>0</v>
+      </c>
+      <c r="CJ41" s="66">
+        <v>0</v>
       </c>
       <c r="CL41" s="52" t="str">
         <f t="shared" si="5"/>
@@ -36856,104 +36503,79 @@
         <v>1</v>
       </c>
       <c r="BL42" s="66">
-        <f>E42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM42" s="66">
-        <f>F42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN42" s="66">
-        <f>G42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO42" s="66">
-        <f>H42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP42" s="66">
-        <f>I42/1000*Conversions!$B$2</f>
-        <v>1.1485838310580205</v>
+        <v>0</v>
       </c>
       <c r="BQ42" s="66">
-        <f>J42/1000*Conversions!$B$2</f>
-        <v>2.3606420317271422</v>
+        <v>0</v>
       </c>
       <c r="BR42" s="66">
-        <f>K42/1000*Conversions!$B$2</f>
-        <v>3.6361746020073644</v>
+        <v>0</v>
       </c>
       <c r="BS42" s="66">
-        <f>L42/1000*Conversions!$B$2</f>
-        <v>4.9751815418986887</v>
+        <v>0</v>
       </c>
       <c r="BT42" s="66">
-        <f>M42/1000*Conversions!$B$2</f>
-        <v>6.377662851401114</v>
+        <v>0</v>
       </c>
       <c r="BU42" s="66">
-        <f>N42/1000*Conversions!$B$2</f>
-        <v>7.8436185305146395</v>
+        <v>0</v>
       </c>
       <c r="BV42" s="66">
-        <f>O42/1000*Conversions!$B$2</f>
-        <v>8.2253283450467034</v>
+        <v>0</v>
       </c>
       <c r="BW42" s="66">
-        <f>P42/1000*Conversions!$B$2</f>
-        <v>8.6161059266660676</v>
+        <v>0</v>
       </c>
       <c r="BX42" s="66">
-        <f>Q42/1000*Conversions!$B$2</f>
-        <v>9.0159512753727302</v>
+        <v>0</v>
       </c>
       <c r="BY42" s="66">
-        <f>R42/1000*Conversions!$B$2</f>
-        <v>9.4248643911666949</v>
+        <v>0</v>
       </c>
       <c r="BZ42" s="66">
-        <f>S42/1000*Conversions!$B$2</f>
-        <v>9.8428452740479582</v>
+        <v>0</v>
       </c>
       <c r="CA42" s="66">
-        <f>T42/1000*Conversions!$B$2</f>
-        <v>10.269893924016518</v>
+        <v>0</v>
       </c>
       <c r="CB42" s="66">
-        <f>U42/1000*Conversions!$B$2</f>
-        <v>10.706010341072385</v>
+        <v>0</v>
       </c>
       <c r="CC42" s="66">
-        <f>V42/1000*Conversions!$B$2</f>
-        <v>11.15119452521555</v>
+        <v>0</v>
       </c>
       <c r="CD42" s="66">
-        <f>W42/1000*Conversions!$B$2</f>
-        <v>11.605446476446016</v>
+        <v>0</v>
       </c>
       <c r="CE42" s="66">
-        <f>X42/1000*Conversions!$B$2</f>
-        <v>12.068766194763782</v>
+        <v>0</v>
       </c>
       <c r="CF42" s="66">
-        <f>Y42/1000*Conversions!$B$2</f>
-        <v>12.541153680168847</v>
+        <v>0</v>
       </c>
       <c r="CG42" s="66">
-        <f>Z42/1000*Conversions!$B$2</f>
-        <v>13.022608932661214</v>
+        <v>0</v>
       </c>
       <c r="CH42" s="66">
-        <f>AA42/1000*Conversions!$B$2</f>
-        <v>13.513131952240876</v>
+        <v>0</v>
       </c>
       <c r="CI42" s="66">
-        <f>AB42/1000*Conversions!$B$2</f>
-        <v>14.012722738907854</v>
-      </c>
-      <c r="CJ42" s="73">
-        <f>TREND(BT42:CI42,$BT$5:$CI$5,$CJ$5)</f>
-        <v>20.870088249162677</v>
+        <v>0</v>
+      </c>
+      <c r="CJ42" s="66">
+        <v>0</v>
       </c>
       <c r="CL42" s="52" t="str">
         <f t="shared" si="5"/>
@@ -37258,103 +36880,78 @@
         <v>1</v>
       </c>
       <c r="BL43" s="66">
-        <f>E43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM43" s="66">
-        <f>F43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN43" s="66">
-        <f>G43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO43" s="66">
-        <f>H43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP43" s="66">
-        <f>I43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ43" s="66">
-        <f>J43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR43" s="66">
-        <f>K43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS43" s="66">
-        <f>L43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT43" s="66">
-        <f>M43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU43" s="66">
-        <f>N43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV43" s="66">
-        <f>O43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW43" s="66">
-        <f>P43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX43" s="66">
-        <f>Q43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY43" s="66">
-        <f>R43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ43" s="66">
-        <f>S43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA43" s="66">
-        <f>T43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB43" s="66">
-        <f>U43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC43" s="66">
-        <f>V43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD43" s="66">
-        <f>W43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE43" s="66">
-        <f>X43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF43" s="66">
-        <f>Y43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG43" s="66">
-        <f>Z43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH43" s="66">
-        <f>AA43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI43" s="66">
-        <f>AB43/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ43" s="73">
-        <f>CI43</f>
+        <v>0</v>
+      </c>
+      <c r="CJ43" s="66">
         <v>0</v>
       </c>
       <c r="CL43" s="52" t="str">
@@ -38045,7 +37642,7 @@
       <c r="BC48" s="46"/>
       <c r="BD48" s="32"/>
       <c r="BG48" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BL48" s="2"/>
       <c r="BM48" s="2"/>
@@ -38522,104 +38119,79 @@
         <v>1</v>
       </c>
       <c r="BL50" s="66">
-        <f>E50/1000*Conversions!$B$2</f>
-        <v>0.29499766100608776</v>
+        <v>0</v>
       </c>
       <c r="BM50" s="66">
-        <f>F50/1000*Conversions!$B$2</f>
-        <v>0.30086875000000007</v>
+        <v>0</v>
       </c>
       <c r="BN50" s="66">
-        <f>G50/1000*Conversions!$B$2</f>
-        <v>0.3193954054054054</v>
+        <v>0</v>
       </c>
       <c r="BO50" s="66">
-        <f>H50/1000*Conversions!$B$2</f>
-        <v>0.20799770270270271</v>
+        <v>0</v>
       </c>
       <c r="BP50" s="66">
-        <f>I50/1000*Conversions!$B$2</f>
-        <v>9.6600000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="BQ50" s="66">
-        <f>J50/1000*Conversions!$B$2</f>
-        <v>9.6600000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="BR50" s="66">
-        <f>K50/1000*Conversions!$B$2</f>
-        <v>0.19044000000000005</v>
+        <v>0</v>
       </c>
       <c r="BS50" s="66">
-        <f>L50/1000*Conversions!$B$2</f>
-        <v>0.34017000000000003</v>
+        <v>0</v>
       </c>
       <c r="BT50" s="66">
-        <f>M50/1000*Conversions!$B$2</f>
-        <v>0.46505999999999997</v>
+        <v>0</v>
       </c>
       <c r="BU50" s="66">
-        <f>N50/1000*Conversions!$B$2</f>
-        <v>0.56014200000000003</v>
+        <v>0</v>
       </c>
       <c r="BV50" s="66">
-        <f>O50/1000*Conversions!$B$2</f>
-        <v>0.96186000000000005</v>
+        <v>0</v>
       </c>
       <c r="BW50" s="66">
-        <f>P50/1000*Conversions!$B$2</f>
-        <v>1.270635</v>
+        <v>0</v>
       </c>
       <c r="BX50" s="66">
-        <f>Q50/1000*Conversions!$B$2</f>
-        <v>1.5773400000000002</v>
+        <v>0</v>
       </c>
       <c r="BY50" s="66">
-        <f>R50/1000*Conversions!$B$2</f>
-        <v>1.7439750000000001</v>
+        <v>0</v>
       </c>
       <c r="BZ50" s="66">
-        <f>S50/1000*Conversions!$B$2</f>
-        <v>2.0989800000000001</v>
+        <v>0</v>
       </c>
       <c r="CA50" s="66">
-        <f>T50/1000*Conversions!$B$2</f>
-        <v>1.5483600000000002</v>
+        <v>0</v>
       </c>
       <c r="CB50" s="66">
-        <f>U50/1000*Conversions!$B$2</f>
-        <v>1.8105600000000002</v>
+        <v>0</v>
       </c>
       <c r="CC50" s="66">
-        <f>V50/1000*Conversions!$B$2</f>
-        <v>1.0843349999999998</v>
+        <v>0</v>
       </c>
       <c r="CD50" s="66">
-        <f>W50/1000*Conversions!$B$2</f>
-        <v>1.3075500000000002</v>
+        <v>0</v>
       </c>
       <c r="CE50" s="66">
-        <f>X50/1000*Conversions!$B$2</f>
-        <v>1.7526000000000002</v>
+        <v>0</v>
       </c>
       <c r="CF50" s="66">
-        <f>Y50/1000*Conversions!$B$2</f>
-        <v>1.3109999999999999</v>
+        <v>0</v>
       </c>
       <c r="CG50" s="66">
-        <f>Z50/1000*Conversions!$B$2</f>
-        <v>1.7249999999999999</v>
+        <v>0</v>
       </c>
       <c r="CH50" s="66">
-        <f>AA50/1000*Conversions!$B$2</f>
-        <v>1.4282999999999997</v>
+        <v>0</v>
       </c>
       <c r="CI50" s="66">
-        <f>AB50/1000*Conversions!$B$2</f>
-        <v>1.4282999999999997</v>
-      </c>
-      <c r="CJ50" s="73">
-        <f>TREND(BW50:CI50,$BW$5:$CI$5,$CJ$5)</f>
-        <v>1.2758896153846173</v>
+        <v>0</v>
+      </c>
+      <c r="CJ50" s="66">
+        <v>0</v>
       </c>
       <c r="CL50" s="52" t="str">
         <f t="shared" ref="CL50:CL65" si="10">BG50</f>
@@ -38924,103 +38496,78 @@
         <v>1</v>
       </c>
       <c r="BL51" s="66">
-        <f>E51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM51" s="66">
-        <f>F51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN51" s="66">
-        <f>G51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO51" s="66">
-        <f>H51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP51" s="66">
-        <f>I51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ51" s="66">
-        <f>J51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR51" s="66">
-        <f>K51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS51" s="66">
-        <f>L51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT51" s="66">
-        <f>M51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU51" s="66">
-        <f>N51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV51" s="66">
-        <f>O51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW51" s="66">
-        <f>P51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX51" s="66">
-        <f>Q51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY51" s="66">
-        <f>R51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ51" s="66">
-        <f>S51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA51" s="66">
-        <f>T51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB51" s="66">
-        <f>U51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC51" s="66">
-        <f>V51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD51" s="66">
-        <f>W51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE51" s="66">
-        <f>X51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF51" s="66">
-        <f>Y51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG51" s="66">
-        <f>Z51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH51" s="66">
-        <f>AA51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI51" s="66">
-        <f>AB51/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ51" s="73">
-        <f>CI51</f>
+        <v>0</v>
+      </c>
+      <c r="CJ51" s="66">
         <v>0</v>
       </c>
       <c r="CL51" s="52" t="str">
@@ -39326,104 +38873,79 @@
         <v>1</v>
       </c>
       <c r="BL52" s="66">
-        <f>E52/1000*Conversions!$B$2</f>
-        <v>0.22047060000000002</v>
+        <v>0</v>
       </c>
       <c r="BM52" s="66">
-        <f>F52/1000*Conversions!$B$2</f>
-        <v>0.23534988827091782</v>
+        <v>0</v>
       </c>
       <c r="BN52" s="66">
-        <f>G52/1000*Conversions!$B$2</f>
-        <v>0.23706384737322286</v>
+        <v>0</v>
       </c>
       <c r="BO52" s="66">
-        <f>H52/1000*Conversions!$B$2</f>
-        <v>0.24317777012234676</v>
+        <v>0</v>
       </c>
       <c r="BP52" s="66">
-        <f>I52/1000*Conversions!$B$2</f>
-        <v>0.24936525020419262</v>
+        <v>0</v>
       </c>
       <c r="BQ52" s="66">
-        <f>J52/1000*Conversions!$B$2</f>
-        <v>0.25681865283380162</v>
+        <v>0</v>
       </c>
       <c r="BR52" s="66">
-        <f>K52/1000*Conversions!$B$2</f>
-        <v>0.26407859803333822</v>
+        <v>0</v>
       </c>
       <c r="BS52" s="66">
-        <f>L52/1000*Conversions!$B$2</f>
-        <v>0.27129820145686256</v>
+        <v>0</v>
       </c>
       <c r="BT52" s="66">
-        <f>M52/1000*Conversions!$B$2</f>
-        <v>0.2784649343212966</v>
+        <v>0</v>
       </c>
       <c r="BU52" s="66">
-        <f>N52/1000*Conversions!$B$2</f>
-        <v>0.28400495246439306</v>
+        <v>0</v>
       </c>
       <c r="BV52" s="66">
-        <f>O52/1000*Conversions!$B$2</f>
-        <v>0.28817857742882308</v>
+        <v>0</v>
       </c>
       <c r="BW52" s="66">
-        <f>P52/1000*Conversions!$B$2</f>
-        <v>0.29243564884197326</v>
+        <v>0</v>
       </c>
       <c r="BX52" s="66">
-        <f>Q52/1000*Conversions!$B$2</f>
-        <v>0.29628285505097024</v>
+        <v>0</v>
       </c>
       <c r="BY52" s="66">
-        <f>R52/1000*Conversions!$B$2</f>
-        <v>0.30079993160220875</v>
+        <v>0</v>
       </c>
       <c r="BZ52" s="66">
-        <f>S52/1000*Conversions!$B$2</f>
-        <v>0.30547746426228395</v>
+        <v>0</v>
       </c>
       <c r="CA52" s="66">
-        <f>T52/1000*Conversions!$B$2</f>
-        <v>0.3102277340126553</v>
+        <v>0</v>
       </c>
       <c r="CB52" s="66">
-        <f>U52/1000*Conversions!$B$2</f>
-        <v>0.31505187193774048</v>
+        <v>0</v>
       </c>
       <c r="CC52" s="66">
-        <f>V52/1000*Conversions!$B$2</f>
-        <v>0.31995102671067238</v>
+        <v>0</v>
       </c>
       <c r="CD52" s="66">
-        <f>W52/1000*Conversions!$B$2</f>
-        <v>0.32492636486680887</v>
+        <v>0</v>
       </c>
       <c r="CE52" s="66">
-        <f>X52/1000*Conversions!$B$2</f>
-        <v>0.32997907108149582</v>
+        <v>0</v>
       </c>
       <c r="CF52" s="66">
-        <f>Y52/1000*Conversions!$B$2</f>
-        <v>0.3351103484521506</v>
+        <v>0</v>
       </c>
       <c r="CG52" s="66">
-        <f>Z52/1000*Conversions!$B$2</f>
-        <v>0.34032141878472949</v>
+        <v>0</v>
       </c>
       <c r="CH52" s="66">
-        <f>AA52/1000*Conversions!$B$2</f>
-        <v>0.34561352288465264</v>
+        <v>0</v>
       </c>
       <c r="CI52" s="66">
-        <f>AB52/1000*Conversions!$B$2</f>
-        <v>0.35098792085225056</v>
-      </c>
-      <c r="CJ52" s="73">
-        <f>TREND(BT52:CI52,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.42118817778752771</v>
+        <v>0</v>
+      </c>
+      <c r="CJ52" s="66">
+        <v>0</v>
       </c>
       <c r="CL52" s="52" t="str">
         <f t="shared" si="10"/>
@@ -39728,103 +39250,78 @@
         <v>1</v>
       </c>
       <c r="BL53" s="66">
-        <f>E53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM53" s="66">
-        <f>F53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN53" s="66">
-        <f>G53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO53" s="66">
-        <f>H53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP53" s="66">
-        <f>I53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ53" s="66">
-        <f>J53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR53" s="66">
-        <f>K53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS53" s="66">
-        <f>L53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT53" s="66">
-        <f>M53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU53" s="66">
-        <f>N53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV53" s="66">
-        <f>O53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW53" s="66">
-        <f>P53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX53" s="66">
-        <f>Q53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY53" s="66">
-        <f>R53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ53" s="66">
-        <f>S53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA53" s="66">
-        <f>T53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB53" s="66">
-        <f>U53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC53" s="66">
-        <f>V53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD53" s="66">
-        <f>W53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE53" s="66">
-        <f>X53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF53" s="66">
-        <f>Y53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG53" s="66">
-        <f>Z53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH53" s="66">
-        <f>AA53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI53" s="66">
-        <f>AB53/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ53" s="73">
-        <f>CI53</f>
+        <v>0</v>
+      </c>
+      <c r="CJ53" s="66">
         <v>0</v>
       </c>
       <c r="CL53" s="52" t="str">
@@ -40130,104 +39627,79 @@
         <v>1</v>
       </c>
       <c r="BL54" s="66">
-        <f>E54/1000*Conversions!$B$2</f>
-        <v>1.1233365706613807</v>
+        <v>0</v>
       </c>
       <c r="BM54" s="66">
-        <f>F54/1000*Conversions!$B$2</f>
-        <v>1.1170739618738903</v>
+        <v>0</v>
       </c>
       <c r="BN54" s="66">
-        <f>G54/1000*Conversions!$B$2</f>
-        <v>1.1108113530864001</v>
+        <v>0</v>
       </c>
       <c r="BO54" s="66">
-        <f>H54/1000*Conversions!$B$2</f>
-        <v>1.1045487442989099</v>
+        <v>0</v>
       </c>
       <c r="BP54" s="66">
-        <f>I54/1000*Conversions!$B$2</f>
-        <v>1.1039455430563747</v>
+        <v>0</v>
       </c>
       <c r="BQ54" s="66">
-        <f>J54/1000*Conversions!$B$2</f>
-        <v>1.0961670648761332</v>
+        <v>0</v>
       </c>
       <c r="BR54" s="66">
-        <f>K54/1000*Conversions!$B$2</f>
-        <v>1.1023826938413788</v>
+        <v>0</v>
       </c>
       <c r="BS54" s="66">
-        <f>L54/1000*Conversions!$B$2</f>
-        <v>1.1073814452073416</v>
+        <v>0</v>
       </c>
       <c r="BT54" s="66">
-        <f>M54/1000*Conversions!$B$2</f>
-        <v>1.1115226404555034</v>
+        <v>0</v>
       </c>
       <c r="BU54" s="66">
-        <f>N54/1000*Conversions!$B$2</f>
-        <v>1.1149225801668601</v>
+        <v>0</v>
       </c>
       <c r="BV54" s="66">
-        <f>O54/1000*Conversions!$B$2</f>
-        <v>1.1185514173676627</v>
+        <v>0</v>
       </c>
       <c r="BW54" s="66">
-        <f>P54/1000*Conversions!$B$2</f>
-        <v>1.1212950054423065</v>
+        <v>0</v>
       </c>
       <c r="BX54" s="66">
-        <f>Q54/1000*Conversions!$B$2</f>
-        <v>1.122295048672705</v>
+        <v>0</v>
       </c>
       <c r="BY54" s="66">
-        <f>R54/1000*Conversions!$B$2</f>
-        <v>1.1218850224067094</v>
+        <v>0</v>
       </c>
       <c r="BZ54" s="66">
-        <f>S54/1000*Conversions!$B$2</f>
-        <v>1.1192456234714765</v>
+        <v>0</v>
       </c>
       <c r="CA54" s="66">
-        <f>T54/1000*Conversions!$B$2</f>
-        <v>1.1149914111304935</v>
+        <v>0</v>
       </c>
       <c r="CB54" s="66">
-        <f>U54/1000*Conversions!$B$2</f>
-        <v>1.1095170355369921</v>
+        <v>0</v>
       </c>
       <c r="CC54" s="66">
-        <f>V54/1000*Conversions!$B$2</f>
-        <v>1.1031181419816745</v>
+        <v>0</v>
       </c>
       <c r="CD54" s="66">
-        <f>W54/1000*Conversions!$B$2</f>
-        <v>1.0960550038943044</v>
+        <v>0</v>
       </c>
       <c r="CE54" s="66">
-        <f>X54/1000*Conversions!$B$2</f>
-        <v>1.0886066251786997</v>
+        <v>0</v>
       </c>
       <c r="CF54" s="66">
-        <f>Y54/1000*Conversions!$B$2</f>
-        <v>1.0809051069636535</v>
+        <v>0</v>
       </c>
       <c r="CG54" s="66">
-        <f>Z54/1000*Conversions!$B$2</f>
-        <v>1.073050468675754</v>
+        <v>0</v>
       </c>
       <c r="CH54" s="66">
-        <f>AA54/1000*Conversions!$B$2</f>
-        <v>1.0651835215254</v>
+        <v>0</v>
       </c>
       <c r="CI54" s="66">
-        <f>AB54/1000*Conversions!$B$2</f>
-        <v>1.0570815861128557</v>
-      </c>
-      <c r="CJ54" s="73">
-        <f>TREND(BL54:CI54,$BL$5:$CI$5,$CJ$5)</f>
-        <v>1.0587869828863461</v>
+        <v>0</v>
+      </c>
+      <c r="CJ54" s="66">
+        <v>0</v>
       </c>
       <c r="CL54" s="52" t="str">
         <f t="shared" si="10"/>
@@ -40532,104 +40004,79 @@
         <v>1</v>
       </c>
       <c r="BL55" s="66">
-        <f>E55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM55" s="66">
-        <f>F55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN55" s="66">
-        <f>G55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO55" s="66">
-        <f>H55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP55" s="66">
-        <f>I55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ55" s="66">
-        <f>J55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR55" s="66">
-        <f>K55/1000*Conversions!$B$2</f>
-        <v>5.997092219999999E-3</v>
+        <v>0</v>
       </c>
       <c r="BS55" s="66">
-        <f>L55/1000*Conversions!$B$2</f>
-        <v>2.7132503384999999E-2</v>
+        <v>0</v>
       </c>
       <c r="BT55" s="66">
-        <f>M55/1000*Conversions!$B$2</f>
-        <v>4.8605990849999989E-2</v>
+        <v>0</v>
       </c>
       <c r="BU55" s="66">
-        <f>N55/1000*Conversions!$B$2</f>
-        <v>7.0421137289999991E-2</v>
+        <v>0</v>
       </c>
       <c r="BV55" s="66">
-        <f>O55/1000*Conversions!$B$2</f>
-        <v>9.2538707639999981E-2</v>
+        <v>0</v>
       </c>
       <c r="BW55" s="66">
-        <f>P55/1000*Conversions!$B$2</f>
-        <v>0.11493683008499998</v>
+        <v>0</v>
       </c>
       <c r="BX55" s="66">
-        <f>Q55/1000*Conversions!$B$2</f>
-        <v>0.13759521722999998</v>
+        <v>0</v>
       </c>
       <c r="BY55" s="66">
-        <f>R55/1000*Conversions!$B$2</f>
-        <v>0.16049825137499998</v>
+        <v>0</v>
       </c>
       <c r="BZ55" s="66">
-        <f>S55/1000*Conversions!$B$2</f>
-        <v>0.18363313631999995</v>
+        <v>0</v>
       </c>
       <c r="CA55" s="66">
-        <f>T55/1000*Conversions!$B$2</f>
-        <v>0.20698735432499993</v>
+        <v>0</v>
       </c>
       <c r="CB55" s="66">
-        <f>U55/1000*Conversions!$B$2</f>
-        <v>0.2305830258599999</v>
+        <v>0</v>
       </c>
       <c r="CC55" s="66">
-        <f>V55/1000*Conversions!$B$2</f>
-        <v>0.25443103930499994</v>
+        <v>0</v>
       </c>
       <c r="CD55" s="66">
-        <f>W55/1000*Conversions!$B$2</f>
-        <v>0.27854301599999992</v>
+        <v>0</v>
       </c>
       <c r="CE55" s="66">
-        <f>X55/1000*Conversions!$B$2</f>
-        <v>0.28012165199999994</v>
+        <v>0</v>
       </c>
       <c r="CF55" s="66">
-        <f>Y55/1000*Conversions!$B$2</f>
-        <v>0.28170703799999991</v>
+        <v>0</v>
       </c>
       <c r="CG55" s="66">
-        <f>Z55/1000*Conversions!$B$2</f>
-        <v>0.28330462799999995</v>
+        <v>0</v>
       </c>
       <c r="CH55" s="66">
-        <f>AA55/1000*Conversions!$B$2</f>
-        <v>0.28492387199999997</v>
+        <v>0</v>
       </c>
       <c r="CI55" s="66">
-        <f>AB55/1000*Conversions!$B$2</f>
-        <v>0.28656552599999996</v>
-      </c>
-      <c r="CJ55" s="73">
-        <f>TREND(CD55:CI55,$CD$5:$CI$5,$CJ$5)</f>
-        <v>0.31058602200000029</v>
+        <v>0</v>
+      </c>
+      <c r="CJ55" s="66">
+        <v>0</v>
       </c>
       <c r="CL55" s="52" t="str">
         <f t="shared" si="10"/>
@@ -40934,104 +40381,79 @@
         <v>1</v>
       </c>
       <c r="BL56" s="66">
-        <f>E56/1000*Conversions!$B$2</f>
-        <v>0.48293664251642127</v>
+        <v>0</v>
       </c>
       <c r="BM56" s="66">
-        <f>F56/1000*Conversions!$B$2</f>
-        <v>0.30482957495881907</v>
+        <v>0</v>
       </c>
       <c r="BN56" s="66">
-        <f>G56/1000*Conversions!$B$2</f>
-        <v>0.36192017421240152</v>
+        <v>0</v>
       </c>
       <c r="BO56" s="66">
-        <f>H56/1000*Conversions!$B$2</f>
-        <v>0.34745869182124445</v>
+        <v>0</v>
       </c>
       <c r="BP56" s="66">
-        <f>I56/1000*Conversions!$B$2</f>
-        <v>0.37476142763345838</v>
+        <v>0</v>
       </c>
       <c r="BQ56" s="66">
-        <f>J56/1000*Conversions!$B$2</f>
-        <v>0.46033881816623529</v>
+        <v>0</v>
       </c>
       <c r="BR56" s="66">
-        <f>K56/1000*Conversions!$B$2</f>
-        <v>0.50041465535338936</v>
+        <v>0</v>
       </c>
       <c r="BS56" s="66">
-        <f>L56/1000*Conversions!$B$2</f>
-        <v>0.54100829675305462</v>
+        <v>0</v>
       </c>
       <c r="BT56" s="66">
-        <f>M56/1000*Conversions!$B$2</f>
-        <v>0.57972417405398491</v>
+        <v>0</v>
       </c>
       <c r="BU56" s="66">
-        <f>N56/1000*Conversions!$B$2</f>
-        <v>0.61331285770406407</v>
+        <v>0</v>
       </c>
       <c r="BV56" s="66">
-        <f>O56/1000*Conversions!$B$2</f>
-        <v>0.64126609024402248</v>
+        <v>0</v>
       </c>
       <c r="BW56" s="66">
-        <f>P56/1000*Conversions!$B$2</f>
-        <v>0.66643189150810134</v>
+        <v>0</v>
       </c>
       <c r="BX56" s="66">
-        <f>Q56/1000*Conversions!$B$2</f>
-        <v>0.69302319512955357</v>
+        <v>0</v>
       </c>
       <c r="BY56" s="66">
-        <f>R56/1000*Conversions!$B$2</f>
-        <v>0.70599570534707967</v>
+        <v>0</v>
       </c>
       <c r="BZ56" s="66">
-        <f>S56/1000*Conversions!$B$2</f>
-        <v>0.69253865341487497</v>
+        <v>0</v>
       </c>
       <c r="CA56" s="66">
-        <f>T56/1000*Conversions!$B$2</f>
-        <v>0.71002465101041778</v>
+        <v>0</v>
       </c>
       <c r="CB56" s="66">
-        <f>U56/1000*Conversions!$B$2</f>
-        <v>0.72963724484217662</v>
+        <v>0</v>
       </c>
       <c r="CC56" s="66">
-        <f>V56/1000*Conversions!$B$2</f>
-        <v>0.750898404173866</v>
+        <v>0</v>
       </c>
       <c r="CD56" s="66">
-        <f>W56/1000*Conversions!$B$2</f>
-        <v>0.77339042129322388</v>
+        <v>0</v>
       </c>
       <c r="CE56" s="66">
-        <f>X56/1000*Conversions!$B$2</f>
-        <v>0.79667606506254451</v>
+        <v>0</v>
       </c>
       <c r="CF56" s="66">
-        <f>Y56/1000*Conversions!$B$2</f>
-        <v>0.82044199464298295</v>
+        <v>0</v>
       </c>
       <c r="CG56" s="66">
-        <f>Z56/1000*Conversions!$B$2</f>
-        <v>0.8442689760595975</v>
+        <v>0</v>
       </c>
       <c r="CH56" s="66">
-        <f>AA56/1000*Conversions!$B$2</f>
-        <v>0.86791858332396399</v>
+        <v>0</v>
       </c>
       <c r="CI56" s="66">
-        <f>AB56/1000*Conversions!$B$2</f>
-        <v>0.89207540895984316</v>
-      </c>
-      <c r="CJ56" s="73">
-        <f>TREND(BT56:CI56,$BT$5:$CI$5,$CJ$5)</f>
-        <v>1.1619967782460137</v>
+        <v>0</v>
+      </c>
+      <c r="CJ56" s="66">
+        <v>0</v>
       </c>
       <c r="CL56" s="52" t="str">
         <f t="shared" si="10"/>
@@ -41336,103 +40758,78 @@
         <v>1</v>
       </c>
       <c r="BL57" s="66">
-        <f>E57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM57" s="66">
-        <f>F57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN57" s="66">
-        <f>G57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO57" s="66">
-        <f>H57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP57" s="66">
-        <f>I57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ57" s="66">
-        <f>J57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR57" s="66">
-        <f>K57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS57" s="66">
-        <f>L57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT57" s="66">
-        <f>M57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU57" s="66">
-        <f>N57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV57" s="66">
-        <f>O57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW57" s="66">
-        <f>P57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX57" s="66">
-        <f>Q57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY57" s="66">
-        <f>R57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ57" s="66">
-        <f>S57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA57" s="66">
-        <f>T57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB57" s="66">
-        <f>U57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC57" s="66">
-        <f>V57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD57" s="66">
-        <f>W57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE57" s="66">
-        <f>X57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF57" s="66">
-        <f>Y57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG57" s="66">
-        <f>Z57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH57" s="66">
-        <f>AA57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI57" s="66">
-        <f>AB57/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ57" s="73">
-        <f>CI57</f>
+        <v>0</v>
+      </c>
+      <c r="CJ57" s="66">
         <v>0</v>
       </c>
       <c r="CL57" s="52" t="str">
@@ -41738,103 +41135,78 @@
         <v>1</v>
       </c>
       <c r="BL58" s="66">
-        <f>E58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM58" s="66">
-        <f>F58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN58" s="66">
-        <f>G58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO58" s="66">
-        <f>H58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP58" s="66">
-        <f>I58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ58" s="66">
-        <f>J58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR58" s="66">
-        <f>K58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS58" s="66">
-        <f>L58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT58" s="66">
-        <f>M58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU58" s="66">
-        <f>N58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV58" s="66">
-        <f>O58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW58" s="66">
-        <f>P58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX58" s="66">
-        <f>Q58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY58" s="66">
-        <f>R58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ58" s="66">
-        <f>S58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA58" s="66">
-        <f>T58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB58" s="66">
-        <f>U58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC58" s="66">
-        <f>V58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD58" s="66">
-        <f>W58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE58" s="66">
-        <f>X58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF58" s="66">
-        <f>Y58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG58" s="66">
-        <f>Z58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH58" s="66">
-        <f>AA58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI58" s="66">
-        <f>AB58/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ58" s="73">
-        <f>CI58</f>
+        <v>0</v>
+      </c>
+      <c r="CJ58" s="66">
         <v>0</v>
       </c>
       <c r="CL58" s="52" t="str">
@@ -42140,104 +41512,79 @@
         <v>1</v>
       </c>
       <c r="BL59" s="66">
-        <f>E59/1000*Conversions!$B$2</f>
-        <v>0.10206997179437498</v>
+        <v>0</v>
       </c>
       <c r="BM59" s="66">
-        <f>F59/1000*Conversions!$B$2</f>
-        <v>0.12762687536742101</v>
+        <v>0</v>
       </c>
       <c r="BN59" s="66">
-        <f>G59/1000*Conversions!$B$2</f>
-        <v>0.13111111859407756</v>
+        <v>0</v>
       </c>
       <c r="BO59" s="66">
-        <f>H59/1000*Conversions!$B$2</f>
-        <v>0.13706461804322786</v>
+        <v>0</v>
       </c>
       <c r="BP59" s="66">
-        <f>I59/1000*Conversions!$B$2</f>
-        <v>0.14772651632149808</v>
+        <v>0</v>
       </c>
       <c r="BQ59" s="66">
-        <f>J59/1000*Conversions!$B$2</f>
-        <v>0.15305968942151191</v>
+        <v>0</v>
       </c>
       <c r="BR59" s="66">
-        <f>K59/1000*Conversions!$B$2</f>
-        <v>0.16342250661010063</v>
+        <v>0</v>
       </c>
       <c r="BS59" s="66">
-        <f>L59/1000*Conversions!$B$2</f>
-        <v>0.17411982451599994</v>
+        <v>0</v>
       </c>
       <c r="BT59" s="66">
-        <f>M59/1000*Conversions!$B$2</f>
-        <v>0.18514262911615337</v>
+        <v>0</v>
       </c>
       <c r="BU59" s="66">
-        <f>N59/1000*Conversions!$B$2</f>
-        <v>0.19540645193976094</v>
+        <v>0</v>
       </c>
       <c r="BV59" s="66">
-        <f>O59/1000*Conversions!$B$2</f>
-        <v>0.2049849195679046</v>
+        <v>0</v>
       </c>
       <c r="BW59" s="66">
-        <f>P59/1000*Conversions!$B$2</f>
-        <v>0.21484890129349377</v>
+        <v>0</v>
       </c>
       <c r="BX59" s="66">
-        <f>Q59/1000*Conversions!$B$2</f>
-        <v>0.22463133791701467</v>
+        <v>0</v>
       </c>
       <c r="BY59" s="66">
-        <f>R59/1000*Conversions!$B$2</f>
-        <v>0.23514839929326761</v>
+        <v>0</v>
       </c>
       <c r="BZ59" s="66">
-        <f>S59/1000*Conversions!$B$2</f>
-        <v>0.24603832348428883</v>
+        <v>0</v>
       </c>
       <c r="CA59" s="66">
-        <f>T59/1000*Conversions!$B$2</f>
-        <v>0.25724095232418215</v>
+        <v>0</v>
       </c>
       <c r="CB59" s="66">
-        <f>U59/1000*Conversions!$B$2</f>
-        <v>0.26156619669433079</v>
+        <v>0</v>
       </c>
       <c r="CC59" s="66">
-        <f>V59/1000*Conversions!$B$2</f>
-        <v>0.26596226492448166</v>
+        <v>0</v>
       </c>
       <c r="CD59" s="66">
-        <f>W59/1000*Conversions!$B$2</f>
-        <v>0.27043027294917671</v>
+        <v>0</v>
       </c>
       <c r="CE59" s="66">
-        <f>X59/1000*Conversions!$B$2</f>
-        <v>0.27497292588992328</v>
+        <v>0</v>
       </c>
       <c r="CF59" s="66">
-        <f>Y59/1000*Conversions!$B$2</f>
-        <v>0.27959146483132008</v>
+        <v>0</v>
       </c>
       <c r="CG59" s="66">
-        <f>Z59/1000*Conversions!$B$2</f>
-        <v>0.28428715140641891</v>
+        <v>0</v>
       </c>
       <c r="CH59" s="66">
-        <f>AA59/1000*Conversions!$B$2</f>
-        <v>0.28906126813568656</v>
+        <v>0</v>
       </c>
       <c r="CI59" s="66">
-        <f>AB59/1000*Conversions!$B$2</f>
-        <v>0.29391511877153675</v>
-      </c>
-      <c r="CJ59" s="73">
-        <f>TREND(BT59:CI59,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.4109850441439864</v>
+        <v>0</v>
+      </c>
+      <c r="CJ59" s="66">
+        <v>0</v>
       </c>
       <c r="CL59" s="52" t="str">
         <f t="shared" si="10"/>
@@ -42542,104 +41889,79 @@
         <v>1</v>
       </c>
       <c r="BL60" s="66">
-        <f>E60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM60" s="66">
-        <f>F60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN60" s="66">
-        <f>G60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO60" s="66">
-        <f>H60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP60" s="66">
-        <f>I60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ60" s="66">
-        <f>J60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR60" s="66">
-        <f>K60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS60" s="66">
-        <f>L60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT60" s="66">
-        <f>M60/1000*Conversions!$B$2</f>
-        <v>0.11177066666666664</v>
+        <v>0</v>
       </c>
       <c r="BU60" s="66">
-        <f>N60/1000*Conversions!$B$2</f>
-        <v>0.21576779999999993</v>
+        <v>0</v>
       </c>
       <c r="BV60" s="66">
-        <f>O60/1000*Conversions!$B$2</f>
-        <v>0.28075159999999988</v>
+        <v>0</v>
       </c>
       <c r="BW60" s="66">
-        <f>P60/1000*Conversions!$B$2</f>
-        <v>0.28417539999999991</v>
+        <v>0</v>
       </c>
       <c r="BX60" s="66">
-        <f>Q60/1000*Conversions!$B$2</f>
-        <v>0.28759919999999989</v>
+        <v>0</v>
       </c>
       <c r="BY60" s="66">
-        <f>R60/1000*Conversions!$B$2</f>
-        <v>0.29102299999999987</v>
+        <v>0</v>
       </c>
       <c r="BZ60" s="66">
-        <f>S60/1000*Conversions!$B$2</f>
-        <v>0.2944467999999999</v>
+        <v>0</v>
       </c>
       <c r="CA60" s="66">
-        <f>T60/1000*Conversions!$B$2</f>
-        <v>0.29787059999999987</v>
+        <v>0</v>
       </c>
       <c r="CB60" s="66">
-        <f>U60/1000*Conversions!$B$2</f>
-        <v>0.30129439999999985</v>
+        <v>0</v>
       </c>
       <c r="CC60" s="66">
-        <f>V60/1000*Conversions!$B$2</f>
-        <v>0.30471819999999983</v>
+        <v>0</v>
       </c>
       <c r="CD60" s="66">
-        <f>W60/1000*Conversions!$B$2</f>
-        <v>0.30814200000000003</v>
+        <v>0</v>
       </c>
       <c r="CE60" s="66">
-        <f>X60/1000*Conversions!$B$2</f>
-        <v>0.31156580000000017</v>
+        <v>0</v>
       </c>
       <c r="CF60" s="66">
-        <f>Y60/1000*Conversions!$B$2</f>
-        <v>0.31498960000000037</v>
+        <v>0</v>
       </c>
       <c r="CG60" s="66">
-        <f>Z60/1000*Conversions!$B$2</f>
-        <v>0.31841340000000051</v>
+        <v>0</v>
       </c>
       <c r="CH60" s="66">
-        <f>AA60/1000*Conversions!$B$2</f>
-        <v>0.32183720000000066</v>
+        <v>0</v>
       </c>
       <c r="CI60" s="66">
-        <f>AB60/1000*Conversions!$B$2</f>
-        <v>0.32526100000000085</v>
-      </c>
-      <c r="CJ60" s="73">
-        <f>TREND(BT60:CI60,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.46958760784313824</v>
+        <v>0</v>
+      </c>
+      <c r="CJ60" s="66">
+        <v>0</v>
       </c>
       <c r="CL60" s="52" t="str">
         <f t="shared" si="10"/>
@@ -42944,103 +42266,78 @@
         <v>1</v>
       </c>
       <c r="BL61" s="66">
-        <f>E61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM61" s="66">
-        <f>F61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN61" s="66">
-        <f>G61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO61" s="66">
-        <f>H61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP61" s="66">
-        <f>I61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ61" s="66">
-        <f>J61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR61" s="66">
-        <f>K61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS61" s="66">
-        <f>L61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT61" s="66">
-        <f>M61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU61" s="66">
-        <f>N61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV61" s="66">
-        <f>O61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW61" s="66">
-        <f>P61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX61" s="66">
-        <f>Q61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY61" s="66">
-        <f>R61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ61" s="66">
-        <f>S61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA61" s="66">
-        <f>T61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB61" s="66">
-        <f>U61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC61" s="66">
-        <f>V61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD61" s="66">
-        <f>W61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE61" s="66">
-        <f>X61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF61" s="66">
-        <f>Y61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG61" s="66">
-        <f>Z61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH61" s="66">
-        <f>AA61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI61" s="66">
-        <f>AB61/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ61" s="73">
-        <f>CI61</f>
+        <v>0</v>
+      </c>
+      <c r="CJ61" s="66">
         <v>0</v>
       </c>
       <c r="CL61" s="52" t="str">
@@ -43346,104 +42643,79 @@
         <v>1</v>
       </c>
       <c r="BL62" s="66">
-        <f>E62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM62" s="66">
-        <f>F62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN62" s="66">
-        <f>G62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO62" s="66">
-        <f>H62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP62" s="66">
-        <f>I62/1000*Conversions!$B$2</f>
-        <v>7.2944130014083855E-2</v>
+        <v>0</v>
       </c>
       <c r="BQ62" s="66">
-        <f>J62/1000*Conversions!$B$2</f>
-        <v>0.1469297913232096</v>
+        <v>0</v>
       </c>
       <c r="BR62" s="66">
-        <f>K62/1000*Conversions!$B$2</f>
-        <v>0.22211680582022408</v>
+        <v>0</v>
       </c>
       <c r="BS62" s="66">
-        <f>L62/1000*Conversions!$B$2</f>
-        <v>0.29831514520493668</v>
+        <v>0</v>
       </c>
       <c r="BT62" s="66">
-        <f>M62/1000*Conversions!$B$2</f>
-        <v>0.37533571223005058</v>
+        <v>0</v>
       </c>
       <c r="BU62" s="66">
-        <f>N62/1000*Conversions!$B$2</f>
-        <v>0.37798947776995845</v>
+        <v>0</v>
       </c>
       <c r="BV62" s="66">
-        <f>O62/1000*Conversions!$B$2</f>
-        <v>0.38064324330986632</v>
+        <v>0</v>
       </c>
       <c r="BW62" s="66">
-        <f>P62/1000*Conversions!$B$2</f>
-        <v>0.38329700884977419</v>
+        <v>0</v>
       </c>
       <c r="BX62" s="66">
-        <f>Q62/1000*Conversions!$B$2</f>
-        <v>0.38595077438968212</v>
+        <v>0</v>
       </c>
       <c r="BY62" s="66">
-        <f>R62/1000*Conversions!$B$2</f>
-        <v>0.38860453992958988</v>
+        <v>0</v>
       </c>
       <c r="BZ62" s="66">
-        <f>S62/1000*Conversions!$B$2</f>
-        <v>0.3912583054694978</v>
+        <v>0</v>
       </c>
       <c r="CA62" s="66">
-        <f>T62/1000*Conversions!$B$2</f>
-        <v>0.39391207100940567</v>
+        <v>0</v>
       </c>
       <c r="CB62" s="66">
-        <f>U62/1000*Conversions!$B$2</f>
-        <v>0.39656583654931354</v>
+        <v>0</v>
       </c>
       <c r="CC62" s="66">
-        <f>V62/1000*Conversions!$B$2</f>
-        <v>0.3992196020892213</v>
+        <v>0</v>
       </c>
       <c r="CD62" s="66">
-        <f>W62/1000*Conversions!$B$2</f>
-        <v>0.40187336762912917</v>
+        <v>0</v>
       </c>
       <c r="CE62" s="66">
-        <f>X62/1000*Conversions!$B$2</f>
-        <v>0.4045271331690371</v>
+        <v>0</v>
       </c>
       <c r="CF62" s="66">
-        <f>Y62/1000*Conversions!$B$2</f>
-        <v>0.40718089870894497</v>
+        <v>0</v>
       </c>
       <c r="CG62" s="66">
-        <f>Z62/1000*Conversions!$B$2</f>
-        <v>0.40983466424885284</v>
+        <v>0</v>
       </c>
       <c r="CH62" s="66">
-        <f>AA62/1000*Conversions!$B$2</f>
-        <v>0.41248842978876071</v>
+        <v>0</v>
       </c>
       <c r="CI62" s="66">
-        <f>AB62/1000*Conversions!$B$2</f>
-        <v>0.41514219532866864</v>
-      </c>
-      <c r="CJ62" s="73">
-        <f>TREND(BT62:CI62,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.4549486784272867</v>
+        <v>0</v>
+      </c>
+      <c r="CJ62" s="66">
+        <v>0</v>
       </c>
       <c r="CL62" s="52" t="str">
         <f t="shared" si="10"/>
@@ -43748,104 +43020,79 @@
         <v>1</v>
       </c>
       <c r="BL63" s="66">
-        <f>E63/1000*Conversions!$B$2</f>
-        <v>0.37559879906054899</v>
+        <v>0</v>
       </c>
       <c r="BM63" s="66">
-        <f>F63/1000*Conversions!$B$2</f>
-        <v>0.49249247408524666</v>
+        <v>0</v>
       </c>
       <c r="BN63" s="66">
-        <f>G63/1000*Conversions!$B$2</f>
-        <v>0.24821620693896435</v>
+        <v>0</v>
       </c>
       <c r="BO63" s="66">
-        <f>H63/1000*Conversions!$B$2</f>
-        <v>0.18765145244585704</v>
+        <v>0</v>
       </c>
       <c r="BP63" s="66">
-        <f>I63/1000*Conversions!$B$2</f>
-        <v>0.50440710417446366</v>
+        <v>0</v>
       </c>
       <c r="BQ63" s="66">
-        <f>J63/1000*Conversions!$B$2</f>
-        <v>0.85799648420076269</v>
+        <v>0</v>
       </c>
       <c r="BR63" s="66">
-        <f>K63/1000*Conversions!$B$2</f>
-        <v>1.2172110122528155</v>
+        <v>0</v>
       </c>
       <c r="BS63" s="66">
-        <f>L63/1000*Conversions!$B$2</f>
-        <v>1.582118060978712</v>
+        <v>0</v>
       </c>
       <c r="BT63" s="66">
-        <f>M63/1000*Conversions!$B$2</f>
-        <v>1.9495310781111395</v>
+        <v>0</v>
       </c>
       <c r="BU63" s="66">
-        <f>N63/1000*Conversions!$B$2</f>
-        <v>1.965127326736029</v>
+        <v>0</v>
       </c>
       <c r="BV63" s="66">
-        <f>O63/1000*Conversions!$B$2</f>
-        <v>1.9808483453499168</v>
+        <v>0</v>
       </c>
       <c r="BW63" s="66">
-        <f>P63/1000*Conversions!$B$2</f>
-        <v>1.9966951321127162</v>
+        <v>0</v>
       </c>
       <c r="BX63" s="66">
-        <f>Q63/1000*Conversions!$B$2</f>
-        <v>2.0126686931696178</v>
+        <v>0</v>
       </c>
       <c r="BY63" s="66">
-        <f>R63/1000*Conversions!$B$2</f>
-        <v>2.0287700427149744</v>
+        <v>0</v>
       </c>
       <c r="BZ63" s="66">
-        <f>S63/1000*Conversions!$B$2</f>
-        <v>2.0450002030566945</v>
+        <v>0</v>
       </c>
       <c r="CA63" s="66">
-        <f>T63/1000*Conversions!$B$2</f>
-        <v>2.0613602046811486</v>
+        <v>0</v>
       </c>
       <c r="CB63" s="66">
-        <f>U63/1000*Conversions!$B$2</f>
-        <v>2.0778510863185975</v>
+        <v>0</v>
       </c>
       <c r="CC63" s="66">
-        <f>V63/1000*Conversions!$B$2</f>
-        <v>2.0944738950091462</v>
+        <v>0</v>
       </c>
       <c r="CD63" s="66">
-        <f>W63/1000*Conversions!$B$2</f>
-        <v>2.111229686169219</v>
+        <v>0</v>
       </c>
       <c r="CE63" s="66">
-        <f>X63/1000*Conversions!$B$2</f>
-        <v>2.127985477329291</v>
+        <v>0</v>
       </c>
       <c r="CF63" s="66">
-        <f>Y63/1000*Conversions!$B$2</f>
-        <v>2.1447412684893634</v>
+        <v>0</v>
       </c>
       <c r="CG63" s="66">
-        <f>Z63/1000*Conversions!$B$2</f>
-        <v>2.1614970596494354</v>
+        <v>0</v>
       </c>
       <c r="CH63" s="66">
-        <f>AA63/1000*Conversions!$B$2</f>
-        <v>2.1782528508095123</v>
+        <v>0</v>
       </c>
       <c r="CI63" s="66">
-        <f>AB63/1000*Conversions!$B$2</f>
-        <v>2.1950086419695851</v>
-      </c>
-      <c r="CJ63" s="73">
-        <f>TREND(BT63:CI63,$BT$5:$CI$5,$CJ$5)</f>
-        <v>2.439848025856989</v>
+        <v>0</v>
+      </c>
+      <c r="CJ63" s="66">
+        <v>0</v>
       </c>
       <c r="CL63" s="52" t="str">
         <f t="shared" si="10"/>
@@ -44150,104 +43397,79 @@
         <v>1</v>
       </c>
       <c r="BL64" s="66">
-        <f>E64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM64" s="66">
-        <f>F64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN64" s="66">
-        <f>G64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO64" s="66">
-        <f>H64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP64" s="66">
-        <f>I64/1000*Conversions!$B$2</f>
-        <v>3.4457514931740612</v>
+        <v>0</v>
       </c>
       <c r="BQ64" s="66">
-        <f>J64/1000*Conversions!$B$2</f>
-        <v>4.7212840634542843</v>
+        <v>0</v>
       </c>
       <c r="BR64" s="66">
-        <f>K64/1000*Conversions!$B$2</f>
-        <v>6.0602910033456077</v>
+        <v>0</v>
       </c>
       <c r="BS64" s="66">
-        <f>L64/1000*Conversions!$B$2</f>
-        <v>7.4627723128480321</v>
+        <v>0</v>
       </c>
       <c r="BT64" s="66">
-        <f>M64/1000*Conversions!$B$2</f>
-        <v>8.9287279919615585</v>
+        <v>0</v>
       </c>
       <c r="BU64" s="66">
-        <f>N64/1000*Conversions!$B$2</f>
-        <v>10.458158040686186</v>
+        <v>0</v>
       </c>
       <c r="BV64" s="66">
-        <f>O64/1000*Conversions!$B$2</f>
-        <v>10.998985577678733</v>
+        <v>0</v>
       </c>
       <c r="BW64" s="66">
-        <f>P64/1000*Conversions!$B$2</f>
-        <v>11.553414765302227</v>
+        <v>0</v>
       </c>
       <c r="BX64" s="66">
-        <f>Q64/1000*Conversions!$B$2</f>
-        <v>12.121445603556674</v>
+        <v>0</v>
       </c>
       <c r="BY64" s="66">
-        <f>R64/1000*Conversions!$B$2</f>
-        <v>12.703078092442071</v>
+        <v>0</v>
       </c>
       <c r="BZ64" s="66">
-        <f>S64/1000*Conversions!$B$2</f>
-        <v>13.298312231958416</v>
+        <v>0</v>
       </c>
       <c r="CA64" s="66">
-        <f>T64/1000*Conversions!$B$2</f>
-        <v>13.907148022105712</v>
+        <v>0</v>
       </c>
       <c r="CB64" s="66">
-        <f>U64/1000*Conversions!$B$2</f>
-        <v>14.529585462883961</v>
+        <v>0</v>
       </c>
       <c r="CC64" s="66">
-        <f>V64/1000*Conversions!$B$2</f>
-        <v>15.165624554293162</v>
+        <v>0</v>
       </c>
       <c r="CD64" s="66">
-        <f>W64/1000*Conversions!$B$2</f>
-        <v>15.81526529633331</v>
+        <v>0</v>
       </c>
       <c r="CE64" s="66">
-        <f>X64/1000*Conversions!$B$2</f>
-        <v>16.47850768900441</v>
+        <v>0</v>
       </c>
       <c r="CF64" s="66">
-        <f>Y64/1000*Conversions!$B$2</f>
-        <v>17.155351732306457</v>
+        <v>0</v>
       </c>
       <c r="CG64" s="66">
-        <f>Z64/1000*Conversions!$B$2</f>
-        <v>17.845797426239457</v>
+        <v>0</v>
       </c>
       <c r="CH64" s="66">
-        <f>AA64/1000*Conversions!$B$2</f>
-        <v>18.549844770803404</v>
+        <v>0</v>
       </c>
       <c r="CI64" s="66">
-        <f>AB64/1000*Conversions!$B$2</f>
-        <v>19.267493765998299</v>
-      </c>
-      <c r="CJ64" s="73">
-        <f>TREND(BT64:CI64,$BT$5:$CI$5,$CJ$5)</f>
-        <v>28.800806238537689</v>
+        <v>0</v>
+      </c>
+      <c r="CJ64" s="66">
+        <v>0</v>
       </c>
       <c r="CL64" s="52" t="str">
         <f t="shared" si="10"/>
@@ -44552,103 +43774,78 @@
         <v>1</v>
       </c>
       <c r="BL65" s="66">
-        <f>E65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM65" s="66">
-        <f>F65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN65" s="66">
-        <f>G65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO65" s="66">
-        <f>H65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP65" s="66">
-        <f>I65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ65" s="66">
-        <f>J65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR65" s="66">
-        <f>K65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS65" s="66">
-        <f>L65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT65" s="66">
-        <f>M65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU65" s="66">
-        <f>N65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV65" s="66">
-        <f>O65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW65" s="66">
-        <f>P65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX65" s="66">
-        <f>Q65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY65" s="66">
-        <f>R65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ65" s="66">
-        <f>S65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA65" s="66">
-        <f>T65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB65" s="66">
-        <f>U65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC65" s="66">
-        <f>V65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD65" s="66">
-        <f>W65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE65" s="66">
-        <f>X65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF65" s="66">
-        <f>Y65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG65" s="66">
-        <f>Z65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH65" s="66">
-        <f>AA65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI65" s="66">
-        <f>AB65/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ65" s="73">
-        <f>CI65</f>
+        <v>0</v>
+      </c>
+      <c r="CJ65" s="66">
         <v>0</v>
       </c>
       <c r="CL65" s="52" t="str">
@@ -44885,7 +44082,7 @@
     <row r="67" spans="1:119" x14ac:dyDescent="0.25">
       <c r="CJ67" s="66">
         <f>SUM(CJ6:CJ21,CJ28:CJ43,CJ50:CJ65)</f>
-        <v>188.50791202135417</v>
+        <v>74.590379859698629</v>
       </c>
       <c r="CK67" s="52" t="s">
         <v>1</v>
@@ -44924,7 +44121,7 @@
       <c r="BC68" s="20"/>
       <c r="CJ68" s="67">
         <f>CJ67*1000/Conversions!$B$2</f>
-        <v>4502434.1268117456</v>
+        <v>1781560.6157375234</v>
       </c>
       <c r="CK68" s="52" t="s">
         <v>19</v>
@@ -45299,12 +44496,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45454,15 +44648,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B7E6A7-FFA9-474C-81D0-41CF87028AB1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0B387-229C-4E2C-9ACB-57F10C5B7407}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45486,10 +44684,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0B387-229C-4E2C-9ACB-57F10C5B7407}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B7E6A7-FFA9-474C-81D0-41CF87028AB1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update low bio potential
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
+++ b/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\ccr-40\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DCEAC2-FCE2-42D8-9216-F5355325BE80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC326A4-C633-4BC2-A4CE-B40223D87D81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BioenergySupply-Baseline" sheetId="17" r:id="rId1"/>
@@ -1576,8 +1576,8 @@
   </sheetPr>
   <dimension ref="A1:DQ68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BH44" sqref="BH44"/>
+    <sheetView tabSelected="1" topLeftCell="AO4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BL28" sqref="BL28:CK43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9475,107 +9475,82 @@
         <v>1</v>
       </c>
       <c r="BL28" s="66">
-        <f>E28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM28" s="66">
-        <f>F28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN28" s="66">
-        <f>G28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO28" s="66">
-        <f>H28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP28" s="66">
-        <f>I28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ28" s="66">
-        <f>J28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR28" s="66">
-        <f>K28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS28" s="66">
-        <f>L28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT28" s="66">
-        <f>M28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU28" s="66">
-        <f>N28/1000*Conversions!$B$2</f>
-        <v>6.2099999999999994E-3</v>
+        <v>0</v>
       </c>
       <c r="BV28" s="66">
-        <f>O28/1000*Conversions!$B$2</f>
-        <v>1.2419999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="BW28" s="66">
-        <f>P28/1000*Conversions!$B$2</f>
-        <v>2.0182500000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="BX28" s="66">
-        <f>Q28/1000*Conversions!$B$2</f>
-        <v>2.5530000000000004E-2</v>
+        <v>0</v>
       </c>
       <c r="BY28" s="66">
-        <f>R28/1000*Conversions!$B$2</f>
-        <v>3.1912500000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="BZ28" s="66">
-        <f>S28/1000*Conversions!$B$2</f>
-        <v>3.7260000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="CA28" s="66">
-        <f>T28/1000*Conversions!$B$2</f>
-        <v>4.3470000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="CB28" s="66">
-        <f>U28/1000*Conversions!$B$2</f>
-        <v>4.692000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="CC28" s="66">
-        <f>V28/1000*Conversions!$B$2</f>
-        <v>5.12325E-2</v>
+        <v>0</v>
       </c>
       <c r="CD28" s="66">
-        <f>W28/1000*Conversions!$B$2</f>
-        <v>5.6925000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="CE28" s="66">
-        <f>X28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF28" s="66">
-        <f>Y28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG28" s="66">
-        <f>Z28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH28" s="66">
-        <f>AA28/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI28" s="66">
-        <f>AB28/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ28" s="73">
-        <f>CI28</f>
-        <v>0</v>
-      </c>
-      <c r="CK28" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ28" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK28" s="66">
+        <v>0</v>
       </c>
       <c r="CM28" s="52" t="str">
         <f t="shared" ref="CM28:CM43" si="4">BG28</f>
@@ -9883,107 +9858,82 @@
         <v>1</v>
       </c>
       <c r="BL29" s="66">
-        <f>E29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM29" s="66">
-        <f>F29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN29" s="66">
-        <f>G29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO29" s="66">
-        <f>H29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP29" s="66">
-        <f>I29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ29" s="66">
-        <f>J29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR29" s="66">
-        <f>K29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS29" s="66">
-        <f>L29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT29" s="66">
-        <f>M29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU29" s="66">
-        <f>N29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV29" s="66">
-        <f>O29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW29" s="66">
-        <f>P29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX29" s="66">
-        <f>Q29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY29" s="66">
-        <f>R29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ29" s="66">
-        <f>S29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA29" s="66">
-        <f>T29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB29" s="66">
-        <f>U29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC29" s="66">
-        <f>V29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD29" s="66">
-        <f>W29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE29" s="66">
-        <f>X29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF29" s="66">
-        <f>Y29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG29" s="66">
-        <f>Z29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH29" s="66">
-        <f>AA29/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI29" s="66">
-        <f>AB29/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ29" s="73">
-        <f>CI29</f>
-        <v>0</v>
-      </c>
-      <c r="CK29" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ29" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK29" s="66">
+        <v>0</v>
       </c>
       <c r="CM29" s="52" t="str">
         <f t="shared" si="4"/>
@@ -10291,107 +10241,82 @@
         <v>1</v>
       </c>
       <c r="BL30" s="66">
-        <f>E30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM30" s="66">
-        <f>F30/1000*Conversions!$B$2</f>
-        <v>5.1812930016045949E-17</v>
+        <v>0</v>
       </c>
       <c r="BN30" s="66">
-        <f>G30/1000*Conversions!$B$2</f>
-        <v>5.219026286149803E-17</v>
+        <v>0</v>
       </c>
       <c r="BO30" s="66">
-        <f>H30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP30" s="66">
-        <f>I30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ30" s="66">
-        <f>J30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR30" s="66">
-        <f>K30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS30" s="66">
-        <f>L30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT30" s="66">
-        <f>M30/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU30" s="66">
-        <f>N30/1000*Conversions!$B$2</f>
-        <v>2.807786322151316E-2</v>
+        <v>0</v>
       </c>
       <c r="BV30" s="66">
-        <f>O30/1000*Conversions!$B$2</f>
-        <v>5.6980968889485645E-2</v>
+        <v>0</v>
       </c>
       <c r="BW30" s="66">
-        <f>P30/1000*Conversions!$B$2</f>
-        <v>8.6734066550921973E-2</v>
+        <v>0</v>
       </c>
       <c r="BX30" s="66">
-        <f>Q30/1000*Conversions!$B$2</f>
-        <v>0.11716682271649489</v>
+        <v>0</v>
       </c>
       <c r="BY30" s="66">
-        <f>R30/1000*Conversions!$B$2</f>
-        <v>0.14869140948565346</v>
+        <v>0</v>
       </c>
       <c r="BZ30" s="66">
-        <f>S30/1000*Conversions!$B$2</f>
-        <v>0.18120432867915748</v>
+        <v>0</v>
       </c>
       <c r="CA30" s="66">
-        <f>T30/1000*Conversions!$B$2</f>
-        <v>0.21469246452501728</v>
+        <v>0</v>
       </c>
       <c r="CB30" s="66">
-        <f>U30/1000*Conversions!$B$2</f>
-        <v>0.24917828484863763</v>
+        <v>0</v>
       </c>
       <c r="CC30" s="66">
-        <f>V30/1000*Conversions!$B$2</f>
-        <v>0.28468472041951881</v>
+        <v>0</v>
       </c>
       <c r="CD30" s="66">
-        <f>W30/1000*Conversions!$B$2</f>
-        <v>0.48185276087417128</v>
+        <v>0</v>
       </c>
       <c r="CE30" s="66">
-        <f>X30/1000*Conversions!$B$2</f>
-        <v>0.48934572144211735</v>
+        <v>0</v>
       </c>
       <c r="CF30" s="66">
-        <f>Y30/1000*Conversions!$B$2</f>
-        <v>0.49695519988156245</v>
+        <v>0</v>
       </c>
       <c r="CG30" s="66">
-        <f>Z30/1000*Conversions!$B$2</f>
-        <v>0.50468300808171207</v>
+        <v>0</v>
       </c>
       <c r="CH30" s="66">
-        <f>AA30/1000*Conversions!$B$2</f>
-        <v>0.51253098610721592</v>
+        <v>0</v>
       </c>
       <c r="CI30" s="66">
-        <f>AB30/1000*Conversions!$B$2</f>
-        <v>0.52050100263629984</v>
-      </c>
-      <c r="CJ30" s="73">
-        <f>TREND(CD30:CI30,$CD$5:$CI$5,$CJ$5)</f>
-        <v>0.63624051867355824</v>
-      </c>
-      <c r="CK30" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ30" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK30" s="66">
+        <v>0</v>
       </c>
       <c r="CM30" s="52" t="str">
         <f t="shared" si="4"/>
@@ -10697,107 +10622,82 @@
         <v>1</v>
       </c>
       <c r="BL31" s="66">
-        <f>E31/1000*Conversions!$B$2</f>
-        <v>2.0096724582357348</v>
+        <v>0</v>
       </c>
       <c r="BM31" s="66">
-        <f>F31/1000*Conversions!$B$2</f>
-        <v>3.6110097381970108</v>
+        <v>0</v>
       </c>
       <c r="BN31" s="66">
-        <f>G31/1000*Conversions!$B$2</f>
-        <v>3.3041335877500391</v>
+        <v>0</v>
       </c>
       <c r="BO31" s="66">
-        <f>H31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP31" s="66">
-        <f>I31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ31" s="66">
-        <f>J31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR31" s="66">
-        <f>K31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS31" s="66">
-        <f>L31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT31" s="66">
-        <f>M31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU31" s="66">
-        <f>N31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV31" s="66">
-        <f>O31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW31" s="66">
-        <f>P31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX31" s="66">
-        <f>Q31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY31" s="66">
-        <f>R31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ31" s="66">
-        <f>S31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA31" s="66">
-        <f>T31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB31" s="66">
-        <f>U31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC31" s="66">
-        <f>V31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD31" s="66">
-        <f>W31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE31" s="66">
-        <f>X31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF31" s="66">
-        <f>Y31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG31" s="66">
-        <f>Z31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH31" s="66">
-        <f>AA31/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI31" s="66">
-        <f>AB31/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ31" s="73">
-        <f>CI31</f>
-        <v>0</v>
-      </c>
-      <c r="CK31" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ31" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK31" s="66">
+        <v>0</v>
       </c>
       <c r="CM31" s="52" t="str">
         <f t="shared" si="4"/>
@@ -11105,107 +11005,82 @@
         <v>1</v>
       </c>
       <c r="BL32" s="66">
-        <f>E32/1000*Conversions!$B$2</f>
-        <v>0.60833943916817546</v>
+        <v>0</v>
       </c>
       <c r="BM32" s="66">
-        <f>F32/1000*Conversions!$B$2</f>
-        <v>0.60494794278408781</v>
+        <v>0</v>
       </c>
       <c r="BN32" s="66">
-        <f>G32/1000*Conversions!$B$2</f>
-        <v>0.60155644640000006</v>
+        <v>0</v>
       </c>
       <c r="BO32" s="66">
-        <f>H32/1000*Conversions!$B$2</f>
-        <v>0.59816495001591241</v>
+        <v>0</v>
       </c>
       <c r="BP32" s="66">
-        <f>I32/1000*Conversions!$B$2</f>
-        <v>0.59783828825204466</v>
+        <v>0</v>
       </c>
       <c r="BQ32" s="66">
-        <f>J32/1000*Conversions!$B$2</f>
-        <v>0.59362587749525431</v>
+        <v>0</v>
       </c>
       <c r="BR32" s="66">
-        <f>K32/1000*Conversions!$B$2</f>
-        <v>0.59699193210217305</v>
+        <v>0</v>
       </c>
       <c r="BS32" s="66">
-        <f>L32/1000*Conversions!$B$2</f>
-        <v>0.59969899041571162</v>
+        <v>0</v>
       </c>
       <c r="BT32" s="66">
-        <f>M32/1000*Conversions!$B$2</f>
-        <v>0.60194164187080423</v>
+        <v>0</v>
       </c>
       <c r="BU32" s="66">
-        <f>N32/1000*Conversions!$B$2</f>
-        <v>0.6037828686867307</v>
+        <v>0</v>
       </c>
       <c r="BV32" s="66">
-        <f>O32/1000*Conversions!$B$2</f>
-        <v>0.6057480542288245</v>
+        <v>0</v>
       </c>
       <c r="BW32" s="66">
-        <f>P32/1000*Conversions!$B$2</f>
-        <v>0.60723383584960289</v>
+        <v>0</v>
       </c>
       <c r="BX32" s="66">
-        <f>Q32/1000*Conversions!$B$2</f>
-        <v>0.60777540616237802</v>
+        <v>0</v>
       </c>
       <c r="BY32" s="66">
-        <f>R32/1000*Conversions!$B$2</f>
-        <v>0.60755335770849983</v>
+        <v>0</v>
       </c>
       <c r="BZ32" s="66">
-        <f>S32/1000*Conversions!$B$2</f>
-        <v>0.60612399939333761</v>
+        <v>0</v>
       </c>
       <c r="CA32" s="66">
-        <f>T32/1000*Conversions!$B$2</f>
-        <v>0.60382014388181271</v>
+        <v>0</v>
       </c>
       <c r="CB32" s="66">
-        <f>U32/1000*Conversions!$B$2</f>
-        <v>0.60085551274157856</v>
+        <v>0</v>
       </c>
       <c r="CC32" s="66">
-        <f>V32/1000*Conversions!$B$2</f>
-        <v>0.59739021176375418</v>
+        <v>0</v>
       </c>
       <c r="CD32" s="66">
-        <f>W32/1000*Conversions!$B$2</f>
-        <v>0.59356519121776741</v>
+        <v>0</v>
       </c>
       <c r="CE32" s="66">
-        <f>X32/1000*Conversions!$B$2</f>
-        <v>0.58953154480323344</v>
+        <v>0</v>
       </c>
       <c r="CF32" s="66">
-        <f>Y32/1000*Conversions!$B$2</f>
-        <v>0.58536081147713315</v>
+        <v>0</v>
       </c>
       <c r="CG32" s="66">
-        <f>Z32/1000*Conversions!$B$2</f>
-        <v>0.58110715645002375</v>
+        <v>0</v>
       </c>
       <c r="CH32" s="66">
-        <f>AA32/1000*Conversions!$B$2</f>
-        <v>0.576846835596591</v>
+        <v>0</v>
       </c>
       <c r="CI32" s="66">
-        <f>AB32/1000*Conversions!$B$2</f>
-        <v>0.57245925757788385</v>
-      </c>
-      <c r="CJ32" s="73">
-        <f>CI32</f>
-        <v>0.57245925757788385</v>
-      </c>
-      <c r="CK32" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ32" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK32" s="66">
+        <v>0</v>
       </c>
       <c r="CM32" s="52" t="str">
         <f t="shared" si="4"/>
@@ -11513,107 +11388,82 @@
         <v>1</v>
       </c>
       <c r="BL33" s="66">
-        <f>E33/1000*Conversions!$B$2</f>
-        <v>0.16513689600000003</v>
+        <v>0</v>
       </c>
       <c r="BM33" s="66">
-        <f>F33/1000*Conversions!$B$2</f>
-        <v>0.165740796</v>
+        <v>0</v>
       </c>
       <c r="BN33" s="66">
-        <f>G33/1000*Conversions!$B$2</f>
-        <v>0.16655122800000002</v>
+        <v>0</v>
       </c>
       <c r="BO33" s="66">
-        <f>H33/1000*Conversions!$B$2</f>
-        <v>0.16754954400000002</v>
+        <v>0</v>
       </c>
       <c r="BP33" s="66">
-        <f>I33/1000*Conversions!$B$2</f>
-        <v>0.16871342400000003</v>
+        <v>0</v>
       </c>
       <c r="BQ33" s="66">
-        <f>J33/1000*Conversions!$B$2</f>
-        <v>0.16996435199999999</v>
+        <v>0</v>
       </c>
       <c r="BR33" s="66">
-        <f>K33/1000*Conversions!$B$2</f>
-        <v>0.17134549199999999</v>
+        <v>0</v>
       </c>
       <c r="BS33" s="66">
-        <f>L33/1000*Conversions!$B$2</f>
-        <v>0.17272681199999998</v>
+        <v>0</v>
       </c>
       <c r="BT33" s="66">
-        <f>M33/1000*Conversions!$B$2</f>
-        <v>0.17411101199999998</v>
+        <v>0</v>
       </c>
       <c r="BU33" s="66">
-        <f>N33/1000*Conversions!$B$2</f>
-        <v>0.17550439200000001</v>
+        <v>0</v>
       </c>
       <c r="BV33" s="66">
-        <f>O33/1000*Conversions!$B$2</f>
-        <v>0.17682555599999999</v>
+        <v>0</v>
       </c>
       <c r="BW33" s="66">
-        <f>P33/1000*Conversions!$B$2</f>
-        <v>0.17808159600000001</v>
+        <v>0</v>
       </c>
       <c r="BX33" s="66">
-        <f>Q33/1000*Conversions!$B$2</f>
-        <v>0.17927715600000002</v>
+        <v>0</v>
       </c>
       <c r="BY33" s="66">
-        <f>R33/1000*Conversions!$B$2</f>
-        <v>0.18041958</v>
+        <v>0</v>
       </c>
       <c r="BZ33" s="66">
-        <f>S33/1000*Conversions!$B$2</f>
-        <v>0.18151545600000005</v>
+        <v>0</v>
       </c>
       <c r="CA33" s="66">
-        <f>T33/1000*Conversions!$B$2</f>
-        <v>0.18256878000000001</v>
+        <v>0</v>
       </c>
       <c r="CB33" s="66">
-        <f>U33/1000*Conversions!$B$2</f>
-        <v>0.18360957600000002</v>
+        <v>0</v>
       </c>
       <c r="CC33" s="66">
-        <f>V33/1000*Conversions!$B$2</f>
-        <v>0.18464907600000005</v>
+        <v>0</v>
       </c>
       <c r="CD33" s="66">
-        <f>W33/1000*Conversions!$B$2</f>
-        <v>0.18569534400000004</v>
+        <v>0</v>
       </c>
       <c r="CE33" s="66">
-        <f>X33/1000*Conversions!$B$2</f>
-        <v>0.18674776800000001</v>
+        <v>0</v>
       </c>
       <c r="CF33" s="66">
-        <f>Y33/1000*Conversions!$B$2</f>
-        <v>0.187804692</v>
+        <v>0</v>
       </c>
       <c r="CG33" s="66">
-        <f>Z33/1000*Conversions!$B$2</f>
-        <v>0.188869752</v>
+        <v>0</v>
       </c>
       <c r="CH33" s="66">
-        <f>AA33/1000*Conversions!$B$2</f>
-        <v>0.18994924800000001</v>
+        <v>0</v>
       </c>
       <c r="CI33" s="66">
-        <f>AB33/1000*Conversions!$B$2</f>
-        <v>0.19104368400000005</v>
-      </c>
-      <c r="CJ33" s="73">
-        <f>TREND(BL33:CI33,$BL$5:$CI$5,$CJ$5)</f>
-        <v>0.20912996939478257</v>
-      </c>
-      <c r="CK33" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ33" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK33" s="66">
+        <v>0</v>
       </c>
       <c r="CM33" s="52" t="str">
         <f t="shared" si="4"/>
@@ -11921,107 +11771,82 @@
         <v>1</v>
       </c>
       <c r="BL34" s="66">
-        <f>E34/1000*Conversions!$B$2</f>
-        <v>1.770767689226878</v>
+        <v>0</v>
       </c>
       <c r="BM34" s="66">
-        <f>F34/1000*Conversions!$B$2</f>
-        <v>1.1177084415156699</v>
+        <v>0</v>
       </c>
       <c r="BN34" s="66">
-        <f>G34/1000*Conversions!$B$2</f>
-        <v>1.3270406387788061</v>
+        <v>0</v>
       </c>
       <c r="BO34" s="66">
-        <f>H34/1000*Conversions!$B$2</f>
-        <v>1.2740152033445633</v>
+        <v>0</v>
       </c>
       <c r="BP34" s="66">
-        <f>I34/1000*Conversions!$B$2</f>
-        <v>1.3741252346560144</v>
+        <v>0</v>
       </c>
       <c r="BQ34" s="66">
-        <f>J34/1000*Conversions!$B$2</f>
-        <v>1.6879089999428629</v>
+        <v>0</v>
       </c>
       <c r="BR34" s="66">
-        <f>K34/1000*Conversions!$B$2</f>
-        <v>1.8348537362957613</v>
+        <v>0</v>
       </c>
       <c r="BS34" s="66">
-        <f>L34/1000*Conversions!$B$2</f>
-        <v>1.9836970880945337</v>
+        <v>0</v>
       </c>
       <c r="BT34" s="66">
-        <f>M34/1000*Conversions!$B$2</f>
-        <v>2.1256553048646114</v>
+        <v>0</v>
       </c>
       <c r="BU34" s="66">
-        <f>N34/1000*Conversions!$B$2</f>
-        <v>2.2488138115815683</v>
+        <v>0</v>
       </c>
       <c r="BV34" s="66">
-        <f>O34/1000*Conversions!$B$2</f>
-        <v>2.3513089975614161</v>
+        <v>0</v>
       </c>
       <c r="BW34" s="66">
-        <f>P34/1000*Conversions!$B$2</f>
-        <v>2.4435836021963722</v>
+        <v>0</v>
       </c>
       <c r="BX34" s="66">
-        <f>Q34/1000*Conversions!$B$2</f>
-        <v>2.5410850488083638</v>
+        <v>0</v>
       </c>
       <c r="BY34" s="66">
-        <f>R34/1000*Conversions!$B$2</f>
-        <v>2.5886509196059588</v>
+        <v>0</v>
       </c>
       <c r="BZ34" s="66">
-        <f>S34/1000*Conversions!$B$2</f>
-        <v>2.5393083958545417</v>
+        <v>0</v>
       </c>
       <c r="CA34" s="66">
-        <f>T34/1000*Conversions!$B$2</f>
-        <v>2.6034237203715316</v>
+        <v>0</v>
       </c>
       <c r="CB34" s="66">
-        <f>U34/1000*Conversions!$B$2</f>
-        <v>2.6753365644213138</v>
+        <v>0</v>
       </c>
       <c r="CC34" s="66">
-        <f>V34/1000*Conversions!$B$2</f>
-        <v>2.7532941486375093</v>
+        <v>0</v>
       </c>
       <c r="CD34" s="66">
-        <f>W34/1000*Conversions!$B$2</f>
-        <v>2.8357648780751545</v>
+        <v>0</v>
       </c>
       <c r="CE34" s="66">
-        <f>X34/1000*Conversions!$B$2</f>
-        <v>2.9211455718959964</v>
+        <v>0</v>
       </c>
       <c r="CF34" s="66">
-        <f>Y34/1000*Conversions!$B$2</f>
-        <v>3.0082873136909374</v>
+        <v>0</v>
       </c>
       <c r="CG34" s="66">
-        <f>Z34/1000*Conversions!$B$2</f>
-        <v>3.095652912218525</v>
+        <v>0</v>
       </c>
       <c r="CH34" s="66">
-        <f>AA34/1000*Conversions!$B$2</f>
-        <v>3.1823681388545353</v>
+        <v>0</v>
       </c>
       <c r="CI34" s="66">
-        <f>AB34/1000*Conversions!$B$2</f>
-        <v>3.2709431661860919</v>
-      </c>
-      <c r="CJ34" s="73">
-        <f>TREND(BT34:CI34,$BT$5:$CI$5,$CJ$5)</f>
-        <v>4.2606548535687239</v>
-      </c>
-      <c r="CK34" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ34" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK34" s="66">
+        <v>0</v>
       </c>
       <c r="CM34" s="52" t="str">
         <f t="shared" si="4"/>
@@ -12329,107 +12154,82 @@
         <v>1</v>
       </c>
       <c r="BL35" s="66">
-        <f>E35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM35" s="66">
-        <f>F35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN35" s="66">
-        <f>G35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO35" s="66">
-        <f>H35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP35" s="66">
-        <f>I35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ35" s="66">
-        <f>J35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR35" s="66">
-        <f>K35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS35" s="66">
-        <f>L35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT35" s="66">
-        <f>M35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU35" s="66">
-        <f>N35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV35" s="66">
-        <f>O35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW35" s="66">
-        <f>P35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX35" s="66">
-        <f>Q35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY35" s="66">
-        <f>R35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ35" s="66">
-        <f>S35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA35" s="66">
-        <f>T35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB35" s="66">
-        <f>U35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC35" s="66">
-        <f>V35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD35" s="66">
-        <f>W35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE35" s="66">
-        <f>X35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF35" s="66">
-        <f>Y35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG35" s="66">
-        <f>Z35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH35" s="66">
-        <f>AA35/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI35" s="66">
-        <f>AB35/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ35" s="73">
-        <f>CI35</f>
-        <v>0</v>
-      </c>
-      <c r="CK35" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ35" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK35" s="66">
+        <v>0</v>
       </c>
       <c r="CM35" s="52" t="str">
         <f t="shared" si="4"/>
@@ -12737,107 +12537,82 @@
         <v>1</v>
       </c>
       <c r="BL36" s="66">
-        <f>E36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM36" s="66">
-        <f>F36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN36" s="66">
-        <f>G36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO36" s="66">
-        <f>H36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP36" s="66">
-        <f>I36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ36" s="66">
-        <f>J36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR36" s="66">
-        <f>K36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS36" s="66">
-        <f>L36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT36" s="66">
-        <f>M36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU36" s="66">
-        <f>N36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV36" s="66">
-        <f>O36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW36" s="66">
-        <f>P36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX36" s="66">
-        <f>Q36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY36" s="66">
-        <f>R36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ36" s="66">
-        <f>S36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA36" s="66">
-        <f>T36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB36" s="66">
-        <f>U36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC36" s="66">
-        <f>V36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD36" s="66">
-        <f>W36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE36" s="66">
-        <f>X36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF36" s="66">
-        <f>Y36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG36" s="66">
-        <f>Z36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH36" s="66">
-        <f>AA36/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI36" s="66">
-        <f>AB36/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ36" s="73">
-        <f>CI36</f>
-        <v>0</v>
-      </c>
-      <c r="CK36" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ36" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK36" s="66">
+        <v>0</v>
       </c>
       <c r="CM36" s="52" t="str">
         <f t="shared" si="4"/>
@@ -13145,107 +12920,82 @@
         <v>1</v>
       </c>
       <c r="BL37" s="66">
-        <f>E37/1000*Conversions!$B$2</f>
-        <v>0.10206997179437498</v>
+        <v>0</v>
       </c>
       <c r="BM37" s="66">
-        <f>F37/1000*Conversions!$B$2</f>
-        <v>0.12762687536742101</v>
+        <v>0</v>
       </c>
       <c r="BN37" s="66">
-        <f>G37/1000*Conversions!$B$2</f>
-        <v>0.13111111859407756</v>
+        <v>0</v>
       </c>
       <c r="BO37" s="66">
-        <f>H37/1000*Conversions!$B$2</f>
-        <v>0.13706461804322786</v>
+        <v>0</v>
       </c>
       <c r="BP37" s="66">
-        <f>I37/1000*Conversions!$B$2</f>
-        <v>0.14772651632149808</v>
+        <v>0</v>
       </c>
       <c r="BQ37" s="66">
-        <f>J37/1000*Conversions!$B$2</f>
-        <v>0.15305968942151191</v>
+        <v>0</v>
       </c>
       <c r="BR37" s="66">
-        <f>K37/1000*Conversions!$B$2</f>
-        <v>0.15752845127929252</v>
+        <v>0</v>
       </c>
       <c r="BS37" s="66">
-        <f>L37/1000*Conversions!$B$2</f>
-        <v>0.16198038327499634</v>
+        <v>0</v>
       </c>
       <c r="BT37" s="66">
-        <f>M37/1000*Conversions!$B$2</f>
-        <v>0.16640788042382051</v>
+        <v>0</v>
       </c>
       <c r="BU37" s="66">
-        <f>N37/1000*Conversions!$B$2</f>
-        <v>0.16986945459576461</v>
+        <v>0</v>
       </c>
       <c r="BV37" s="66">
-        <f>O37/1000*Conversions!$B$2</f>
-        <v>0.17251831028316919</v>
+        <v>0</v>
       </c>
       <c r="BW37" s="66">
-        <f>P37/1000*Conversions!$B$2</f>
-        <v>0.1752209539618505</v>
+        <v>0</v>
       </c>
       <c r="BX37" s="66">
-        <f>Q37/1000*Conversions!$B$2</f>
-        <v>0.17768164056101368</v>
+        <v>0</v>
       </c>
       <c r="BY37" s="66">
-        <f>R37/1000*Conversions!$B$2</f>
-        <v>0.18054777510164682</v>
+        <v>0</v>
       </c>
       <c r="BZ37" s="66">
-        <f>S37/1000*Conversions!$B$2</f>
-        <v>0.18351434041788497</v>
+        <v>0</v>
       </c>
       <c r="CA37" s="66">
-        <f>T37/1000*Conversions!$B$2</f>
-        <v>0.1865288042440558</v>
+        <v>0</v>
       </c>
       <c r="CB37" s="66">
-        <f>U37/1000*Conversions!$B$2</f>
-        <v>0.18959191897396205</v>
+        <v>0</v>
       </c>
       <c r="CC37" s="66">
-        <f>V37/1000*Conversions!$B$2</f>
-        <v>0.19270444857351815</v>
+        <v>0</v>
       </c>
       <c r="CD37" s="66">
-        <f>W37/1000*Conversions!$B$2</f>
-        <v>0.19586716876006988</v>
+        <v>0</v>
       </c>
       <c r="CE37" s="66">
-        <f>X37/1000*Conversions!$B$2</f>
-        <v>0.19908165323052696</v>
+        <v>0</v>
       </c>
       <c r="CF37" s="66">
-        <f>Y37/1000*Conversions!$B$2</f>
-        <v>0.20234874710208081</v>
+        <v>0</v>
       </c>
       <c r="CG37" s="66">
-        <f>Z37/1000*Conversions!$B$2</f>
-        <v>0.20566930925835936</v>
+        <v>0</v>
       </c>
       <c r="CH37" s="66">
-        <f>AA37/1000*Conversions!$B$2</f>
-        <v>0.20904421257321212</v>
+        <v>0</v>
       </c>
       <c r="CI37" s="66">
-        <f>AB37/1000*Conversions!$B$2</f>
-        <v>0.21247434413812613</v>
-      </c>
-      <c r="CJ37" s="73">
-        <f>TREND(BT37:CI37,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.25705588327448137</v>
-      </c>
-      <c r="CK37" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ37" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK37" s="66">
+        <v>0</v>
       </c>
       <c r="CM37" s="52" t="str">
         <f t="shared" si="4"/>
@@ -13553,107 +13303,82 @@
         <v>1</v>
       </c>
       <c r="BL38" s="66">
-        <f>E38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM38" s="66">
-        <f>F38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN38" s="66">
-        <f>G38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO38" s="66">
-        <f>H38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP38" s="66">
-        <f>I38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ38" s="66">
-        <f>J38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR38" s="66">
-        <f>K38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS38" s="66">
-        <f>L38/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT38" s="66">
-        <f>M38/1000*Conversions!$B$2</f>
-        <v>8.1066666666666648E-2</v>
+        <v>0</v>
       </c>
       <c r="BU38" s="66">
-        <f>N38/1000*Conversions!$B$2</f>
-        <v>0.16415999999999997</v>
+        <v>0</v>
       </c>
       <c r="BV38" s="66">
-        <f>O38/1000*Conversions!$B$2</f>
-        <v>0.25862799999999991</v>
+        <v>0</v>
       </c>
       <c r="BW38" s="66">
-        <f>P38/1000*Conversions!$B$2</f>
-        <v>0.36581143333333316</v>
+        <v>0</v>
       </c>
       <c r="BX38" s="66">
-        <f>Q38/1000*Conversions!$B$2</f>
-        <v>0.48720293999999986</v>
+        <v>0</v>
       </c>
       <c r="BY38" s="66">
-        <f>R38/1000*Conversions!$B$2</f>
-        <v>0.62446384041666647</v>
+        <v>0</v>
       </c>
       <c r="BZ38" s="66">
-        <f>S38/1000*Conversions!$B$2</f>
-        <v>0.77944277552499963</v>
+        <v>0</v>
       </c>
       <c r="CA38" s="66">
-        <f>T38/1000*Conversions!$B$2</f>
-        <v>0.95419637789312461</v>
+        <v>0</v>
       </c>
       <c r="CB38" s="66">
-        <f>U38/1000*Conversions!$B$2</f>
-        <v>1.1510121930092492</v>
+        <v>0</v>
       </c>
       <c r="CC38" s="66">
-        <f>V38/1000*Conversions!$B$2</f>
-        <v>1.3724340934620873</v>
+        <v>0</v>
       </c>
       <c r="CD38" s="66">
-        <f>W38/1000*Conversions!$B$2</f>
-        <v>1.6212904547034868</v>
+        <v>0</v>
       </c>
       <c r="CE38" s="66">
-        <f>X38/1000*Conversions!$B$2</f>
-        <v>1.9007253898606336</v>
+        <v>0</v>
       </c>
       <c r="CF38" s="66">
-        <f>Y38/1000*Conversions!$B$2</f>
-        <v>2.2142333729024264</v>
+        <v>0</v>
       </c>
       <c r="CG38" s="66">
-        <f>Z38/1000*Conversions!$B$2</f>
-        <v>2.5656976146923678</v>
+        <v>0</v>
       </c>
       <c r="CH38" s="66">
-        <f>AA38/1000*Conversions!$B$2</f>
-        <v>2.959432595438126</v>
+        <v>0</v>
       </c>
       <c r="CI38" s="66">
-        <f>AB38/1000*Conversions!$B$2</f>
-        <v>2.9909159209215121</v>
-      </c>
-      <c r="CJ38" s="73">
-        <f>TREND(BL38:CI38,$BL$5:$CI$5,$CJ$5)</f>
-        <v>4.3423334668420353</v>
-      </c>
-      <c r="CK38" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ38" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK38" s="66">
+        <v>0</v>
       </c>
       <c r="CM38" s="52" t="str">
         <f t="shared" si="4"/>
@@ -13961,107 +13686,82 @@
         <v>1</v>
       </c>
       <c r="BL39" s="66">
-        <f>E39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM39" s="66">
-        <f>F39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN39" s="66">
-        <f>G39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO39" s="66">
-        <f>H39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP39" s="66">
-        <f>I39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ39" s="66">
-        <f>J39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR39" s="66">
-        <f>K39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS39" s="66">
-        <f>L39/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT39" s="66">
-        <f>M39/1000*Conversions!$B$2</f>
-        <v>1.0133333333333331E-2</v>
+        <v>0</v>
       </c>
       <c r="BU39" s="66">
-        <f>N39/1000*Conversions!$B$2</f>
-        <v>3.0779999999999991E-2</v>
+        <v>0</v>
       </c>
       <c r="BV39" s="66">
-        <f>O39/1000*Conversions!$B$2</f>
-        <v>5.5049333333333318E-2</v>
+        <v>0</v>
       </c>
       <c r="BW39" s="66">
-        <f>P39/1000*Conversions!$B$2</f>
-        <v>8.3423299999999964E-2</v>
+        <v>0</v>
       </c>
       <c r="BX39" s="66">
-        <f>Q39/1000*Conversions!$B$2</f>
-        <v>0.11644149999999995</v>
+        <v>0</v>
       </c>
       <c r="BY39" s="66">
-        <f>R39/1000*Conversions!$B$2</f>
-        <v>0.15470771374999998</v>
+        <v>0</v>
       </c>
       <c r="BZ39" s="66">
-        <f>S39/1000*Conversions!$B$2</f>
-        <v>0.19889717259166664</v>
+        <v>0</v>
       </c>
       <c r="CA39" s="66">
-        <f>T39/1000*Conversions!$B$2</f>
-        <v>0.24976463137312499</v>
+        <v>0</v>
       </c>
       <c r="CB39" s="66">
-        <f>U39/1000*Conversions!$B$2</f>
-        <v>0.30815333021458335</v>
+        <v>0</v>
       </c>
       <c r="CC39" s="66">
-        <f>V39/1000*Conversions!$B$2</f>
-        <v>0.3750049419363547</v>
+        <v>0</v>
       </c>
       <c r="CD39" s="66">
-        <f>W39/1000*Conversions!$B$2</f>
-        <v>0.45137061199508699</v>
+        <v>0</v>
       </c>
       <c r="CE39" s="66">
-        <f>X39/1000*Conversions!$B$2</f>
-        <v>0.53842320924828968</v>
+        <v>0</v>
       </c>
       <c r="CF39" s="66">
-        <f>Y39/1000*Conversions!$B$2</f>
-        <v>0.63747091856576821</v>
+        <v>0</v>
       </c>
       <c r="CG39" s="66">
-        <f>Z39/1000*Conversions!$B$2</f>
-        <v>0.74997232035932204</v>
+        <v>0</v>
       </c>
       <c r="CH39" s="66">
-        <f>AA39/1000*Conversions!$B$2</f>
-        <v>0.87755311765278154</v>
+        <v>0</v>
       </c>
       <c r="CI39" s="66">
-        <f>AB39/1000*Conversions!$B$2</f>
-        <v>0.88688878911717328</v>
-      </c>
-      <c r="CJ39" s="73">
-        <f>TREND(BL39:CI39,$BL$5:$CI$5,$CJ$5)</f>
-        <v>1.2478764716703523</v>
-      </c>
-      <c r="CK39" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ39" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK39" s="66">
+        <v>0</v>
       </c>
       <c r="CM39" s="52" t="str">
         <f t="shared" si="4"/>
@@ -14369,107 +14069,82 @@
         <v>1</v>
       </c>
       <c r="BL40" s="66">
-        <f>E40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM40" s="66">
-        <f>F40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN40" s="66">
-        <f>G40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO40" s="66">
-        <f>H40/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP40" s="66">
-        <f>I40/1000*Conversions!$B$2</f>
-        <v>0.10941619502112578</v>
+        <v>0</v>
       </c>
       <c r="BQ40" s="66">
-        <f>J40/1000*Conversions!$B$2</f>
-        <v>0.22039468698481438</v>
+        <v>0</v>
       </c>
       <c r="BR40" s="66">
-        <f>K40/1000*Conversions!$B$2</f>
-        <v>0.33317520873033607</v>
+        <v>0</v>
       </c>
       <c r="BS40" s="66">
-        <f>L40/1000*Conversions!$B$2</f>
-        <v>0.447472717807405</v>
+        <v>0</v>
       </c>
       <c r="BT40" s="66">
-        <f>M40/1000*Conversions!$B$2</f>
-        <v>0.5630035683450757</v>
+        <v>0</v>
       </c>
       <c r="BU40" s="66">
-        <f>N40/1000*Conversions!$B$2</f>
-        <v>0.56698421665493748</v>
+        <v>0</v>
       </c>
       <c r="BV40" s="66">
-        <f>O40/1000*Conversions!$B$2</f>
-        <v>0.57096486496479937</v>
+        <v>0</v>
       </c>
       <c r="BW40" s="66">
-        <f>P40/1000*Conversions!$B$2</f>
-        <v>0.57494551327466115</v>
+        <v>0</v>
       </c>
       <c r="BX40" s="66">
-        <f>Q40/1000*Conversions!$B$2</f>
-        <v>0.57892616158452292</v>
+        <v>0</v>
       </c>
       <c r="BY40" s="66">
-        <f>R40/1000*Conversions!$B$2</f>
-        <v>0.58290680989438481</v>
+        <v>0</v>
       </c>
       <c r="BZ40" s="66">
-        <f>S40/1000*Conversions!$B$2</f>
-        <v>0.58688745820424659</v>
+        <v>0</v>
       </c>
       <c r="CA40" s="66">
-        <f>T40/1000*Conversions!$B$2</f>
-        <v>0.59086810651410837</v>
+        <v>0</v>
       </c>
       <c r="CB40" s="66">
-        <f>U40/1000*Conversions!$B$2</f>
-        <v>0.59484875482397015</v>
+        <v>0</v>
       </c>
       <c r="CC40" s="66">
-        <f>V40/1000*Conversions!$B$2</f>
-        <v>0.59882940313383193</v>
+        <v>0</v>
       </c>
       <c r="CD40" s="66">
-        <f>W40/1000*Conversions!$B$2</f>
-        <v>0.60281005144369371</v>
+        <v>0</v>
       </c>
       <c r="CE40" s="66">
-        <f>X40/1000*Conversions!$B$2</f>
-        <v>0.60679069975355548</v>
+        <v>0</v>
       </c>
       <c r="CF40" s="66">
-        <f>Y40/1000*Conversions!$B$2</f>
-        <v>0.61077134806341726</v>
+        <v>0</v>
       </c>
       <c r="CG40" s="66">
-        <f>Z40/1000*Conversions!$B$2</f>
-        <v>0.61475199637327915</v>
+        <v>0</v>
       </c>
       <c r="CH40" s="66">
-        <f>AA40/1000*Conversions!$B$2</f>
-        <v>0.61873264468314093</v>
+        <v>0</v>
       </c>
       <c r="CI40" s="66">
-        <f>AB40/1000*Conversions!$B$2</f>
-        <v>0.62271329299300271</v>
-      </c>
-      <c r="CJ40" s="73">
-        <f>TREND(BT40:CI40,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.6824230176409305</v>
-      </c>
-      <c r="CK40" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ40" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK40" s="66">
+        <v>0</v>
       </c>
       <c r="CM40" s="52" t="str">
         <f t="shared" si="4"/>
@@ -14777,107 +14452,82 @@
         <v>1</v>
       </c>
       <c r="BL41" s="66">
-        <f>E41/1000*Conversions!$B$2</f>
-        <v>0.25039919937369937</v>
+        <v>0</v>
       </c>
       <c r="BM41" s="66">
-        <f>F41/1000*Conversions!$B$2</f>
-        <v>0.3283283160568311</v>
+        <v>0</v>
       </c>
       <c r="BN41" s="66">
-        <f>G41/1000*Conversions!$B$2</f>
-        <v>0.16547747129264292</v>
+        <v>0</v>
       </c>
       <c r="BO41" s="66">
-        <f>H41/1000*Conversions!$B$2</f>
-        <v>0.12510096829723802</v>
+        <v>0</v>
       </c>
       <c r="BP41" s="66">
-        <f>I41/1000*Conversions!$B$2</f>
-        <v>0.33627140278297579</v>
+        <v>0</v>
       </c>
       <c r="BQ41" s="66">
-        <f>J41/1000*Conversions!$B$2</f>
-        <v>0.5719976561338419</v>
+        <v>0</v>
       </c>
       <c r="BR41" s="66">
-        <f>K41/1000*Conversions!$B$2</f>
-        <v>0.81147400816854365</v>
+        <v>0</v>
       </c>
       <c r="BS41" s="66">
-        <f>L41/1000*Conversions!$B$2</f>
-        <v>1.0547453739858081</v>
+        <v>0</v>
       </c>
       <c r="BT41" s="66">
-        <f>M41/1000*Conversions!$B$2</f>
-        <v>1.2996873854074265</v>
+        <v>0</v>
       </c>
       <c r="BU41" s="66">
-        <f>N41/1000*Conversions!$B$2</f>
-        <v>1.3100848844906861</v>
+        <v>0</v>
       </c>
       <c r="BV41" s="66">
-        <f>O41/1000*Conversions!$B$2</f>
-        <v>1.3205655635666114</v>
+        <v>0</v>
       </c>
       <c r="BW41" s="66">
-        <f>P41/1000*Conversions!$B$2</f>
-        <v>1.3311300880751442</v>
+        <v>0</v>
       </c>
       <c r="BX41" s="66">
-        <f>Q41/1000*Conversions!$B$2</f>
-        <v>1.3417791287797456</v>
+        <v>0</v>
       </c>
       <c r="BY41" s="66">
-        <f>R41/1000*Conversions!$B$2</f>
-        <v>1.3525133618099832</v>
+        <v>0</v>
       </c>
       <c r="BZ41" s="66">
-        <f>S41/1000*Conversions!$B$2</f>
-        <v>1.3633334687044634</v>
+        <v>0</v>
       </c>
       <c r="CA41" s="66">
-        <f>T41/1000*Conversions!$B$2</f>
-        <v>1.3742401364540988</v>
+        <v>0</v>
       </c>
       <c r="CB41" s="66">
-        <f>U41/1000*Conversions!$B$2</f>
-        <v>1.385234057545732</v>
+        <v>0</v>
       </c>
       <c r="CC41" s="66">
-        <f>V41/1000*Conversions!$B$2</f>
-        <v>1.3963159300060974</v>
+        <v>0</v>
       </c>
       <c r="CD41" s="66">
-        <f>W41/1000*Conversions!$B$2</f>
-        <v>1.4074864574461463</v>
+        <v>0</v>
       </c>
       <c r="CE41" s="66">
-        <f>X41/1000*Conversions!$B$2</f>
-        <v>1.4186569848861941</v>
+        <v>0</v>
       </c>
       <c r="CF41" s="66">
-        <f>Y41/1000*Conversions!$B$2</f>
-        <v>1.4298275123262427</v>
+        <v>0</v>
       </c>
       <c r="CG41" s="66">
-        <f>Z41/1000*Conversions!$B$2</f>
-        <v>1.4409980397662905</v>
+        <v>0</v>
       </c>
       <c r="CH41" s="66">
-        <f>AA41/1000*Conversions!$B$2</f>
-        <v>1.4521685672063418</v>
+        <v>0</v>
       </c>
       <c r="CI41" s="66">
-        <f>AB41/1000*Conversions!$B$2</f>
-        <v>1.46333909464639</v>
-      </c>
-      <c r="CJ41" s="73">
-        <f>TREND(BT41:CI41,$BT$5:$CI$5,$CJ$5)</f>
-        <v>1.626565350571326</v>
-      </c>
-      <c r="CK41" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ41" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK41" s="66">
+        <v>0</v>
       </c>
       <c r="CM41" s="52" t="str">
         <f t="shared" si="4"/>
@@ -15185,107 +14835,82 @@
         <v>1</v>
       </c>
       <c r="BL42" s="66">
-        <f>E42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM42" s="66">
-        <f>F42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN42" s="66">
-        <f>G42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO42" s="66">
-        <f>H42/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP42" s="66">
-        <f>I42/1000*Conversions!$B$2</f>
-        <v>1.1485838310580205</v>
+        <v>0</v>
       </c>
       <c r="BQ42" s="66">
-        <f>J42/1000*Conversions!$B$2</f>
-        <v>1.6524494222089994</v>
+        <v>0</v>
       </c>
       <c r="BR42" s="66">
-        <f>K42/1000*Conversions!$B$2</f>
-        <v>2.1817047612044185</v>
+        <v>0</v>
       </c>
       <c r="BS42" s="66">
-        <f>L42/1000*Conversions!$B$2</f>
-        <v>2.7363498480442785</v>
+        <v>0</v>
       </c>
       <c r="BT42" s="66">
-        <f>M42/1000*Conversions!$B$2</f>
-        <v>3.3163846827285788</v>
+        <v>0</v>
       </c>
       <c r="BU42" s="66">
-        <f>N42/1000*Conversions!$B$2</f>
-        <v>3.6603553142401655</v>
+        <v>0</v>
       </c>
       <c r="BV42" s="66">
-        <f>O42/1000*Conversions!$B$2</f>
-        <v>4.017020819673971</v>
+        <v>0</v>
       </c>
       <c r="BW42" s="66">
-        <f>P42/1000*Conversions!$B$2</f>
-        <v>4.3863811990299988</v>
+        <v>0</v>
       </c>
       <c r="BX42" s="66">
-        <f>Q42/1000*Conversions!$B$2</f>
-        <v>4.6749376983414157</v>
+        <v>0</v>
       </c>
       <c r="BY42" s="66">
-        <f>R42/1000*Conversions!$B$2</f>
-        <v>5.1631865795087126</v>
+        <v>0</v>
       </c>
       <c r="BZ42" s="66">
-        <f>S42/1000*Conversions!$B$2</f>
-        <v>5.6683619592389682</v>
+        <v>0</v>
       </c>
       <c r="CA42" s="66">
-        <f>T42/1000*Conversions!$B$2</f>
-        <v>5.9907714556763061</v>
+        <v>0</v>
       </c>
       <c r="CB42" s="66">
-        <f>U42/1000*Conversions!$B$2</f>
-        <v>6.4236062046434332</v>
+        <v>0</v>
       </c>
       <c r="CC42" s="66">
-        <f>V42/1000*Conversions!$B$2</f>
-        <v>6.556902380826747</v>
+        <v>0</v>
       </c>
       <c r="CD42" s="66">
-        <f>W42/1000*Conversions!$B$2</f>
-        <v>6.6901985570100591</v>
+        <v>0</v>
       </c>
       <c r="CE42" s="66">
-        <f>X42/1000*Conversions!$B$2</f>
-        <v>6.8234947331933729</v>
+        <v>0</v>
       </c>
       <c r="CF42" s="66">
-        <f>Y42/1000*Conversions!$B$2</f>
-        <v>6.9567909093766849</v>
+        <v>0</v>
       </c>
       <c r="CG42" s="66">
-        <f>Z42/1000*Conversions!$B$2</f>
-        <v>7.0900870855599978</v>
+        <v>0</v>
       </c>
       <c r="CH42" s="66">
-        <f>AA42/1000*Conversions!$B$2</f>
-        <v>7.2233832617433116</v>
+        <v>0</v>
       </c>
       <c r="CI42" s="66">
-        <f>AB42/1000*Conversions!$B$2</f>
-        <v>7.3566794379266236</v>
-      </c>
-      <c r="CJ42" s="73">
-        <f>TREND(BT42:CI42,$BT$5:$CI$5,$CJ$5)</f>
-        <v>12.024583690130271</v>
-      </c>
-      <c r="CK42" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ42" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK42" s="66">
+        <v>0</v>
       </c>
       <c r="CM42" s="52" t="str">
         <f t="shared" si="4"/>
@@ -15593,107 +15218,82 @@
         <v>1</v>
       </c>
       <c r="BL43" s="66">
-        <f>E43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM43" s="66">
-        <f>F43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN43" s="66">
-        <f>G43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO43" s="66">
-        <f>H43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP43" s="66">
-        <f>I43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ43" s="66">
-        <f>J43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR43" s="66">
-        <f>K43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS43" s="66">
-        <f>L43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT43" s="66">
-        <f>M43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU43" s="66">
-        <f>N43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV43" s="66">
-        <f>O43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW43" s="66">
-        <f>P43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX43" s="66">
-        <f>Q43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY43" s="66">
-        <f>R43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ43" s="66">
-        <f>S43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA43" s="66">
-        <f>T43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB43" s="66">
-        <f>U43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC43" s="66">
-        <f>V43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD43" s="66">
-        <f>W43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE43" s="66">
-        <f>X43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF43" s="66">
-        <f>Y43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG43" s="66">
-        <f>Z43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH43" s="66">
-        <f>AA43/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI43" s="66">
-        <f>AB43/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ43" s="73">
-        <f>CI43</f>
-        <v>0</v>
-      </c>
-      <c r="CK43" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ43" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK43" s="66">
+        <v>0</v>
       </c>
       <c r="CM43" s="52" t="str">
         <f t="shared" si="4"/>
@@ -16552,107 +16152,82 @@
         <v>1</v>
       </c>
       <c r="BL50" s="66">
-        <f>E50/1000*Conversions!$B$2</f>
-        <v>0.29499766100608776</v>
+        <v>0</v>
       </c>
       <c r="BM50" s="66">
-        <f>F50/1000*Conversions!$B$2</f>
-        <v>0.30086875000000007</v>
+        <v>0</v>
       </c>
       <c r="BN50" s="66">
-        <f>G50/1000*Conversions!$B$2</f>
-        <v>0.3193954054054054</v>
+        <v>0</v>
       </c>
       <c r="BO50" s="66">
-        <f>H50/1000*Conversions!$B$2</f>
-        <v>0.20799770270270271</v>
+        <v>0</v>
       </c>
       <c r="BP50" s="66">
-        <f>I50/1000*Conversions!$B$2</f>
-        <v>9.6600000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="BQ50" s="66">
-        <f>J50/1000*Conversions!$B$2</f>
-        <v>9.6600000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="BR50" s="66">
-        <f>K50/1000*Conversions!$B$2</f>
-        <v>9.6600000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="BS50" s="66">
-        <f>L50/1000*Conversions!$B$2</f>
-        <v>0.12075</v>
+        <v>0</v>
       </c>
       <c r="BT50" s="66">
-        <f>M50/1000*Conversions!$B$2</f>
-        <v>0.11730000000000002</v>
+        <v>0</v>
       </c>
       <c r="BU50" s="66">
-        <f>N50/1000*Conversions!$B$2</f>
-        <v>0.11799</v>
+        <v>0</v>
       </c>
       <c r="BV50" s="66">
-        <f>O50/1000*Conversions!$B$2</f>
-        <v>0.11177999999999999</v>
+        <v>0</v>
       </c>
       <c r="BW50" s="66">
-        <f>P50/1000*Conversions!$B$2</f>
-        <v>0.11436749999999998</v>
+        <v>0</v>
       </c>
       <c r="BX50" s="66">
-        <f>Q50/1000*Conversions!$B$2</f>
-        <v>0.10212</v>
+        <v>0</v>
       </c>
       <c r="BY50" s="66">
-        <f>R50/1000*Conversions!$B$2</f>
-        <v>9.5737499999999975E-2</v>
+        <v>0</v>
       </c>
       <c r="BZ50" s="66">
-        <f>S50/1000*Conversions!$B$2</f>
-        <v>8.6939999999999962E-2</v>
+        <v>0</v>
       </c>
       <c r="CA50" s="66">
-        <f>T50/1000*Conversions!$B$2</f>
-        <v>8.0729999999999955E-2</v>
+        <v>0</v>
       </c>
       <c r="CB50" s="66">
-        <f>U50/1000*Conversions!$B$2</f>
-        <v>7.037999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="CC50" s="66">
-        <f>V50/1000*Conversions!$B$2</f>
-        <v>6.2617499999999965E-2</v>
+        <v>0</v>
       </c>
       <c r="CD50" s="66">
-        <f>W50/1000*Conversions!$B$2</f>
-        <v>5.6925000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="CE50" s="66">
-        <f>X50/1000*Conversions!$B$2</f>
-        <v>0.10350000000000001</v>
+        <v>0</v>
       </c>
       <c r="CF50" s="66">
-        <f>Y50/1000*Conversions!$B$2</f>
-        <v>9.6600000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="CG50" s="66">
-        <f>Z50/1000*Conversions!$B$2</f>
-        <v>9.3149999999999983E-2</v>
+        <v>0</v>
       </c>
       <c r="CH50" s="66">
-        <f>AA50/1000*Conversions!$B$2</f>
-        <v>8.9700000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="CI50" s="66">
-        <f>AB50/1000*Conversions!$B$2</f>
-        <v>8.9700000000000002E-2</v>
-      </c>
-      <c r="CJ50" s="73">
-        <f>TREND(BT50:CI50,$BT$5:$CI$5,$CJ$5)</f>
-        <v>4.6298492647058431E-2</v>
-      </c>
-      <c r="CK50" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ50" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK50" s="66">
+        <v>0</v>
       </c>
       <c r="CM50" s="52" t="str">
         <f t="shared" ref="CM50:CM65" si="8">BG50</f>
@@ -16960,107 +16535,82 @@
         <v>1</v>
       </c>
       <c r="BL51" s="66">
-        <f>E51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM51" s="66">
-        <f>F51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN51" s="66">
-        <f>G51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO51" s="66">
-        <f>H51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP51" s="66">
-        <f>I51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ51" s="66">
-        <f>J51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR51" s="66">
-        <f>K51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS51" s="66">
-        <f>L51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT51" s="66">
-        <f>M51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU51" s="66">
-        <f>N51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV51" s="66">
-        <f>O51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW51" s="66">
-        <f>P51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX51" s="66">
-        <f>Q51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY51" s="66">
-        <f>R51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ51" s="66">
-        <f>S51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA51" s="66">
-        <f>T51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB51" s="66">
-        <f>U51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC51" s="66">
-        <f>V51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD51" s="66">
-        <f>W51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE51" s="66">
-        <f>X51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF51" s="66">
-        <f>Y51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG51" s="66">
-        <f>Z51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH51" s="66">
-        <f>AA51/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI51" s="66">
-        <f>AB51/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ51" s="73">
-        <f>CI51</f>
-        <v>0</v>
-      </c>
-      <c r="CK51" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ51" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK51" s="66">
+        <v>0</v>
       </c>
       <c r="CM51" s="52" t="str">
         <f t="shared" si="8"/>
@@ -17368,107 +16918,82 @@
         <v>1</v>
       </c>
       <c r="BL52" s="66">
-        <f>E52/1000*Conversions!$B$2</f>
-        <v>0.22047060000000002</v>
+        <v>0</v>
       </c>
       <c r="BM52" s="66">
-        <f>F52/1000*Conversions!$B$2</f>
-        <v>0.23534988827091782</v>
+        <v>0</v>
       </c>
       <c r="BN52" s="66">
-        <f>G52/1000*Conversions!$B$2</f>
-        <v>0.23706384737322286</v>
+        <v>0</v>
       </c>
       <c r="BO52" s="66">
-        <f>H52/1000*Conversions!$B$2</f>
-        <v>0.24317777012234676</v>
+        <v>0</v>
       </c>
       <c r="BP52" s="66">
-        <f>I52/1000*Conversions!$B$2</f>
-        <v>0.24936525020419262</v>
+        <v>0</v>
       </c>
       <c r="BQ52" s="66">
-        <f>J52/1000*Conversions!$B$2</f>
-        <v>0.25681865283380162</v>
+        <v>0</v>
       </c>
       <c r="BR52" s="66">
-        <f>K52/1000*Conversions!$B$2</f>
-        <v>0.26407859803333822</v>
+        <v>0</v>
       </c>
       <c r="BS52" s="66">
-        <f>L52/1000*Conversions!$B$2</f>
-        <v>0.27129820145686256</v>
+        <v>0</v>
       </c>
       <c r="BT52" s="66">
-        <f>M52/1000*Conversions!$B$2</f>
-        <v>0.2784649343212966</v>
+        <v>0</v>
       </c>
       <c r="BU52" s="66">
-        <f>N52/1000*Conversions!$B$2</f>
-        <v>0.28400495246439306</v>
+        <v>0</v>
       </c>
       <c r="BV52" s="66">
-        <f>O52/1000*Conversions!$B$2</f>
-        <v>0.28817857742882308</v>
+        <v>0</v>
       </c>
       <c r="BW52" s="66">
-        <f>P52/1000*Conversions!$B$2</f>
-        <v>0.29243564884197326</v>
+        <v>0</v>
       </c>
       <c r="BX52" s="66">
-        <f>Q52/1000*Conversions!$B$2</f>
-        <v>0.29628285505097024</v>
+        <v>0</v>
       </c>
       <c r="BY52" s="66">
-        <f>R52/1000*Conversions!$B$2</f>
-        <v>0.30079993160220875</v>
+        <v>0</v>
       </c>
       <c r="BZ52" s="66">
-        <f>S52/1000*Conversions!$B$2</f>
-        <v>0.30547746426228395</v>
+        <v>0</v>
       </c>
       <c r="CA52" s="66">
-        <f>T52/1000*Conversions!$B$2</f>
-        <v>0.3102277340126553</v>
+        <v>0</v>
       </c>
       <c r="CB52" s="66">
-        <f>U52/1000*Conversions!$B$2</f>
-        <v>0.31505187193774048</v>
+        <v>0</v>
       </c>
       <c r="CC52" s="66">
-        <f>V52/1000*Conversions!$B$2</f>
-        <v>0.31995102671067238</v>
+        <v>0</v>
       </c>
       <c r="CD52" s="66">
-        <f>W52/1000*Conversions!$B$2</f>
-        <v>0.32492636486680887</v>
+        <v>0</v>
       </c>
       <c r="CE52" s="66">
-        <f>X52/1000*Conversions!$B$2</f>
-        <v>0.32997907108149582</v>
+        <v>0</v>
       </c>
       <c r="CF52" s="66">
-        <f>Y52/1000*Conversions!$B$2</f>
-        <v>0.3351103484521506</v>
+        <v>0</v>
       </c>
       <c r="CG52" s="66">
-        <f>Z52/1000*Conversions!$B$2</f>
-        <v>0.34032141878472949</v>
+        <v>0</v>
       </c>
       <c r="CH52" s="66">
-        <f>AA52/1000*Conversions!$B$2</f>
-        <v>0.34561352288465264</v>
+        <v>0</v>
       </c>
       <c r="CI52" s="66">
-        <f>AB52/1000*Conversions!$B$2</f>
-        <v>0.35098792085225056</v>
-      </c>
-      <c r="CJ52" s="73">
-        <f>TREND(BT52:CI52,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.42118817778752771</v>
-      </c>
-      <c r="CK52" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ52" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK52" s="66">
+        <v>0</v>
       </c>
       <c r="CM52" s="52" t="str">
         <f t="shared" si="8"/>
@@ -17776,107 +17301,82 @@
         <v>1</v>
       </c>
       <c r="BL53" s="66">
-        <f>E53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM53" s="66">
-        <f>F53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN53" s="66">
-        <f>G53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO53" s="66">
-        <f>H53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP53" s="66">
-        <f>I53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ53" s="66">
-        <f>J53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR53" s="66">
-        <f>K53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS53" s="66">
-        <f>L53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT53" s="66">
-        <f>M53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU53" s="66">
-        <f>N53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV53" s="66">
-        <f>O53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW53" s="66">
-        <f>P53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX53" s="66">
-        <f>Q53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY53" s="66">
-        <f>R53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ53" s="66">
-        <f>S53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA53" s="66">
-        <f>T53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB53" s="66">
-        <f>U53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC53" s="66">
-        <f>V53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD53" s="66">
-        <f>W53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE53" s="66">
-        <f>X53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF53" s="66">
-        <f>Y53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG53" s="66">
-        <f>Z53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH53" s="66">
-        <f>AA53/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI53" s="66">
-        <f>AB53/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ53" s="73">
-        <f>CI53</f>
-        <v>0</v>
-      </c>
-      <c r="CK53" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ53" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK53" s="66">
+        <v>0</v>
       </c>
       <c r="CM53" s="52" t="str">
         <f t="shared" si="8"/>
@@ -18184,107 +17684,82 @@
         <v>1</v>
       </c>
       <c r="BL54" s="66">
-        <f>E54/1000*Conversions!$B$2</f>
-        <v>1.1233365706613807</v>
+        <v>0</v>
       </c>
       <c r="BM54" s="66">
-        <f>F54/1000*Conversions!$B$2</f>
-        <v>1.1170739618738903</v>
+        <v>0</v>
       </c>
       <c r="BN54" s="66">
-        <f>G54/1000*Conversions!$B$2</f>
-        <v>1.1108113530864001</v>
+        <v>0</v>
       </c>
       <c r="BO54" s="66">
-        <f>H54/1000*Conversions!$B$2</f>
-        <v>1.1045487442989099</v>
+        <v>0</v>
       </c>
       <c r="BP54" s="66">
-        <f>I54/1000*Conversions!$B$2</f>
-        <v>1.1039455430563747</v>
+        <v>0</v>
       </c>
       <c r="BQ54" s="66">
-        <f>J54/1000*Conversions!$B$2</f>
-        <v>1.0961670648761332</v>
+        <v>0</v>
       </c>
       <c r="BR54" s="66">
-        <f>K54/1000*Conversions!$B$2</f>
-        <v>1.1023826938413788</v>
+        <v>0</v>
       </c>
       <c r="BS54" s="66">
-        <f>L54/1000*Conversions!$B$2</f>
-        <v>1.1073814452073416</v>
+        <v>0</v>
       </c>
       <c r="BT54" s="66">
-        <f>M54/1000*Conversions!$B$2</f>
-        <v>1.1115226404555034</v>
+        <v>0</v>
       </c>
       <c r="BU54" s="66">
-        <f>N54/1000*Conversions!$B$2</f>
-        <v>1.1149225801668601</v>
+        <v>0</v>
       </c>
       <c r="BV54" s="66">
-        <f>O54/1000*Conversions!$B$2</f>
-        <v>1.1185514173676627</v>
+        <v>0</v>
       </c>
       <c r="BW54" s="66">
-        <f>P54/1000*Conversions!$B$2</f>
-        <v>1.1212950054423065</v>
+        <v>0</v>
       </c>
       <c r="BX54" s="66">
-        <f>Q54/1000*Conversions!$B$2</f>
-        <v>1.122295048672705</v>
+        <v>0</v>
       </c>
       <c r="BY54" s="66">
-        <f>R54/1000*Conversions!$B$2</f>
-        <v>1.1218850224067094</v>
+        <v>0</v>
       </c>
       <c r="BZ54" s="66">
-        <f>S54/1000*Conversions!$B$2</f>
-        <v>1.1192456234714765</v>
+        <v>0</v>
       </c>
       <c r="CA54" s="66">
-        <f>T54/1000*Conversions!$B$2</f>
-        <v>1.1149914111304935</v>
+        <v>0</v>
       </c>
       <c r="CB54" s="66">
-        <f>U54/1000*Conversions!$B$2</f>
-        <v>1.1095170355369921</v>
+        <v>0</v>
       </c>
       <c r="CC54" s="66">
-        <f>V54/1000*Conversions!$B$2</f>
-        <v>1.1031181419816745</v>
+        <v>0</v>
       </c>
       <c r="CD54" s="66">
-        <f>W54/1000*Conversions!$B$2</f>
-        <v>1.0960550038943044</v>
+        <v>0</v>
       </c>
       <c r="CE54" s="66">
-        <f>X54/1000*Conversions!$B$2</f>
-        <v>1.0886066251786997</v>
+        <v>0</v>
       </c>
       <c r="CF54" s="66">
-        <f>Y54/1000*Conversions!$B$2</f>
-        <v>1.0809051069636535</v>
+        <v>0</v>
       </c>
       <c r="CG54" s="66">
-        <f>Z54/1000*Conversions!$B$2</f>
-        <v>1.073050468675754</v>
+        <v>0</v>
       </c>
       <c r="CH54" s="66">
-        <f>AA54/1000*Conversions!$B$2</f>
-        <v>1.0651835215254</v>
+        <v>0</v>
       </c>
       <c r="CI54" s="66">
-        <f>AB54/1000*Conversions!$B$2</f>
-        <v>1.0570815861128557</v>
-      </c>
-      <c r="CJ54" s="73">
-        <f>TREND(BL54:CI54,$BL$5:$CI$5,$CJ$5)</f>
-        <v>1.0587869828863461</v>
-      </c>
-      <c r="CK54" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ54" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK54" s="66">
+        <v>0</v>
       </c>
       <c r="CM54" s="52" t="str">
         <f t="shared" si="8"/>
@@ -18592,107 +18067,82 @@
         <v>1</v>
       </c>
       <c r="BL55" s="66">
-        <f>E55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM55" s="66">
-        <f>F55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN55" s="66">
-        <f>G55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO55" s="66">
-        <f>H55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP55" s="66">
-        <f>I55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ55" s="66">
-        <f>J55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR55" s="66">
-        <f>K55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS55" s="66">
-        <f>L55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT55" s="66">
-        <f>M55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU55" s="66">
-        <f>N55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV55" s="66">
-        <f>O55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW55" s="66">
-        <f>P55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX55" s="66">
-        <f>Q55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY55" s="66">
-        <f>R55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ55" s="66">
-        <f>S55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA55" s="66">
-        <f>T55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB55" s="66">
-        <f>U55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC55" s="66">
-        <f>V55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD55" s="66">
-        <f>W55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE55" s="66">
-        <f>X55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF55" s="66">
-        <f>Y55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG55" s="66">
-        <f>Z55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH55" s="66">
-        <f>AA55/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI55" s="66">
-        <f>AB55/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ55" s="73">
-        <f>CI55</f>
-        <v>0</v>
-      </c>
-      <c r="CK55" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ55" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK55" s="66">
+        <v>0</v>
       </c>
       <c r="CM55" s="52" t="str">
         <f t="shared" si="8"/>
@@ -19000,107 +18450,82 @@
         <v>1</v>
       </c>
       <c r="BL56" s="66">
-        <f>E56/1000*Conversions!$B$2</f>
-        <v>0.48293664251642127</v>
+        <v>0</v>
       </c>
       <c r="BM56" s="66">
-        <f>F56/1000*Conversions!$B$2</f>
-        <v>0.30482957495881907</v>
+        <v>0</v>
       </c>
       <c r="BN56" s="66">
-        <f>G56/1000*Conversions!$B$2</f>
-        <v>0.36192017421240152</v>
+        <v>0</v>
       </c>
       <c r="BO56" s="66">
-        <f>H56/1000*Conversions!$B$2</f>
-        <v>0.34745869182124445</v>
+        <v>0</v>
       </c>
       <c r="BP56" s="66">
-        <f>I56/1000*Conversions!$B$2</f>
-        <v>0.37476142763345838</v>
+        <v>0</v>
       </c>
       <c r="BQ56" s="66">
-        <f>J56/1000*Conversions!$B$2</f>
-        <v>0.46033881816623529</v>
+        <v>0</v>
       </c>
       <c r="BR56" s="66">
-        <f>K56/1000*Conversions!$B$2</f>
-        <v>0.50041465535338936</v>
+        <v>0</v>
       </c>
       <c r="BS56" s="66">
-        <f>L56/1000*Conversions!$B$2</f>
-        <v>0.54100829675305462</v>
+        <v>0</v>
       </c>
       <c r="BT56" s="66">
-        <f>M56/1000*Conversions!$B$2</f>
-        <v>0.57972417405398491</v>
+        <v>0</v>
       </c>
       <c r="BU56" s="66">
-        <f>N56/1000*Conversions!$B$2</f>
-        <v>0.61331285770406407</v>
+        <v>0</v>
       </c>
       <c r="BV56" s="66">
-        <f>O56/1000*Conversions!$B$2</f>
-        <v>0.64126609024402248</v>
+        <v>0</v>
       </c>
       <c r="BW56" s="66">
-        <f>P56/1000*Conversions!$B$2</f>
-        <v>0.66643189150810134</v>
+        <v>0</v>
       </c>
       <c r="BX56" s="66">
-        <f>Q56/1000*Conversions!$B$2</f>
-        <v>0.69302319512955357</v>
+        <v>0</v>
       </c>
       <c r="BY56" s="66">
-        <f>R56/1000*Conversions!$B$2</f>
-        <v>0.70599570534707967</v>
+        <v>0</v>
       </c>
       <c r="BZ56" s="66">
-        <f>S56/1000*Conversions!$B$2</f>
-        <v>0.69253865341487497</v>
+        <v>0</v>
       </c>
       <c r="CA56" s="66">
-        <f>T56/1000*Conversions!$B$2</f>
-        <v>0.71002465101041778</v>
+        <v>0</v>
       </c>
       <c r="CB56" s="66">
-        <f>U56/1000*Conversions!$B$2</f>
-        <v>0.72963724484217662</v>
+        <v>0</v>
       </c>
       <c r="CC56" s="66">
-        <f>V56/1000*Conversions!$B$2</f>
-        <v>0.750898404173866</v>
+        <v>0</v>
       </c>
       <c r="CD56" s="66">
-        <f>W56/1000*Conversions!$B$2</f>
-        <v>0.77339042129322388</v>
+        <v>0</v>
       </c>
       <c r="CE56" s="66">
-        <f>X56/1000*Conversions!$B$2</f>
-        <v>0.79667606506254451</v>
+        <v>0</v>
       </c>
       <c r="CF56" s="66">
-        <f>Y56/1000*Conversions!$B$2</f>
-        <v>0.82044199464298295</v>
+        <v>0</v>
       </c>
       <c r="CG56" s="66">
-        <f>Z56/1000*Conversions!$B$2</f>
-        <v>0.8442689760595975</v>
+        <v>0</v>
       </c>
       <c r="CH56" s="66">
-        <f>AA56/1000*Conversions!$B$2</f>
-        <v>0.86791858332396399</v>
+        <v>0</v>
       </c>
       <c r="CI56" s="66">
-        <f>AB56/1000*Conversions!$B$2</f>
-        <v>0.89207540895984316</v>
-      </c>
-      <c r="CJ56" s="73">
-        <f>TREND(BT56:CI56,$BT$5:$CI$5,$CJ$5)</f>
-        <v>1.1619967782460137</v>
-      </c>
-      <c r="CK56" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ56" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK56" s="66">
+        <v>0</v>
       </c>
       <c r="CM56" s="52" t="str">
         <f t="shared" si="8"/>
@@ -19408,107 +18833,82 @@
         <v>1</v>
       </c>
       <c r="BL57" s="66">
-        <f>E57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM57" s="66">
-        <f>F57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN57" s="66">
-        <f>G57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO57" s="66">
-        <f>H57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP57" s="66">
-        <f>I57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ57" s="66">
-        <f>J57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR57" s="66">
-        <f>K57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS57" s="66">
-        <f>L57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT57" s="66">
-        <f>M57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU57" s="66">
-        <f>N57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV57" s="66">
-        <f>O57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW57" s="66">
-        <f>P57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX57" s="66">
-        <f>Q57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY57" s="66">
-        <f>R57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ57" s="66">
-        <f>S57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA57" s="66">
-        <f>T57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB57" s="66">
-        <f>U57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC57" s="66">
-        <f>V57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD57" s="66">
-        <f>W57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE57" s="66">
-        <f>X57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF57" s="66">
-        <f>Y57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG57" s="66">
-        <f>Z57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH57" s="66">
-        <f>AA57/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI57" s="66">
-        <f>AB57/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ57" s="73">
-        <f>CI57</f>
-        <v>0</v>
-      </c>
-      <c r="CK57" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ57" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK57" s="66">
+        <v>0</v>
       </c>
       <c r="CM57" s="52" t="str">
         <f t="shared" si="8"/>
@@ -19816,107 +19216,82 @@
         <v>1</v>
       </c>
       <c r="BL58" s="66">
-        <f>E58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM58" s="66">
-        <f>F58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN58" s="66">
-        <f>G58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO58" s="66">
-        <f>H58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP58" s="66">
-        <f>I58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ58" s="66">
-        <f>J58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR58" s="66">
-        <f>K58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS58" s="66">
-        <f>L58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT58" s="66">
-        <f>M58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU58" s="66">
-        <f>N58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV58" s="66">
-        <f>O58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW58" s="66">
-        <f>P58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX58" s="66">
-        <f>Q58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY58" s="66">
-        <f>R58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ58" s="66">
-        <f>S58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA58" s="66">
-        <f>T58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB58" s="66">
-        <f>U58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC58" s="66">
-        <f>V58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD58" s="66">
-        <f>W58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE58" s="66">
-        <f>X58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF58" s="66">
-        <f>Y58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG58" s="66">
-        <f>Z58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH58" s="66">
-        <f>AA58/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI58" s="66">
-        <f>AB58/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ58" s="73">
-        <f>CI58</f>
-        <v>0</v>
-      </c>
-      <c r="CK58" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ58" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK58" s="66">
+        <v>0</v>
       </c>
       <c r="CM58" s="52" t="str">
         <f t="shared" si="8"/>
@@ -20224,107 +19599,82 @@
         <v>1</v>
       </c>
       <c r="BL59" s="66">
-        <f>E59/1000*Conversions!$B$2</f>
-        <v>0.10206997179437498</v>
+        <v>0</v>
       </c>
       <c r="BM59" s="66">
-        <f>F59/1000*Conversions!$B$2</f>
-        <v>0.12762687536742101</v>
+        <v>0</v>
       </c>
       <c r="BN59" s="66">
-        <f>G59/1000*Conversions!$B$2</f>
-        <v>0.13111111859407756</v>
+        <v>0</v>
       </c>
       <c r="BO59" s="66">
-        <f>H59/1000*Conversions!$B$2</f>
-        <v>0.13706461804322786</v>
+        <v>0</v>
       </c>
       <c r="BP59" s="66">
-        <f>I59/1000*Conversions!$B$2</f>
-        <v>0.14772651632149808</v>
+        <v>0</v>
       </c>
       <c r="BQ59" s="66">
-        <f>J59/1000*Conversions!$B$2</f>
-        <v>0.15305968942151191</v>
+        <v>0</v>
       </c>
       <c r="BR59" s="66">
-        <f>K59/1000*Conversions!$B$2</f>
-        <v>0.15752845127929252</v>
+        <v>0</v>
       </c>
       <c r="BS59" s="66">
-        <f>L59/1000*Conversions!$B$2</f>
-        <v>0.16198038327499634</v>
+        <v>0</v>
       </c>
       <c r="BT59" s="66">
-        <f>M59/1000*Conversions!$B$2</f>
-        <v>0.16640788042382051</v>
+        <v>0</v>
       </c>
       <c r="BU59" s="66">
-        <f>N59/1000*Conversions!$B$2</f>
-        <v>0.16986945459576461</v>
+        <v>0</v>
       </c>
       <c r="BV59" s="66">
-        <f>O59/1000*Conversions!$B$2</f>
-        <v>0.17251831028316919</v>
+        <v>0</v>
       </c>
       <c r="BW59" s="66">
-        <f>P59/1000*Conversions!$B$2</f>
-        <v>0.1752209539618505</v>
+        <v>0</v>
       </c>
       <c r="BX59" s="66">
-        <f>Q59/1000*Conversions!$B$2</f>
-        <v>0.17768164056101368</v>
+        <v>0</v>
       </c>
       <c r="BY59" s="66">
-        <f>R59/1000*Conversions!$B$2</f>
-        <v>0.18054777510164682</v>
+        <v>0</v>
       </c>
       <c r="BZ59" s="66">
-        <f>S59/1000*Conversions!$B$2</f>
-        <v>0.18351434041788497</v>
+        <v>0</v>
       </c>
       <c r="CA59" s="66">
-        <f>T59/1000*Conversions!$B$2</f>
-        <v>0.1865288042440558</v>
+        <v>0</v>
       </c>
       <c r="CB59" s="66">
-        <f>U59/1000*Conversions!$B$2</f>
-        <v>0.18959191897396205</v>
+        <v>0</v>
       </c>
       <c r="CC59" s="66">
-        <f>V59/1000*Conversions!$B$2</f>
-        <v>0.19270444857351815</v>
+        <v>0</v>
       </c>
       <c r="CD59" s="66">
-        <f>W59/1000*Conversions!$B$2</f>
-        <v>0.19586716876006988</v>
+        <v>0</v>
       </c>
       <c r="CE59" s="66">
-        <f>X59/1000*Conversions!$B$2</f>
-        <v>0.19908165323052696</v>
+        <v>0</v>
       </c>
       <c r="CF59" s="66">
-        <f>Y59/1000*Conversions!$B$2</f>
-        <v>0.20234874710208081</v>
+        <v>0</v>
       </c>
       <c r="CG59" s="66">
-        <f>Z59/1000*Conversions!$B$2</f>
-        <v>0.20566930925835936</v>
+        <v>0</v>
       </c>
       <c r="CH59" s="66">
-        <f>AA59/1000*Conversions!$B$2</f>
-        <v>0.20904421257321212</v>
+        <v>0</v>
       </c>
       <c r="CI59" s="66">
-        <f>AB59/1000*Conversions!$B$2</f>
-        <v>0.21247434413812613</v>
-      </c>
-      <c r="CJ59" s="73">
-        <f>TREND(BT59:CI59,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.25705588327448137</v>
-      </c>
-      <c r="CK59" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ59" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK59" s="66">
+        <v>0</v>
       </c>
       <c r="CM59" s="52" t="str">
         <f t="shared" si="8"/>
@@ -20632,107 +19982,82 @@
         <v>1</v>
       </c>
       <c r="BL60" s="66">
-        <f>E60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM60" s="66">
-        <f>F60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN60" s="66">
-        <f>G60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO60" s="66">
-        <f>H60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP60" s="66">
-        <f>I60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ60" s="66">
-        <f>J60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR60" s="66">
-        <f>K60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS60" s="66">
-        <f>L60/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT60" s="66">
-        <f>M60/1000*Conversions!$B$2</f>
-        <v>0.11177066666666664</v>
+        <v>0</v>
       </c>
       <c r="BU60" s="66">
-        <f>N60/1000*Conversions!$B$2</f>
-        <v>0.31836779999999992</v>
+        <v>0</v>
       </c>
       <c r="BV60" s="66">
-        <f>O60/1000*Conversions!$B$2</f>
-        <v>0.61312493333333318</v>
+        <v>0</v>
       </c>
       <c r="BW60" s="66">
-        <f>P60/1000*Conversions!$B$2</f>
-        <v>1.0264167333333329</v>
+        <v>0</v>
       </c>
       <c r="BX60" s="66">
-        <f>Q60/1000*Conversions!$B$2</f>
-        <v>1.5984471999999996</v>
+        <v>0</v>
       </c>
       <c r="BY60" s="66">
-        <f>R60/1000*Conversions!$B$2</f>
-        <v>2.3528719666666658</v>
+        <v>0</v>
       </c>
       <c r="BZ60" s="66">
-        <f>S60/1000*Conversions!$B$2</f>
-        <v>3.2893585586666649</v>
+        <v>0</v>
       </c>
       <c r="CA60" s="66">
-        <f>T60/1000*Conversions!$B$2</f>
-        <v>4.448602638999998</v>
+        <v>0</v>
       </c>
       <c r="CB60" s="66">
-        <f>U60/1000*Conversions!$B$2</f>
-        <v>5.8801398826133298</v>
+        <v>0</v>
       </c>
       <c r="CC60" s="66">
-        <f>V60/1000*Conversions!$B$2</f>
-        <v>7.6442365366553293</v>
+        <v>0</v>
       </c>
       <c r="CD60" s="66">
-        <f>W60/1000*Conversions!$B$2</f>
-        <v>9.8141806385579962</v>
+        <v>0</v>
       </c>
       <c r="CE60" s="66">
-        <f>X60/1000*Conversions!$B$2</f>
-        <v>12.479058315684568</v>
+        <v>0</v>
       </c>
       <c r="CF60" s="66">
-        <f>Y60/1000*Conversions!$B$2</f>
-        <v>15.74711730972979</v>
+        <v>0</v>
       </c>
       <c r="CG60" s="66">
-        <f>Z60/1000*Conversions!$B$2</f>
-        <v>19.749841296754308</v>
+        <v>0</v>
       </c>
       <c r="CH60" s="66">
-        <f>AA60/1000*Conversions!$B$2</f>
-        <v>23.373612778945326</v>
+        <v>0</v>
       </c>
       <c r="CI60" s="66">
-        <f>AB60/1000*Conversions!$B$2</f>
-        <v>23.622268234040501</v>
-      </c>
-      <c r="CJ60" s="73">
-        <f>TREND(BL60:CI60,$BL$5:$CI$5,$CJ$5)</f>
-        <v>30.618994906411899</v>
-      </c>
-      <c r="CK60" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ60" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK60" s="66">
+        <v>0</v>
       </c>
       <c r="CM60" s="52" t="str">
         <f t="shared" si="8"/>
@@ -21040,107 +20365,82 @@
         <v>1</v>
       </c>
       <c r="BL61" s="66">
-        <f>E61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM61" s="66">
-        <f>F61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN61" s="66">
-        <f>G61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO61" s="66">
-        <f>H61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP61" s="66">
-        <f>I61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ61" s="66">
-        <f>J61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR61" s="66">
-        <f>K61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS61" s="66">
-        <f>L61/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT61" s="66">
-        <f>M61/1000*Conversions!$B$2</f>
-        <v>5.5733333333333322E-2</v>
+        <v>0</v>
       </c>
       <c r="BU61" s="66">
-        <f>N61/1000*Conversions!$B$2</f>
-        <v>0.16928999999999997</v>
+        <v>0</v>
       </c>
       <c r="BV61" s="66">
-        <f>O61/1000*Conversions!$B$2</f>
-        <v>0.3282186666666666</v>
+        <v>0</v>
       </c>
       <c r="BW61" s="66">
-        <f>P61/1000*Conversions!$B$2</f>
-        <v>0.54784979999999983</v>
+        <v>0</v>
       </c>
       <c r="BX61" s="66">
-        <f>Q61/1000*Conversions!$B$2</f>
-        <v>0.84844423999999985</v>
+        <v>0</v>
       </c>
       <c r="BY61" s="66">
-        <f>R61/1000*Conversions!$B$2</f>
-        <v>1.2567510099999997</v>
+        <v>0</v>
       </c>
       <c r="BZ61" s="66">
-        <f>S61/1000*Conversions!$B$2</f>
-        <v>1.8080537889333321</v>
+        <v>0</v>
       </c>
       <c r="CA61" s="66">
-        <f>T61/1000*Conversions!$B$2</f>
-        <v>2.5488587890199992</v>
+        <v>0</v>
       </c>
       <c r="CB61" s="66">
-        <f>U61/1000*Conversions!$B$2</f>
-        <v>3.5404244209546656</v>
+        <v>0</v>
       </c>
       <c r="CC61" s="66">
-        <f>V61/1000*Conversions!$B$2</f>
-        <v>4.8633956011193984</v>
+        <v>0</v>
       </c>
       <c r="CD61" s="66">
-        <f>W61/1000*Conversions!$B$2</f>
-        <v>6.623887473587402</v>
+        <v>0</v>
       </c>
       <c r="CE61" s="66">
-        <f>X61/1000*Conversions!$B$2</f>
-        <v>8.961470728336133</v>
+        <v>0</v>
       </c>
       <c r="CF61" s="66">
-        <f>Y61/1000*Conversions!$B$2</f>
-        <v>12.059651517363399</v>
+        <v>0</v>
       </c>
       <c r="CG61" s="66">
-        <f>Z61/1000*Conversions!$B$2</f>
-        <v>16.159623582061705</v>
+        <v>0</v>
       </c>
       <c r="CH61" s="66">
-        <f>AA61/1000*Conversions!$B$2</f>
-        <v>19.924387995111189</v>
+        <v>0</v>
       </c>
       <c r="CI61" s="66">
-        <f>AB61/1000*Conversions!$B$2</f>
-        <v>20.136349569527276</v>
-      </c>
-      <c r="CJ61" s="73">
-        <f>TREND(BL61:CI61,$BL$5:$CI$5,$CJ$5)</f>
-        <v>24.071791809190245</v>
-      </c>
-      <c r="CK61" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ61" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK61" s="66">
+        <v>0</v>
       </c>
       <c r="CM61" s="52" t="str">
         <f t="shared" si="8"/>
@@ -21448,107 +20748,82 @@
         <v>1</v>
       </c>
       <c r="BL62" s="66">
-        <f>E62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM62" s="66">
-        <f>F62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN62" s="66">
-        <f>G62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO62" s="66">
-        <f>H62/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP62" s="66">
-        <f>I62/1000*Conversions!$B$2</f>
-        <v>7.2944130014083855E-2</v>
+        <v>0</v>
       </c>
       <c r="BQ62" s="66">
-        <f>J62/1000*Conversions!$B$2</f>
-        <v>0.1469297913232096</v>
+        <v>0</v>
       </c>
       <c r="BR62" s="66">
-        <f>K62/1000*Conversions!$B$2</f>
-        <v>0.22211680582022408</v>
+        <v>0</v>
       </c>
       <c r="BS62" s="66">
-        <f>L62/1000*Conversions!$B$2</f>
-        <v>0.29831514520493668</v>
+        <v>0</v>
       </c>
       <c r="BT62" s="66">
-        <f>M62/1000*Conversions!$B$2</f>
-        <v>0.37533571223005058</v>
+        <v>0</v>
       </c>
       <c r="BU62" s="66">
-        <f>N62/1000*Conversions!$B$2</f>
-        <v>0.37798947776995845</v>
+        <v>0</v>
       </c>
       <c r="BV62" s="66">
-        <f>O62/1000*Conversions!$B$2</f>
-        <v>0.38064324330986632</v>
+        <v>0</v>
       </c>
       <c r="BW62" s="66">
-        <f>P62/1000*Conversions!$B$2</f>
-        <v>0.38329700884977419</v>
+        <v>0</v>
       </c>
       <c r="BX62" s="66">
-        <f>Q62/1000*Conversions!$B$2</f>
-        <v>0.38595077438968212</v>
+        <v>0</v>
       </c>
       <c r="BY62" s="66">
-        <f>R62/1000*Conversions!$B$2</f>
-        <v>0.38860453992958988</v>
+        <v>0</v>
       </c>
       <c r="BZ62" s="66">
-        <f>S62/1000*Conversions!$B$2</f>
-        <v>0.3912583054694978</v>
+        <v>0</v>
       </c>
       <c r="CA62" s="66">
-        <f>T62/1000*Conversions!$B$2</f>
-        <v>0.39391207100940567</v>
+        <v>0</v>
       </c>
       <c r="CB62" s="66">
-        <f>U62/1000*Conversions!$B$2</f>
-        <v>0.39656583654931354</v>
+        <v>0</v>
       </c>
       <c r="CC62" s="66">
-        <f>V62/1000*Conversions!$B$2</f>
-        <v>0.3992196020892213</v>
+        <v>0</v>
       </c>
       <c r="CD62" s="66">
-        <f>W62/1000*Conversions!$B$2</f>
-        <v>0.40187336762912917</v>
+        <v>0</v>
       </c>
       <c r="CE62" s="66">
-        <f>X62/1000*Conversions!$B$2</f>
-        <v>0.4045271331690371</v>
+        <v>0</v>
       </c>
       <c r="CF62" s="66">
-        <f>Y62/1000*Conversions!$B$2</f>
-        <v>0.40718089870894497</v>
+        <v>0</v>
       </c>
       <c r="CG62" s="66">
-        <f>Z62/1000*Conversions!$B$2</f>
-        <v>0.40983466424885284</v>
+        <v>0</v>
       </c>
       <c r="CH62" s="66">
-        <f>AA62/1000*Conversions!$B$2</f>
-        <v>0.41248842978876071</v>
+        <v>0</v>
       </c>
       <c r="CI62" s="66">
-        <f>AB62/1000*Conversions!$B$2</f>
-        <v>0.41514219532866864</v>
-      </c>
-      <c r="CJ62" s="73">
-        <f>TREND(BT62:CI62,$BT$5:$CI$5,$CJ$5)</f>
-        <v>0.4549486784272867</v>
-      </c>
-      <c r="CK62" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ62" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK62" s="66">
+        <v>0</v>
       </c>
       <c r="CM62" s="52" t="str">
         <f t="shared" si="8"/>
@@ -21856,107 +21131,82 @@
         <v>1</v>
       </c>
       <c r="BL63" s="66">
-        <f>E63/1000*Conversions!$B$2</f>
-        <v>0.37559879906054899</v>
+        <v>0</v>
       </c>
       <c r="BM63" s="66">
-        <f>F63/1000*Conversions!$B$2</f>
-        <v>0.49249247408524666</v>
+        <v>0</v>
       </c>
       <c r="BN63" s="66">
-        <f>G63/1000*Conversions!$B$2</f>
-        <v>0.24821620693896435</v>
+        <v>0</v>
       </c>
       <c r="BO63" s="66">
-        <f>H63/1000*Conversions!$B$2</f>
-        <v>0.18765145244585704</v>
+        <v>0</v>
       </c>
       <c r="BP63" s="66">
-        <f>I63/1000*Conversions!$B$2</f>
-        <v>0.50440710417446366</v>
+        <v>0</v>
       </c>
       <c r="BQ63" s="66">
-        <f>J63/1000*Conversions!$B$2</f>
-        <v>0.85799648420076269</v>
+        <v>0</v>
       </c>
       <c r="BR63" s="66">
-        <f>K63/1000*Conversions!$B$2</f>
-        <v>1.2172110122528155</v>
+        <v>0</v>
       </c>
       <c r="BS63" s="66">
-        <f>L63/1000*Conversions!$B$2</f>
-        <v>1.582118060978712</v>
+        <v>0</v>
       </c>
       <c r="BT63" s="66">
-        <f>M63/1000*Conversions!$B$2</f>
-        <v>1.9495310781111395</v>
+        <v>0</v>
       </c>
       <c r="BU63" s="66">
-        <f>N63/1000*Conversions!$B$2</f>
-        <v>1.965127326736029</v>
+        <v>0</v>
       </c>
       <c r="BV63" s="66">
-        <f>O63/1000*Conversions!$B$2</f>
-        <v>1.9808483453499168</v>
+        <v>0</v>
       </c>
       <c r="BW63" s="66">
-        <f>P63/1000*Conversions!$B$2</f>
-        <v>1.9966951321127162</v>
+        <v>0</v>
       </c>
       <c r="BX63" s="66">
-        <f>Q63/1000*Conversions!$B$2</f>
-        <v>2.0126686931696178</v>
+        <v>0</v>
       </c>
       <c r="BY63" s="66">
-        <f>R63/1000*Conversions!$B$2</f>
-        <v>2.0287700427149744</v>
+        <v>0</v>
       </c>
       <c r="BZ63" s="66">
-        <f>S63/1000*Conversions!$B$2</f>
-        <v>2.0450002030566945</v>
+        <v>0</v>
       </c>
       <c r="CA63" s="66">
-        <f>T63/1000*Conversions!$B$2</f>
-        <v>2.0613602046811486</v>
+        <v>0</v>
       </c>
       <c r="CB63" s="66">
-        <f>U63/1000*Conversions!$B$2</f>
-        <v>2.0778510863185975</v>
+        <v>0</v>
       </c>
       <c r="CC63" s="66">
-        <f>V63/1000*Conversions!$B$2</f>
-        <v>2.0944738950091462</v>
+        <v>0</v>
       </c>
       <c r="CD63" s="66">
-        <f>W63/1000*Conversions!$B$2</f>
-        <v>2.111229686169219</v>
+        <v>0</v>
       </c>
       <c r="CE63" s="66">
-        <f>X63/1000*Conversions!$B$2</f>
-        <v>2.127985477329291</v>
+        <v>0</v>
       </c>
       <c r="CF63" s="66">
-        <f>Y63/1000*Conversions!$B$2</f>
-        <v>2.1447412684893634</v>
+        <v>0</v>
       </c>
       <c r="CG63" s="66">
-        <f>Z63/1000*Conversions!$B$2</f>
-        <v>2.1614970596494354</v>
+        <v>0</v>
       </c>
       <c r="CH63" s="66">
-        <f>AA63/1000*Conversions!$B$2</f>
-        <v>2.1782528508095123</v>
+        <v>0</v>
       </c>
       <c r="CI63" s="66">
-        <f>AB63/1000*Conversions!$B$2</f>
-        <v>2.1950086419695851</v>
-      </c>
-      <c r="CJ63" s="73">
-        <f>TREND(BT63:CI63,$BT$5:$CI$5,$CJ$5)</f>
-        <v>2.439848025856989</v>
-      </c>
-      <c r="CK63" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ63" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK63" s="66">
+        <v>0</v>
       </c>
       <c r="CM63" s="52" t="str">
         <f t="shared" si="8"/>
@@ -22264,107 +21514,82 @@
         <v>1</v>
       </c>
       <c r="BL64" s="66">
-        <f>E64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM64" s="66">
-        <f>F64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN64" s="66">
-        <f>G64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO64" s="66">
-        <f>H64/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP64" s="66">
-        <f>I64/1000*Conversions!$B$2</f>
-        <v>3.4457514931740612</v>
+        <v>0</v>
       </c>
       <c r="BQ64" s="66">
-        <f>J64/1000*Conversions!$B$2</f>
-        <v>4.0130914539361413</v>
+        <v>0</v>
       </c>
       <c r="BR64" s="66">
-        <f>K64/1000*Conversions!$B$2</f>
-        <v>4.6058211625426617</v>
+        <v>0</v>
       </c>
       <c r="BS64" s="66">
-        <f>L64/1000*Conversions!$B$2</f>
-        <v>5.2239406189936224</v>
+        <v>0</v>
       </c>
       <c r="BT64" s="66">
-        <f>M64/1000*Conversions!$B$2</f>
-        <v>5.867449823289026</v>
+        <v>0</v>
       </c>
       <c r="BU64" s="66">
-        <f>N64/1000*Conversions!$B$2</f>
-        <v>6.2748948244117111</v>
+        <v>0</v>
       </c>
       <c r="BV64" s="66">
-        <f>O64/1000*Conversions!$B$2</f>
-        <v>6.6950346994566186</v>
+        <v>0</v>
       </c>
       <c r="BW64" s="66">
-        <f>P64/1000*Conversions!$B$2</f>
-        <v>7.1278694484237475</v>
+        <v>0</v>
       </c>
       <c r="BX64" s="66">
-        <f>Q64/1000*Conversions!$B$2</f>
-        <v>7.5733990713130952</v>
+        <v>0</v>
       </c>
       <c r="BY64" s="66">
-        <f>R64/1000*Conversions!$B$2</f>
-        <v>8.0316235681246653</v>
+        <v>0</v>
       </c>
       <c r="BZ64" s="66">
-        <f>S64/1000*Conversions!$B$2</f>
-        <v>8.5025429388584506</v>
+        <v>0</v>
       </c>
       <c r="CA64" s="66">
-        <f>T64/1000*Conversions!$B$2</f>
-        <v>8.9861571835144574</v>
+        <v>0</v>
       </c>
       <c r="CB64" s="66">
-        <f>U64/1000*Conversions!$B$2</f>
-        <v>9.1765802923477615</v>
+        <v>0</v>
       </c>
       <c r="CC64" s="66">
-        <f>V64/1000*Conversions!$B$2</f>
-        <v>9.3670034011810674</v>
+        <v>0</v>
       </c>
       <c r="CD64" s="66">
-        <f>W64/1000*Conversions!$B$2</f>
-        <v>9.5574265100143716</v>
+        <v>0</v>
       </c>
       <c r="CE64" s="66">
-        <f>X64/1000*Conversions!$B$2</f>
-        <v>9.7478496188476758</v>
+        <v>0</v>
       </c>
       <c r="CF64" s="66">
-        <f>Y64/1000*Conversions!$B$2</f>
-        <v>9.9382727276809781</v>
+        <v>0</v>
       </c>
       <c r="CG64" s="66">
-        <f>Z64/1000*Conversions!$B$2</f>
-        <v>10.128695836514284</v>
+        <v>0</v>
       </c>
       <c r="CH64" s="66">
-        <f>AA64/1000*Conversions!$B$2</f>
-        <v>10.319118945347586</v>
+        <v>0</v>
       </c>
       <c r="CI64" s="66">
-        <f>AB64/1000*Conversions!$B$2</f>
-        <v>10.509542054180891</v>
-      </c>
-      <c r="CJ64" s="73">
-        <f>TREND(BT64:CI64,$BT$5:$CI$5,$CJ$5)</f>
-        <v>15.59116317974258</v>
-      </c>
-      <c r="CK64" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ64" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK64" s="66">
+        <v>0</v>
       </c>
       <c r="CM64" s="52" t="str">
         <f t="shared" si="8"/>
@@ -22672,107 +21897,82 @@
         <v>1</v>
       </c>
       <c r="BL65" s="66">
-        <f>E65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BM65" s="66">
-        <f>F65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BN65" s="66">
-        <f>G65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BO65" s="66">
-        <f>H65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BP65" s="66">
-        <f>I65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BQ65" s="66">
-        <f>J65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BR65" s="66">
-        <f>K65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BS65" s="66">
-        <f>L65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BT65" s="66">
-        <f>M65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BU65" s="66">
-        <f>N65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BV65" s="66">
-        <f>O65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BW65" s="66">
-        <f>P65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BX65" s="66">
-        <f>Q65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BY65" s="66">
-        <f>R65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="BZ65" s="66">
-        <f>S65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CA65" s="66">
-        <f>T65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CB65" s="66">
-        <f>U65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CC65" s="66">
-        <f>V65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CD65" s="66">
-        <f>W65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CE65" s="66">
-        <f>X65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CF65" s="66">
-        <f>Y65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CG65" s="66">
-        <f>Z65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CH65" s="66">
-        <f>AA65/1000*Conversions!$B$2</f>
         <v>0</v>
       </c>
       <c r="CI65" s="66">
-        <f>AB65/1000*Conversions!$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="CJ65" s="73">
-        <f>CI65</f>
-        <v>0</v>
-      </c>
-      <c r="CK65" s="52">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="CJ65" s="66">
+        <v>0</v>
+      </c>
+      <c r="CK65" s="66">
+        <v>0</v>
       </c>
       <c r="CM65" s="52" t="str">
         <f t="shared" si="8"/>
@@ -22956,7 +22156,7 @@
     <row r="67" spans="1:121" x14ac:dyDescent="0.25">
       <c r="CJ67" s="66">
         <f>SUM(CJ6:CJ21,CJ28:CJ43,CJ50:CJ65)</f>
-        <v>155.46564495117042</v>
+        <v>53.48424955735566</v>
       </c>
       <c r="CK67" s="52" t="s">
         <v>1</v>
@@ -22970,7 +22170,7 @@
       <c r="BC68" s="20"/>
       <c r="CJ68" s="67">
         <f>CJ67*1000/Conversions!$B$2</f>
-        <v>3713233.1363134235</v>
+        <v>1277449.3540975365</v>
       </c>
       <c r="CK68" s="52" t="s">
         <v>19</v>
@@ -22996,8 +22196,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:DO69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BL50" sqref="BL50:CJ65"/>
+    <sheetView topLeftCell="AW26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BG48" sqref="BG48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44496,9 +43696,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44648,19 +43851,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0B387-229C-4E2C-9ACB-57F10C5B7407}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B7E6A7-FFA9-474C-81D0-41CF87028AB1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44684,9 +43883,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B7E6A7-FFA9-474C-81D0-41CF87028AB1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0B387-229C-4E2C-9ACB-57F10C5B7407}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enable step 2 of MSW potential in the DomBioPot_Low scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
+++ b/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\ccr-40\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC326A4-C633-4BC2-A4CE-B40223D87D81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B12273-1D17-40D2-A4F3-896D393A4B0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1576,8 +1576,8 @@
   </sheetPr>
   <dimension ref="A1:DQ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BL28" sqref="BL28:CK43"/>
+    <sheetView tabSelected="1" topLeftCell="BN4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CD23" sqref="CD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12907,7 +12907,7 @@
         <v>MINBIOMSW2_S2</v>
       </c>
       <c r="BH37" s="52" t="str">
-        <f t="shared" si="7"/>
+        <f>A37</f>
         <v>BMSW - Me</v>
       </c>
       <c r="BI37" s="55" t="s">
@@ -12920,79 +12920,104 @@
         <v>1</v>
       </c>
       <c r="BL37" s="66">
-        <v>0</v>
+        <f>E37/1000*Conversions!$B$2</f>
+        <v>0.10206997179437498</v>
       </c>
       <c r="BM37" s="66">
-        <v>0</v>
+        <f>F37/1000*Conversions!$B$2</f>
+        <v>0.12762687536742101</v>
       </c>
       <c r="BN37" s="66">
-        <v>0</v>
+        <f>G37/1000*Conversions!$B$2</f>
+        <v>0.13111111859407756</v>
       </c>
       <c r="BO37" s="66">
-        <v>0</v>
+        <f>H37/1000*Conversions!$B$2</f>
+        <v>0.13706461804322786</v>
       </c>
       <c r="BP37" s="66">
-        <v>0</v>
+        <f>I37/1000*Conversions!$B$2</f>
+        <v>0.14772651632149808</v>
       </c>
       <c r="BQ37" s="66">
-        <v>0</v>
+        <f>J37/1000*Conversions!$B$2</f>
+        <v>0.15305968942151191</v>
       </c>
       <c r="BR37" s="66">
-        <v>0</v>
+        <f>K37/1000*Conversions!$B$2</f>
+        <v>0.15752845127929252</v>
       </c>
       <c r="BS37" s="66">
-        <v>0</v>
+        <f>L37/1000*Conversions!$B$2</f>
+        <v>0.16198038327499634</v>
       </c>
       <c r="BT37" s="66">
-        <v>0</v>
+        <f>M37/1000*Conversions!$B$2</f>
+        <v>0.16640788042382051</v>
       </c>
       <c r="BU37" s="66">
-        <v>0</v>
+        <f>N37/1000*Conversions!$B$2</f>
+        <v>0.16986945459576461</v>
       </c>
       <c r="BV37" s="66">
-        <v>0</v>
+        <f>O37/1000*Conversions!$B$2</f>
+        <v>0.17251831028316919</v>
       </c>
       <c r="BW37" s="66">
-        <v>0</v>
+        <f>P37/1000*Conversions!$B$2</f>
+        <v>0.1752209539618505</v>
       </c>
       <c r="BX37" s="66">
-        <v>0</v>
+        <f>Q37/1000*Conversions!$B$2</f>
+        <v>0.17768164056101368</v>
       </c>
       <c r="BY37" s="66">
-        <v>0</v>
+        <f>R37/1000*Conversions!$B$2</f>
+        <v>0.18054777510164682</v>
       </c>
       <c r="BZ37" s="66">
-        <v>0</v>
+        <f>S37/1000*Conversions!$B$2</f>
+        <v>0.18351434041788497</v>
       </c>
       <c r="CA37" s="66">
-        <v>0</v>
+        <f>T37/1000*Conversions!$B$2</f>
+        <v>0.1865288042440558</v>
       </c>
       <c r="CB37" s="66">
-        <v>0</v>
+        <f>U37/1000*Conversions!$B$2</f>
+        <v>0.18959191897396205</v>
       </c>
       <c r="CC37" s="66">
-        <v>0</v>
+        <f>V37/1000*Conversions!$B$2</f>
+        <v>0.19270444857351815</v>
       </c>
       <c r="CD37" s="66">
-        <v>0</v>
+        <f>W37/1000*Conversions!$B$2</f>
+        <v>0.19586716876006988</v>
       </c>
       <c r="CE37" s="66">
-        <v>0</v>
+        <f>X37/1000*Conversions!$B$2</f>
+        <v>0.19908165323052696</v>
       </c>
       <c r="CF37" s="66">
-        <v>0</v>
+        <f>Y37/1000*Conversions!$B$2</f>
+        <v>0.20234874710208081</v>
       </c>
       <c r="CG37" s="66">
-        <v>0</v>
+        <f>Z37/1000*Conversions!$B$2</f>
+        <v>0.20566930925835936</v>
       </c>
       <c r="CH37" s="66">
-        <v>0</v>
+        <f>AA37/1000*Conversions!$B$2</f>
+        <v>0.20904421257321212</v>
       </c>
       <c r="CI37" s="66">
-        <v>0</v>
-      </c>
-      <c r="CJ37" s="66">
-        <v>0</v>
+        <f>AB37/1000*Conversions!$B$2</f>
+        <v>0.21247434413812613</v>
+      </c>
+      <c r="CJ37" s="73">
+        <f>TREND(BT37:CI37,$BT$5:$CI$5,$CJ$5)</f>
+        <v>0.25705588327448137</v>
       </c>
       <c r="CK37" s="66">
         <v>0</v>
@@ -22156,7 +22181,7 @@
     <row r="67" spans="1:121" x14ac:dyDescent="0.25">
       <c r="CJ67" s="66">
         <f>SUM(CJ6:CJ21,CJ28:CJ43,CJ50:CJ65)</f>
-        <v>53.48424955735566</v>
+        <v>53.741305440630143</v>
       </c>
       <c r="CK67" s="52" t="s">
         <v>1</v>
@@ -22170,7 +22195,7 @@
       <c r="BC68" s="20"/>
       <c r="CJ68" s="67">
         <f>CJ67*1000/Conversions!$B$2</f>
-        <v>1277449.3540975365</v>
+        <v>1283589.0283899433</v>
       </c>
       <c r="CK68" s="52" t="s">
         <v>19</v>
@@ -43696,15 +43721,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -43850,6 +43866,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -43857,14 +43882,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B7E6A7-FFA9-474C-81D0-41CF87028AB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C50E7D6-5F29-4A57-95C7-88A3E0AAEB93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43882,6 +43899,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B7E6A7-FFA9-474C-81D0-41CF87028AB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0B387-229C-4E2C-9ACB-57F10C5B7407}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Enable step 3 of MWS2 to avoid dummies in lowBio cases
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
+++ b/SuppXLS/Scen_B_SUP_DomBioPot_Low.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B12273-1D17-40D2-A4F3-896D393A4B0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77493CB-77F7-4B16-A379-FBEC5058C9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1576,8 +1576,8 @@
   </sheetPr>
   <dimension ref="A1:DQ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD23" sqref="CD23"/>
+    <sheetView tabSelected="1" topLeftCell="BF22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CK59" sqref="CK59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19624,79 +19624,104 @@
         <v>1</v>
       </c>
       <c r="BL59" s="66">
-        <v>0</v>
+        <f>E59/1000*Conversions!$B$2</f>
+        <v>0.10206997179437498</v>
       </c>
       <c r="BM59" s="66">
-        <v>0</v>
+        <f>F59/1000*Conversions!$B$2</f>
+        <v>0.12762687536742101</v>
       </c>
       <c r="BN59" s="66">
-        <v>0</v>
+        <f>G59/1000*Conversions!$B$2</f>
+        <v>0.13111111859407756</v>
       </c>
       <c r="BO59" s="66">
-        <v>0</v>
+        <f>H59/1000*Conversions!$B$2</f>
+        <v>0.13706461804322786</v>
       </c>
       <c r="BP59" s="66">
-        <v>0</v>
+        <f>I59/1000*Conversions!$B$2</f>
+        <v>0.14772651632149808</v>
       </c>
       <c r="BQ59" s="66">
-        <v>0</v>
+        <f>J59/1000*Conversions!$B$2</f>
+        <v>0.15305968942151191</v>
       </c>
       <c r="BR59" s="66">
-        <v>0</v>
+        <f>K59/1000*Conversions!$B$2</f>
+        <v>0.15752845127929252</v>
       </c>
       <c r="BS59" s="66">
-        <v>0</v>
+        <f>L59/1000*Conversions!$B$2</f>
+        <v>0.16198038327499634</v>
       </c>
       <c r="BT59" s="66">
-        <v>0</v>
+        <f>M59/1000*Conversions!$B$2</f>
+        <v>0.16640788042382051</v>
       </c>
       <c r="BU59" s="66">
-        <v>0</v>
+        <f>N59/1000*Conversions!$B$2</f>
+        <v>0.16986945459576461</v>
       </c>
       <c r="BV59" s="66">
-        <v>0</v>
+        <f>O59/1000*Conversions!$B$2</f>
+        <v>0.17251831028316919</v>
       </c>
       <c r="BW59" s="66">
-        <v>0</v>
+        <f>P59/1000*Conversions!$B$2</f>
+        <v>0.1752209539618505</v>
       </c>
       <c r="BX59" s="66">
-        <v>0</v>
+        <f>Q59/1000*Conversions!$B$2</f>
+        <v>0.17768164056101368</v>
       </c>
       <c r="BY59" s="66">
-        <v>0</v>
+        <f>R59/1000*Conversions!$B$2</f>
+        <v>0.18054777510164682</v>
       </c>
       <c r="BZ59" s="66">
-        <v>0</v>
+        <f>S59/1000*Conversions!$B$2</f>
+        <v>0.18351434041788497</v>
       </c>
       <c r="CA59" s="66">
-        <v>0</v>
+        <f>T59/1000*Conversions!$B$2</f>
+        <v>0.1865288042440558</v>
       </c>
       <c r="CB59" s="66">
-        <v>0</v>
+        <f>U59/1000*Conversions!$B$2</f>
+        <v>0.18959191897396205</v>
       </c>
       <c r="CC59" s="66">
-        <v>0</v>
+        <f>V59/1000*Conversions!$B$2</f>
+        <v>0.19270444857351815</v>
       </c>
       <c r="CD59" s="66">
-        <v>0</v>
+        <f>W59/1000*Conversions!$B$2</f>
+        <v>0.19586716876006988</v>
       </c>
       <c r="CE59" s="66">
-        <v>0</v>
+        <f>X59/1000*Conversions!$B$2</f>
+        <v>0.19908165323052696</v>
       </c>
       <c r="CF59" s="66">
-        <v>0</v>
+        <f>Y59/1000*Conversions!$B$2</f>
+        <v>0.20234874710208081</v>
       </c>
       <c r="CG59" s="66">
-        <v>0</v>
+        <f>Z59/1000*Conversions!$B$2</f>
+        <v>0.20566930925835936</v>
       </c>
       <c r="CH59" s="66">
-        <v>0</v>
+        <f>AA59/1000*Conversions!$B$2</f>
+        <v>0.20904421257321212</v>
       </c>
       <c r="CI59" s="66">
-        <v>0</v>
-      </c>
-      <c r="CJ59" s="66">
-        <v>0</v>
+        <f>AB59/1000*Conversions!$B$2</f>
+        <v>0.21247434413812613</v>
+      </c>
+      <c r="CJ59" s="73">
+        <f>TREND(BT59:CI59,$BT$5:$CI$5,$CJ$5)</f>
+        <v>0.25705588327448137</v>
       </c>
       <c r="CK59" s="66">
         <v>0</v>
@@ -22181,7 +22206,7 @@
     <row r="67" spans="1:121" x14ac:dyDescent="0.25">
       <c r="CJ67" s="66">
         <f>SUM(CJ6:CJ21,CJ28:CJ43,CJ50:CJ65)</f>
-        <v>53.741305440630143</v>
+        <v>53.998361323904625</v>
       </c>
       <c r="CK67" s="52" t="s">
         <v>1</v>
@@ -22195,7 +22220,7 @@
       <c r="BC68" s="20"/>
       <c r="CJ68" s="67">
         <f>CJ67*1000/Conversions!$B$2</f>
-        <v>1283589.0283899433</v>
+        <v>1289728.7026823498</v>
       </c>
       <c r="CK68" s="52" t="s">
         <v>19</v>

</xml_diff>